<commit_message>
add data and scripts
</commit_message>
<xml_diff>
--- a/frontend/data/data_available.xlsx
+++ b/frontend/data/data_available.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bianka\Documents\MSc-Internship\Observatory-of-the-Mountains\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bianka\Documents\MSc-Internship\Observatory-of-the-Mountains\frontend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E48FC0-3ABF-4702-B2E3-DA28EECC8A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199C7C39-C643-4304-AEC1-A664BC26866E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8809251D-B3C6-41F0-B60D-9556D90BF91D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{8809251D-B3C6-41F0-B60D-9556D90BF91D}"/>
   </bookViews>
   <sheets>
     <sheet name="per county" sheetId="1" r:id="rId1"/>
@@ -1988,9 +1988,6 @@
     <t>GDHI per inhabitant</t>
   </si>
   <si>
-    <t>unique biodiveristy</t>
-  </si>
-  <si>
     <t>GDP per inhabitants</t>
   </si>
   <si>
@@ -2073,6 +2070,9 @@
   </si>
   <si>
     <t>total aerial biomass, total air carbon, volume with bark, foliar biomass, basal area, tree cover, average normal diamter, average heights, leaf area index</t>
+  </si>
+  <si>
+    <t>unique biodiversity</t>
   </si>
 </sst>
 </file>
@@ -2223,7 +2223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2292,17 +2292,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2311,13 +2302,19 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2661,8 +2658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CD66C7E-061F-43E9-BB3A-8D29200B2BF1}">
   <dimension ref="A1:I195"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="88" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
@@ -2681,11 +2678,11 @@
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
       <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
@@ -2711,13 +2708,13 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" s="34" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+    <row r="3" spans="1:9" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+    <row r="4" spans="1:9" s="30" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2767,8 +2764,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+    <row r="7" spans="1:9" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2809,8 +2806,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="31" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+    <row r="10" spans="1:9" s="30" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2889,8 +2886,8 @@
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="38" t="s">
-        <v>585</v>
+      <c r="B15" s="1" t="s">
+        <v>584</v>
       </c>
       <c r="C15" s="1">
         <v>2005</v>
@@ -2905,18 +2902,18 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
+    <row r="17" spans="1:9" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="31" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
+    <row r="18" spans="1:9" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="33" t="s">
         <v>46</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -2942,7 +2939,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
+      <c r="A20" s="33"/>
       <c r="B20" s="2" t="s">
         <v>282</v>
       </c>
@@ -2966,7 +2963,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
+      <c r="A21" s="33"/>
       <c r="B21" s="2" t="s">
         <v>284</v>
       </c>
@@ -2990,9 +2987,9 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
+      <c r="A22" s="33"/>
       <c r="B22" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C22" s="1">
         <v>1999</v>
@@ -3011,7 +3008,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
+      <c r="A23" s="33"/>
       <c r="B23" s="1" t="s">
         <v>287</v>
       </c>
@@ -3035,7 +3032,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
+      <c r="A24" s="33"/>
       <c r="B24" s="1" t="s">
         <v>291</v>
       </c>
@@ -3059,7 +3056,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
+      <c r="A25" s="33"/>
       <c r="B25" s="1" t="s">
         <v>294</v>
       </c>
@@ -3083,7 +3080,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
+      <c r="A26" s="33"/>
       <c r="B26" s="1" t="s">
         <v>297</v>
       </c>
@@ -3107,7 +3104,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
+      <c r="A27" s="33"/>
       <c r="B27" s="1" t="s">
         <v>300</v>
       </c>
@@ -3131,7 +3128,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="30" t="s">
+      <c r="A28" s="33" t="s">
         <v>49</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -3157,7 +3154,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
+      <c r="A29" s="33"/>
       <c r="B29" s="1" t="s">
         <v>306</v>
       </c>
@@ -3181,7 +3178,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
+      <c r="A30" s="33"/>
       <c r="B30" s="1" t="s">
         <v>309</v>
       </c>
@@ -3205,7 +3202,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
+      <c r="A31" s="33"/>
       <c r="B31" s="1" t="s">
         <v>312</v>
       </c>
@@ -3229,7 +3226,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
+      <c r="A32" s="33"/>
       <c r="B32" s="1" t="s">
         <v>314</v>
       </c>
@@ -3253,7 +3250,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
+      <c r="A33" s="33"/>
       <c r="B33" s="1" t="s">
         <v>317</v>
       </c>
@@ -3277,7 +3274,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
+      <c r="A34" s="33"/>
       <c r="B34" s="1" t="s">
         <v>320</v>
       </c>
@@ -3301,7 +3298,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
+      <c r="A35" s="33"/>
       <c r="B35" s="1" t="s">
         <v>323</v>
       </c>
@@ -3325,7 +3322,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
+      <c r="A36" s="33"/>
       <c r="B36" s="1" t="s">
         <v>327</v>
       </c>
@@ -3349,7 +3346,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="33" t="s">
         <v>346</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -3375,7 +3372,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="30"/>
+      <c r="A38" s="33"/>
       <c r="B38" s="1" t="s">
         <v>330</v>
       </c>
@@ -3399,7 +3396,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
+      <c r="A39" s="33"/>
       <c r="B39" s="1" t="s">
         <v>335</v>
       </c>
@@ -3423,7 +3420,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="30"/>
+      <c r="A40" s="33"/>
       <c r="B40" s="1" t="s">
         <v>338</v>
       </c>
@@ -3447,7 +3444,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="30"/>
+      <c r="A41" s="33"/>
       <c r="B41" s="1" t="s">
         <v>340</v>
       </c>
@@ -3471,7 +3468,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="30"/>
+      <c r="A42" s="33"/>
       <c r="B42" s="1" t="s">
         <v>343</v>
       </c>
@@ -3495,7 +3492,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="33" t="s">
         <v>48</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -3521,7 +3518,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="30"/>
+      <c r="A44" s="33"/>
       <c r="B44" s="1" t="s">
         <v>348</v>
       </c>
@@ -3545,7 +3542,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="30"/>
+      <c r="A45" s="33"/>
       <c r="B45" s="1" t="s">
         <v>349</v>
       </c>
@@ -3569,7 +3566,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="30"/>
+      <c r="A46" s="33"/>
       <c r="B46" s="1" t="s">
         <v>350</v>
       </c>
@@ -3593,7 +3590,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="30" t="s">
+      <c r="A47" s="33" t="s">
         <v>50</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -3619,7 +3616,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
+      <c r="A48" s="33"/>
       <c r="B48" s="1" t="s">
         <v>360</v>
       </c>
@@ -3643,7 +3640,7 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="30" t="s">
+      <c r="A49" s="33" t="s">
         <v>51</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -3669,7 +3666,7 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="30"/>
+      <c r="A50" s="33"/>
       <c r="B50" s="1" t="s">
         <v>367</v>
       </c>
@@ -3693,7 +3690,7 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="30"/>
+      <c r="A51" s="33"/>
       <c r="B51" s="1" t="s">
         <v>368</v>
       </c>
@@ -3717,7 +3714,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="30"/>
+      <c r="A52" s="33"/>
       <c r="B52" s="1" t="s">
         <v>369</v>
       </c>
@@ -3741,7 +3738,7 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="30"/>
+      <c r="A53" s="33"/>
       <c r="B53" s="1" t="s">
         <v>370</v>
       </c>
@@ -3765,7 +3762,7 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="30"/>
+      <c r="A54" s="33"/>
       <c r="B54" s="1" t="s">
         <v>371</v>
       </c>
@@ -3789,7 +3786,7 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="30"/>
+      <c r="A55" s="33"/>
       <c r="B55" s="2" t="s">
         <v>383</v>
       </c>
@@ -3813,7 +3810,7 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="30"/>
+      <c r="A56" s="33"/>
       <c r="B56" s="2" t="s">
         <v>384</v>
       </c>
@@ -3837,7 +3834,7 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="30"/>
+      <c r="A57" s="33"/>
       <c r="B57" s="1" t="s">
         <v>80</v>
       </c>
@@ -3861,7 +3858,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="30"/>
+      <c r="A58" s="33"/>
       <c r="B58" s="1" t="s">
         <v>80</v>
       </c>
@@ -3885,7 +3882,7 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="30"/>
+      <c r="A59" s="33"/>
       <c r="B59" s="1" t="s">
         <v>80</v>
       </c>
@@ -3909,7 +3906,7 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="30"/>
+      <c r="A60" s="33"/>
       <c r="B60" s="1" t="s">
         <v>80</v>
       </c>
@@ -3933,7 +3930,7 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="30"/>
+      <c r="A61" s="33"/>
       <c r="B61" s="1" t="s">
         <v>396</v>
       </c>
@@ -3957,7 +3954,7 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="30"/>
+      <c r="A62" s="33"/>
       <c r="B62" s="2" t="s">
         <v>401</v>
       </c>
@@ -3981,7 +3978,7 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="30"/>
+      <c r="A63" s="33"/>
       <c r="B63" s="1" t="s">
         <v>402</v>
       </c>
@@ -4004,13 +4001,13 @@
         <v>404</v>
       </c>
     </row>
-    <row r="65" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="31" t="s">
+    <row r="65" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="30" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="30" t="s">
+      <c r="A66" s="33" t="s">
         <v>54</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -4036,7 +4033,7 @@
       </c>
     </row>
     <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="30"/>
+      <c r="A67" s="33"/>
       <c r="B67" s="1" t="s">
         <v>236</v>
       </c>
@@ -4060,7 +4057,7 @@
       </c>
     </row>
     <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="30"/>
+      <c r="A68" s="33"/>
       <c r="B68" s="1" t="s">
         <v>239</v>
       </c>
@@ -4084,7 +4081,7 @@
       </c>
     </row>
     <row r="69" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="30"/>
+      <c r="A69" s="33"/>
       <c r="B69" s="1" t="s">
         <v>507</v>
       </c>
@@ -4108,7 +4105,7 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="30"/>
+      <c r="A70" s="33"/>
       <c r="B70" s="1" t="s">
         <v>245</v>
       </c>
@@ -4132,7 +4129,7 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="30"/>
+      <c r="A71" s="33"/>
       <c r="B71" s="1" t="s">
         <v>248</v>
       </c>
@@ -4156,7 +4153,7 @@
       </c>
     </row>
     <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="30"/>
+      <c r="A72" s="33"/>
       <c r="B72" s="1" t="s">
         <v>250</v>
       </c>
@@ -4180,7 +4177,7 @@
       </c>
     </row>
     <row r="73" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="30" t="s">
+      <c r="A73" s="33" t="s">
         <v>55</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -4206,7 +4203,7 @@
       </c>
     </row>
     <row r="74" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="30"/>
+      <c r="A74" s="33"/>
       <c r="B74" s="1" t="s">
         <v>255</v>
       </c>
@@ -4230,7 +4227,7 @@
       </c>
     </row>
     <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="30"/>
+      <c r="A75" s="33"/>
       <c r="B75" s="1" t="s">
         <v>258</v>
       </c>
@@ -4254,7 +4251,7 @@
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="30"/>
+      <c r="A76" s="33"/>
       <c r="B76" s="1" t="s">
         <v>261</v>
       </c>
@@ -4278,7 +4275,7 @@
       </c>
     </row>
     <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="30"/>
+      <c r="A77" s="33"/>
       <c r="B77" s="1" t="s">
         <v>264</v>
       </c>
@@ -4302,7 +4299,7 @@
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="30"/>
+      <c r="A78" s="33"/>
       <c r="B78" s="1" t="s">
         <v>267</v>
       </c>
@@ -4326,7 +4323,7 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="30"/>
+      <c r="A79" s="33"/>
       <c r="B79" s="1" t="s">
         <v>270</v>
       </c>
@@ -4350,7 +4347,7 @@
       </c>
     </row>
     <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="30"/>
+      <c r="A80" s="33"/>
       <c r="B80" s="1" t="s">
         <v>273</v>
       </c>
@@ -4374,7 +4371,7 @@
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="30"/>
+      <c r="A81" s="33"/>
       <c r="B81" s="1" t="s">
         <v>276</v>
       </c>
@@ -4397,13 +4394,13 @@
         <v>278</v>
       </c>
     </row>
-    <row r="83" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="31" t="s">
+    <row r="83" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="30" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="30" t="s">
+      <c r="A84" s="33" t="s">
         <v>57</v>
       </c>
       <c r="B84" s="2" t="s">
@@ -4429,7 +4426,7 @@
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="30"/>
+      <c r="A85" s="33"/>
       <c r="B85" s="2" t="s">
         <v>196</v>
       </c>
@@ -4453,7 +4450,7 @@
       </c>
     </row>
     <row r="86" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A86" s="30"/>
+      <c r="A86" s="33"/>
       <c r="B86" s="2" t="s">
         <v>199</v>
       </c>
@@ -4477,7 +4474,7 @@
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="30"/>
+      <c r="A87" s="33"/>
       <c r="B87" s="2" t="s">
         <v>202</v>
       </c>
@@ -4501,7 +4498,7 @@
       </c>
     </row>
     <row r="88" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="30"/>
+      <c r="A88" s="33"/>
       <c r="B88" s="2" t="s">
         <v>205</v>
       </c>
@@ -4525,7 +4522,7 @@
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="30" t="s">
+      <c r="A89" s="33" t="s">
         <v>58</v>
       </c>
       <c r="B89" s="2" t="s">
@@ -4551,7 +4548,7 @@
       </c>
     </row>
     <row r="90" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="30"/>
+      <c r="A90" s="33"/>
       <c r="B90" s="2" t="s">
         <v>211</v>
       </c>
@@ -4575,7 +4572,7 @@
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="30" t="s">
+      <c r="A91" s="33" t="s">
         <v>59</v>
       </c>
       <c r="B91" s="2" t="s">
@@ -4598,7 +4595,7 @@
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="30"/>
+      <c r="A92" s="33"/>
       <c r="B92" s="2" t="s">
         <v>216</v>
       </c>
@@ -4622,7 +4619,7 @@
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="30"/>
+      <c r="A93" s="33"/>
       <c r="B93" s="1" t="s">
         <v>218</v>
       </c>
@@ -4646,7 +4643,7 @@
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="30"/>
+      <c r="A94" s="33"/>
       <c r="B94" s="1" t="s">
         <v>219</v>
       </c>
@@ -4670,7 +4667,7 @@
       </c>
     </row>
     <row r="95" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="30"/>
+      <c r="A95" s="33"/>
       <c r="B95" s="1" t="s">
         <v>223</v>
       </c>
@@ -4694,7 +4691,7 @@
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="30" t="s">
+      <c r="A96" s="33" t="s">
         <v>60</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -4720,7 +4717,7 @@
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="30"/>
+      <c r="A97" s="33"/>
       <c r="B97" s="1" t="s">
         <v>229</v>
       </c>
@@ -4743,16 +4740,16 @@
         <v>231</v>
       </c>
     </row>
-    <row r="99" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="31" t="s">
+    <row r="99" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="30" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A100" s="30" t="s">
+      <c r="A100" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="B100" s="38" t="s">
+      <c r="B100" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C100" s="1">
@@ -4775,7 +4772,7 @@
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="30"/>
+      <c r="A101" s="33"/>
       <c r="B101" s="1" t="s">
         <v>72</v>
       </c>
@@ -4799,7 +4796,7 @@
       </c>
     </row>
     <row r="102" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A102" s="30"/>
+      <c r="A102" s="33"/>
       <c r="B102" s="1" t="s">
         <v>74</v>
       </c>
@@ -4823,7 +4820,7 @@
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="30"/>
+      <c r="A103" s="33"/>
       <c r="B103" s="1" t="s">
         <v>77</v>
       </c>
@@ -4847,7 +4844,7 @@
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="30"/>
+      <c r="A104" s="33"/>
       <c r="B104" s="1" t="s">
         <v>80</v>
       </c>
@@ -4871,7 +4868,7 @@
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="30"/>
+      <c r="A105" s="33"/>
       <c r="B105" s="1" t="s">
         <v>84</v>
       </c>
@@ -4895,7 +4892,7 @@
       </c>
     </row>
     <row r="106" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A106" s="30"/>
+      <c r="A106" s="33"/>
       <c r="B106" s="2" t="s">
         <v>87</v>
       </c>
@@ -4919,7 +4916,7 @@
       </c>
     </row>
     <row r="107" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A107" s="30"/>
+      <c r="A107" s="33"/>
       <c r="B107" s="1" t="s">
         <v>90</v>
       </c>
@@ -4943,7 +4940,7 @@
       </c>
     </row>
     <row r="108" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A108" s="30"/>
+      <c r="A108" s="33"/>
       <c r="B108" s="2" t="s">
         <v>93</v>
       </c>
@@ -4967,7 +4964,7 @@
       </c>
     </row>
     <row r="109" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A109" s="30"/>
+      <c r="A109" s="33"/>
       <c r="B109" s="1" t="s">
         <v>97</v>
       </c>
@@ -4991,7 +4988,7 @@
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="30" t="s">
+      <c r="A110" s="33" t="s">
         <v>106</v>
       </c>
       <c r="B110" s="1" t="s">
@@ -5017,7 +5014,7 @@
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" s="30"/>
+      <c r="A111" s="33"/>
       <c r="B111" s="1" t="s">
         <v>102</v>
       </c>
@@ -5041,7 +5038,7 @@
       </c>
     </row>
     <row r="112" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A112" s="30" t="s">
+      <c r="A112" s="33" t="s">
         <v>61</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -5067,7 +5064,7 @@
       </c>
     </row>
     <row r="113" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" s="30"/>
+      <c r="A113" s="33"/>
       <c r="B113" s="1" t="s">
         <v>110</v>
       </c>
@@ -5091,7 +5088,7 @@
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="30"/>
+      <c r="A114" s="33"/>
       <c r="B114" s="1" t="s">
         <v>112</v>
       </c>
@@ -5115,7 +5112,7 @@
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="30"/>
+      <c r="A115" s="33"/>
       <c r="B115" s="1" t="s">
         <v>115</v>
       </c>
@@ -5139,7 +5136,7 @@
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" s="30"/>
+      <c r="A116" s="33"/>
       <c r="B116" s="1" t="s">
         <v>118</v>
       </c>
@@ -5163,7 +5160,7 @@
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117" s="30"/>
+      <c r="A117" s="33"/>
       <c r="B117" s="1" t="s">
         <v>123</v>
       </c>
@@ -5187,7 +5184,7 @@
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A118" s="30"/>
+      <c r="A118" s="33"/>
       <c r="B118" s="1" t="s">
         <v>124</v>
       </c>
@@ -5211,7 +5208,7 @@
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119" s="30"/>
+      <c r="A119" s="33"/>
       <c r="B119" s="1" t="s">
         <v>127</v>
       </c>
@@ -5235,7 +5232,7 @@
       </c>
     </row>
     <row r="120" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="30" t="s">
+      <c r="A120" s="33" t="s">
         <v>62</v>
       </c>
       <c r="B120" s="1" t="s">
@@ -5261,7 +5258,7 @@
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A121" s="30"/>
+      <c r="A121" s="33"/>
       <c r="B121" s="1" t="s">
         <v>133</v>
       </c>
@@ -5285,7 +5282,7 @@
       </c>
     </row>
     <row r="122" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A122" s="30" t="s">
+      <c r="A122" s="33" t="s">
         <v>63</v>
       </c>
       <c r="B122" s="1" t="s">
@@ -5311,7 +5308,7 @@
       </c>
     </row>
     <row r="123" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A123" s="30"/>
+      <c r="A123" s="33"/>
       <c r="B123" s="1" t="s">
         <v>139</v>
       </c>
@@ -5335,7 +5332,7 @@
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" s="30"/>
+      <c r="A124" s="33"/>
       <c r="B124" s="1" t="s">
         <v>142</v>
       </c>
@@ -5359,7 +5356,7 @@
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A125" s="30"/>
+      <c r="A125" s="33"/>
       <c r="B125" s="1" t="s">
         <v>146</v>
       </c>
@@ -5382,13 +5379,13 @@
         <v>148</v>
       </c>
     </row>
-    <row r="127" spans="1:9" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="31" t="s">
+    <row r="127" spans="1:9" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="30" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A128" s="30" t="s">
+      <c r="A128" s="33" t="s">
         <v>65</v>
       </c>
       <c r="B128" s="1" t="s">
@@ -5414,7 +5411,7 @@
       </c>
     </row>
     <row r="129" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A129" s="30"/>
+      <c r="A129" s="33"/>
       <c r="B129" s="2" t="s">
         <v>152</v>
       </c>
@@ -5438,7 +5435,7 @@
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A130" s="30"/>
+      <c r="A130" s="33"/>
       <c r="B130" s="2" t="s">
         <v>154</v>
       </c>
@@ -5462,7 +5459,7 @@
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A131" s="30"/>
+      <c r="A131" s="33"/>
       <c r="B131" s="1" t="s">
         <v>158</v>
       </c>
@@ -5486,7 +5483,7 @@
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="30"/>
+      <c r="A132" s="33"/>
       <c r="B132" s="2" t="s">
         <v>161</v>
       </c>
@@ -5510,7 +5507,7 @@
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A133" s="30"/>
+      <c r="A133" s="33"/>
       <c r="B133" s="2" t="s">
         <v>164</v>
       </c>
@@ -5534,7 +5531,7 @@
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A134" s="30"/>
+      <c r="A134" s="33"/>
       <c r="B134" s="1" t="s">
         <v>166</v>
       </c>
@@ -5558,7 +5555,7 @@
       </c>
     </row>
     <row r="135" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A135" s="30"/>
+      <c r="A135" s="33"/>
       <c r="B135" s="2" t="s">
         <v>169</v>
       </c>
@@ -5582,7 +5579,7 @@
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A136" s="30"/>
+      <c r="A136" s="33"/>
       <c r="B136" s="1" t="s">
         <v>172</v>
       </c>
@@ -5606,7 +5603,7 @@
       </c>
     </row>
     <row r="137" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A137" s="30"/>
+      <c r="A137" s="33"/>
       <c r="B137" s="1" t="s">
         <v>175</v>
       </c>
@@ -5630,7 +5627,7 @@
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A138" s="30"/>
+      <c r="A138" s="33"/>
       <c r="B138" s="1" t="s">
         <v>178</v>
       </c>
@@ -5654,7 +5651,7 @@
       </c>
     </row>
     <row r="139" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A139" s="30"/>
+      <c r="A139" s="33"/>
       <c r="B139" s="1" t="s">
         <v>181</v>
       </c>
@@ -5678,7 +5675,7 @@
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A140" s="30" t="s">
+      <c r="A140" s="33" t="s">
         <v>66</v>
       </c>
       <c r="B140" s="1" t="s">
@@ -5690,7 +5687,7 @@
       <c r="I140" s="1"/>
     </row>
     <row r="141" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A141" s="30"/>
+      <c r="A141" s="33"/>
       <c r="B141" s="2" t="s">
         <v>185</v>
       </c>
@@ -5714,7 +5711,7 @@
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A142" s="30"/>
+      <c r="A142" s="33"/>
       <c r="B142" s="1" t="s">
         <v>188</v>
       </c>
@@ -5726,7 +5723,7 @@
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A143" s="30"/>
+      <c r="A143" s="33"/>
       <c r="B143" s="1" t="s">
         <v>190</v>
       </c>
@@ -5746,13 +5743,13 @@
         <v>192</v>
       </c>
     </row>
-    <row r="145" spans="1:9" s="32" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="32" t="s">
+    <row r="145" spans="1:9" s="35" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="35" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A146" s="30" t="s">
+      <c r="A146" s="33" t="s">
         <v>416</v>
       </c>
       <c r="B146" s="1" t="s">
@@ -5766,7 +5763,7 @@
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A147" s="30"/>
+      <c r="A147" s="33"/>
       <c r="B147" s="1" t="s">
         <v>408</v>
       </c>
@@ -5781,7 +5778,7 @@
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A148" s="30"/>
+      <c r="A148" s="33"/>
       <c r="B148" s="1" t="s">
         <v>409</v>
       </c>
@@ -5793,7 +5790,7 @@
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A149" s="30"/>
+      <c r="A149" s="33"/>
       <c r="B149" s="1" t="s">
         <v>158</v>
       </c>
@@ -5811,7 +5808,7 @@
       </c>
     </row>
     <row r="150" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="30"/>
+      <c r="A150" s="33"/>
       <c r="B150" s="1" t="s">
         <v>410</v>
       </c>
@@ -5826,7 +5823,7 @@
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A151" s="30"/>
+      <c r="A151" s="33"/>
       <c r="B151" s="1" t="s">
         <v>432</v>
       </c>
@@ -5838,7 +5835,7 @@
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A152" s="30"/>
+      <c r="A152" s="33"/>
       <c r="B152" s="1" t="s">
         <v>411</v>
       </c>
@@ -5853,7 +5850,7 @@
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A153" s="30"/>
+      <c r="A153" s="33"/>
       <c r="B153" s="1" t="s">
         <v>412</v>
       </c>
@@ -5865,7 +5862,7 @@
       </c>
     </row>
     <row r="154" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A154" s="30"/>
+      <c r="A154" s="33"/>
       <c r="B154" s="1" t="s">
         <v>413</v>
       </c>
@@ -5877,7 +5874,7 @@
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A155" s="30"/>
+      <c r="A155" s="33"/>
       <c r="B155" s="1" t="s">
         <v>414</v>
       </c>
@@ -5906,7 +5903,7 @@
       </c>
     </row>
     <row r="157" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="30" t="s">
+      <c r="A157" s="33" t="s">
         <v>420</v>
       </c>
       <c r="B157" s="1" t="s">
@@ -5923,7 +5920,7 @@
       </c>
     </row>
     <row r="158" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A158" s="30"/>
+      <c r="A158" s="33"/>
       <c r="B158" s="1" t="s">
         <v>441</v>
       </c>
@@ -5941,7 +5938,7 @@
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A159" s="30"/>
+      <c r="A159" s="33"/>
       <c r="B159" s="1" t="s">
         <v>444</v>
       </c>
@@ -5953,7 +5950,7 @@
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A160" s="30"/>
+      <c r="A160" s="33"/>
       <c r="B160" s="1" t="s">
         <v>446</v>
       </c>
@@ -5965,7 +5962,7 @@
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A161" s="30"/>
+      <c r="A161" s="33"/>
       <c r="B161" s="1" t="s">
         <v>448</v>
       </c>
@@ -5977,7 +5974,7 @@
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A162" s="30"/>
+      <c r="A162" s="33"/>
       <c r="B162" s="1" t="s">
         <v>450</v>
       </c>
@@ -5989,7 +5986,7 @@
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A163" s="30"/>
+      <c r="A163" s="33"/>
       <c r="B163" s="1" t="s">
         <v>452</v>
       </c>
@@ -6001,7 +5998,7 @@
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A164" s="30" t="s">
+      <c r="A164" s="33" t="s">
         <v>454</v>
       </c>
       <c r="B164" s="1" t="s">
@@ -6018,7 +6015,7 @@
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A165" s="30"/>
+      <c r="A165" s="33"/>
       <c r="B165" s="1" t="s">
         <v>457</v>
       </c>
@@ -6030,7 +6027,7 @@
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A166" s="30" t="s">
+      <c r="A166" s="33" t="s">
         <v>458</v>
       </c>
       <c r="B166" s="1" t="s">
@@ -6047,7 +6044,7 @@
       </c>
     </row>
     <row r="167" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A167" s="30"/>
+      <c r="A167" s="33"/>
       <c r="B167" s="1" t="s">
         <v>461</v>
       </c>
@@ -6062,7 +6059,7 @@
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A168" s="30" t="s">
+      <c r="A168" s="33" t="s">
         <v>463</v>
       </c>
       <c r="B168" s="1" t="s">
@@ -6079,7 +6076,7 @@
       </c>
     </row>
     <row r="169" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="30"/>
+      <c r="A169" s="33"/>
       <c r="B169" s="1" t="s">
         <v>465</v>
       </c>
@@ -6094,7 +6091,7 @@
       </c>
     </row>
     <row r="170" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="30" t="s">
+      <c r="A170" s="33" t="s">
         <v>467</v>
       </c>
       <c r="B170" s="1" t="s">
@@ -6115,7 +6112,7 @@
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A171" s="30"/>
+      <c r="A171" s="33"/>
       <c r="B171" s="1" t="s">
         <v>469</v>
       </c>
@@ -6128,14 +6125,14 @@
       <c r="H171" s="7"/>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A172" s="30"/>
+      <c r="A172" s="33"/>
       <c r="B172" s="1" t="s">
         <v>470</v>
       </c>
       <c r="H172" s="7"/>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A173" s="30"/>
+      <c r="A173" s="33"/>
       <c r="B173" s="1" t="s">
         <v>471</v>
       </c>
@@ -6148,14 +6145,14 @@
       <c r="H173" s="7"/>
     </row>
     <row r="174" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A174" s="30"/>
+      <c r="A174" s="33"/>
       <c r="B174" s="1" t="s">
         <v>472</v>
       </c>
       <c r="H174" s="7"/>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A175" s="30"/>
+      <c r="A175" s="33"/>
       <c r="B175" s="1" t="s">
         <v>473</v>
       </c>
@@ -6168,7 +6165,7 @@
       <c r="H175" s="7"/>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A176" s="30"/>
+      <c r="A176" s="33"/>
       <c r="B176" s="1" t="s">
         <v>474</v>
       </c>
@@ -6181,7 +6178,7 @@
       <c r="H176" s="7"/>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A177" s="30"/>
+      <c r="A177" s="33"/>
       <c r="B177" s="1" t="s">
         <v>475</v>
       </c>
@@ -6194,7 +6191,7 @@
       <c r="H177" s="7"/>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A178" s="30"/>
+      <c r="A178" s="33"/>
       <c r="B178" s="1" t="s">
         <v>476</v>
       </c>
@@ -6207,7 +6204,7 @@
       <c r="H178" s="7"/>
     </row>
     <row r="179" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="30" t="s">
+      <c r="A179" s="33" t="s">
         <v>478</v>
       </c>
       <c r="B179" s="1" t="s">
@@ -6225,7 +6222,7 @@
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A180" s="30"/>
+      <c r="A180" s="33"/>
       <c r="B180" s="1" t="s">
         <v>480</v>
       </c>
@@ -6238,7 +6235,7 @@
       <c r="H180" s="7"/>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A181" s="30"/>
+      <c r="A181" s="33"/>
       <c r="B181" s="1" t="s">
         <v>481</v>
       </c>
@@ -6251,7 +6248,7 @@
       <c r="H181" s="7"/>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A182" s="30"/>
+      <c r="A182" s="33"/>
       <c r="B182" s="1" t="s">
         <v>482</v>
       </c>
@@ -6264,7 +6261,7 @@
       <c r="H182" s="7"/>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A183" s="30"/>
+      <c r="A183" s="33"/>
       <c r="B183" s="1" t="s">
         <v>483</v>
       </c>
@@ -6277,7 +6274,7 @@
       <c r="H183" s="7"/>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A184" s="30"/>
+      <c r="A184" s="33"/>
       <c r="B184" s="1" t="s">
         <v>484</v>
       </c>
@@ -6290,7 +6287,7 @@
       <c r="H184" s="7"/>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A185" s="30"/>
+      <c r="A185" s="33"/>
       <c r="B185" s="1" t="s">
         <v>485</v>
       </c>
@@ -6303,7 +6300,7 @@
       <c r="H185" s="7"/>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A186" s="30"/>
+      <c r="A186" s="33"/>
       <c r="B186" s="1" t="s">
         <v>486</v>
       </c>
@@ -6316,7 +6313,7 @@
       <c r="H186" s="7"/>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A187" s="30"/>
+      <c r="A187" s="33"/>
       <c r="B187" s="1" t="s">
         <v>487</v>
       </c>
@@ -6329,7 +6326,7 @@
       <c r="H187" s="7"/>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A188" s="30"/>
+      <c r="A188" s="33"/>
       <c r="B188" s="1" t="s">
         <v>488</v>
       </c>
@@ -6342,7 +6339,7 @@
       <c r="H188" s="7"/>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A189" s="30"/>
+      <c r="A189" s="33"/>
       <c r="B189" s="2" t="s">
         <v>489</v>
       </c>
@@ -6355,7 +6352,7 @@
       <c r="H189" s="7"/>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A190" s="30"/>
+      <c r="A190" s="33"/>
       <c r="B190" s="1" t="s">
         <v>490</v>
       </c>
@@ -6388,7 +6385,7 @@
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A192" s="30" t="s">
+      <c r="A192" s="33" t="s">
         <v>495</v>
       </c>
       <c r="B192" s="1" t="s">
@@ -6408,7 +6405,7 @@
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A193" s="30"/>
+      <c r="A193" s="33"/>
       <c r="B193" s="1" t="s">
         <v>498</v>
       </c>
@@ -6417,7 +6414,7 @@
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A194" s="30" t="s">
+      <c r="A194" s="33" t="s">
         <v>106</v>
       </c>
       <c r="B194" s="1" t="s">
@@ -6434,7 +6431,7 @@
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A195" s="30"/>
+      <c r="A195" s="33"/>
       <c r="B195" s="1" t="s">
         <v>502</v>
       </c>
@@ -6448,24 +6445,14 @@
   </sheetData>
   <autoFilter ref="E1:E195" xr:uid="{1CD66C7E-061F-43E9-BB3A-8D29200B2BF1}"/>
   <mergeCells count="40">
-    <mergeCell ref="A83:XFD83"/>
-    <mergeCell ref="A99:XFD99"/>
-    <mergeCell ref="A3:XFD3"/>
-    <mergeCell ref="A17:XFD17"/>
-    <mergeCell ref="A49:A63"/>
-    <mergeCell ref="A66:A72"/>
-    <mergeCell ref="A73:A81"/>
-    <mergeCell ref="A65:XFD65"/>
-    <mergeCell ref="A19:A27"/>
-    <mergeCell ref="A28:A36"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="A4:XFD4"/>
-    <mergeCell ref="A7:XFD7"/>
-    <mergeCell ref="A10:XFD10"/>
-    <mergeCell ref="A18:XFD18"/>
+    <mergeCell ref="A179:A190"/>
+    <mergeCell ref="A192:A193"/>
+    <mergeCell ref="A194:A195"/>
+    <mergeCell ref="A157:A163"/>
+    <mergeCell ref="A164:A165"/>
+    <mergeCell ref="A166:A167"/>
+    <mergeCell ref="A168:A169"/>
+    <mergeCell ref="A170:A178"/>
     <mergeCell ref="A146:A155"/>
     <mergeCell ref="A84:A88"/>
     <mergeCell ref="A89:A90"/>
@@ -6480,14 +6467,24 @@
     <mergeCell ref="A122:A125"/>
     <mergeCell ref="A128:A139"/>
     <mergeCell ref="A140:A143"/>
-    <mergeCell ref="A179:A190"/>
-    <mergeCell ref="A192:A193"/>
-    <mergeCell ref="A194:A195"/>
-    <mergeCell ref="A157:A163"/>
-    <mergeCell ref="A164:A165"/>
-    <mergeCell ref="A166:A167"/>
-    <mergeCell ref="A168:A169"/>
-    <mergeCell ref="A170:A178"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="A4:XFD4"/>
+    <mergeCell ref="A7:XFD7"/>
+    <mergeCell ref="A10:XFD10"/>
+    <mergeCell ref="A18:XFD18"/>
+    <mergeCell ref="A83:XFD83"/>
+    <mergeCell ref="A99:XFD99"/>
+    <mergeCell ref="A3:XFD3"/>
+    <mergeCell ref="A17:XFD17"/>
+    <mergeCell ref="A49:A63"/>
+    <mergeCell ref="A66:A72"/>
+    <mergeCell ref="A73:A81"/>
+    <mergeCell ref="A65:XFD65"/>
+    <mergeCell ref="A19:A27"/>
+    <mergeCell ref="A28:A36"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A47:A48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I61" r:id="rId1" xr:uid="{551A33CD-200A-4B76-8CDC-E646EC35A9E5}"/>
@@ -6539,8 +6536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27833425-745A-496A-BBBC-9D84991CFB19}">
   <dimension ref="B2:S199"/>
   <sheetViews>
-    <sheetView zoomScale="88" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="88" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6563,7 +6560,7 @@
   <sheetData>
     <row r="2" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="27" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D2" s="1"/>
       <c r="F2" s="26" t="s">
@@ -6576,7 +6573,7 @@
       <c r="I2" s="37"/>
       <c r="J2" s="37"/>
       <c r="M2" s="27" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="36"/>
@@ -6594,7 +6591,7 @@
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="11"/>
       <c r="C4" s="24" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="24" t="s">
@@ -6611,7 +6608,7 @@
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
       <c r="M4" s="16" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="S4" s="14"/>
     </row>
@@ -6664,7 +6661,7 @@
         <v>2024</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E7">
         <v>2024</v>
@@ -6680,7 +6677,7 @@
         <v>2024</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E8">
         <v>2024</v>
@@ -6695,7 +6692,7 @@
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
       <c r="M8" s="16" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="S8" s="14"/>
     </row>
@@ -6753,7 +6750,7 @@
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
       <c r="M11" s="16" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="S11" s="14"/>
     </row>
@@ -6803,7 +6800,7 @@
     <row r="14" spans="2:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11"/>
       <c r="C14" s="24" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E14">
         <v>2024</v>
@@ -6826,7 +6823,7 @@
         <v>2022</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E15">
         <v>2024</v>
@@ -6842,7 +6839,7 @@
         <v>2022</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E16">
         <v>2023</v>
@@ -6854,7 +6851,7 @@
       <c r="J16"/>
       <c r="L16" s="12"/>
       <c r="M16" s="16" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="N16" s="15"/>
       <c r="P16" s="14"/>
@@ -6962,7 +6959,7 @@
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
       <c r="M21" s="16" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
@@ -6977,11 +6974,11 @@
     <row r="23" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="11"/>
       <c r="C23" s="24" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="25" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="20" t="s">
@@ -7030,7 +7027,7 @@
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
       <c r="M25" s="16" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
@@ -7072,7 +7069,7 @@
         <v>2020</v>
       </c>
       <c r="M27" s="17" t="s">
-        <v>568</v>
+        <v>585</v>
       </c>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
@@ -7814,6 +7811,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="9050bc6f-8f89-47a3-86fa-b072ef53d328" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F6363AD6CE09334FA2B4FF9AA95D73C5" ma:contentTypeVersion="15" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="fea41b385c3c40a857800e800f56fbc8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9050bc6f-8f89-47a3-86fa-b072ef53d328" xmlns:ns4="bccbb3ce-f1a4-4a6f-aa39-0efc4956b4fd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="507616ff13059a37d7288ac12b1b548c" ns3:_="" ns4:_="">
     <xsd:import namespace="9050bc6f-8f89-47a3-86fa-b072ef53d328"/>
@@ -8046,14 +8051,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="9050bc6f-8f89-47a3-86fa-b072ef53d328" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55792E88-4A72-42AB-9F80-0618B4EBFE2A}">
   <ds:schemaRefs>
@@ -8063,6 +8060,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFC416A1-3111-4849-A533-05CA95BC2A5C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bccbb3ce-f1a4-4a6f-aa39-0efc4956b4fd"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9050bc6f-8f89-47a3-86fa-b072ef53d328"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13FC5822-06D7-4595-B74F-3FC67EA3A23C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8079,21 +8093,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFC416A1-3111-4849-A533-05CA95BC2A5C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="bccbb3ce-f1a4-4a6f-aa39-0efc4956b4fd"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="9050bc6f-8f89-47a3-86fa-b072ef53d328"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updating metadata on the dahsboard
</commit_message>
<xml_diff>
--- a/frontend/data/data_available.xlsx
+++ b/frontend/data/data_available.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bianka\Documents\MSc-Internship\Observatory-of-the-Mountains\frontend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199C7C39-C643-4304-AEC1-A664BC26866E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06A039C-D867-43CA-B369-EA05A02727EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{8809251D-B3C6-41F0-B60D-9556D90BF91D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{8809251D-B3C6-41F0-B60D-9556D90BF91D}"/>
   </bookViews>
   <sheets>
     <sheet name="per county" sheetId="1" r:id="rId1"/>
     <sheet name="per topic" sheetId="4" r:id="rId2"/>
+    <sheet name="Q1_a" sheetId="5" r:id="rId3"/>
+    <sheet name="Q1_b" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'per county'!$E$1:$E$195</definedName>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="604">
   <si>
     <r>
       <t xml:space="preserve">gencat </t>
@@ -2073,6 +2075,161 @@
   </si>
   <si>
     <t>unique biodiversity</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>specifications</t>
+  </si>
+  <si>
+    <t>population strucutre by sex and age group</t>
+  </si>
+  <si>
+    <t>public sector finance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, surfaces area, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>density</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>population strucutre by</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sex </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>age group</t>
+    </r>
+  </si>
+  <si>
+    <t>level of education attained (illiterate, primary, secondary, university edu)</t>
+  </si>
+  <si>
+    <t>GDP</t>
+  </si>
+  <si>
+    <t>rural estate tax</t>
+  </si>
+  <si>
+    <t>urban estate tax</t>
+  </si>
+  <si>
+    <t>cleared forest</t>
+  </si>
+  <si>
+    <t>reforested area</t>
+  </si>
+  <si>
+    <t>forest fire</t>
+  </si>
+  <si>
+    <t>organic farms</t>
+  </si>
+  <si>
+    <t>municipal waste</t>
+  </si>
+  <si>
+    <r>
+      <t>6. Pyrenean</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tourism</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> integral, regenerative and sustainable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Population</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2129,7 +2286,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2154,8 +2311,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F8D8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -2218,12 +2381,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2316,6 +2488,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hypertextové prepojenie" xfId="1" builtinId="8"/>
@@ -2325,6 +2531,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF8F8D8"/>
       <color rgb="FFFDA631"/>
     </mruColors>
   </colors>
@@ -2659,8 +2866,8 @@
   <dimension ref="A1:I195"/>
   <sheetViews>
     <sheetView zoomScale="88" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B148" sqref="B148"/>
+      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B131" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6536,8 +6743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27833425-745A-496A-BBBC-9D84991CFB19}">
   <dimension ref="B2:S199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="88" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView topLeftCell="A13" zoomScale="88" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7796,6 +8003,3721 @@
   <mergeCells count="2">
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="H2:J2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC2F606-BCE5-41DE-997B-370E48010E8A}">
+  <dimension ref="A1:H129"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="H123" sqref="H123"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" style="1" customWidth="1"/>
+    <col min="3" max="5" width="23.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="69" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="38" t="s">
+        <v>421</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>422</v>
+      </c>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1986</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="33"/>
+      <c r="B6" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1981</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="33"/>
+      <c r="B7" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1986</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="33"/>
+      <c r="B8" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="33"/>
+      <c r="B9" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1996</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="33"/>
+      <c r="B10" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1996</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="33"/>
+      <c r="B11" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2004</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="33"/>
+      <c r="B12" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2009</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2025</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="33"/>
+      <c r="B13" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2009</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2025</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E14" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="33"/>
+      <c r="B15" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E15" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="33"/>
+      <c r="B16" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="33"/>
+      <c r="B17" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1997</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E17" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="33"/>
+      <c r="B18" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1998</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="33"/>
+      <c r="B19" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E19" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="33"/>
+      <c r="B20" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="33"/>
+      <c r="B21" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="33"/>
+      <c r="B22" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2004</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E22" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
+        <v>346</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2002</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="33"/>
+      <c r="B24" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2002</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="33"/>
+      <c r="B25" s="43" t="s">
+        <v>335</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E25" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="33"/>
+      <c r="B26" s="43" t="s">
+        <v>338</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E26" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="33"/>
+      <c r="B27" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E27" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="33"/>
+      <c r="B28" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1996</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E28" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="E29" s="1">
+        <v>2019</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="33"/>
+      <c r="B30" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C30" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="E30" s="1">
+        <v>2019</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="33"/>
+      <c r="B31" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E31" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="33"/>
+      <c r="B32" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="E32" s="1">
+        <v>2019</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E33" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="33"/>
+      <c r="B34" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2004</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E34" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="H34" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E35" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="33"/>
+      <c r="B36" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E36" s="1">
+        <v>2015</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="33"/>
+      <c r="B37" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E37" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="H37" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="33"/>
+      <c r="B38" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E38" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="H38" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="33"/>
+      <c r="B39" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E39" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="33"/>
+      <c r="B40" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C40" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E40" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="H40" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="33"/>
+      <c r="B41" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1996</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E41" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="H41" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="33"/>
+      <c r="B42" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="C42" s="1">
+        <v>1996</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E42" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="H42" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="33"/>
+      <c r="B43" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1996</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E43" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G43" s="43" t="s">
+        <v>388</v>
+      </c>
+      <c r="H43" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="33"/>
+      <c r="B44" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1996</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E44" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="H44" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="33"/>
+      <c r="B45" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1996</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E45" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="33"/>
+      <c r="B46" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1996</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E46" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="H46" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="33"/>
+      <c r="B47" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C47" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E47" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="33"/>
+      <c r="B48" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E48" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="H48" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="33"/>
+      <c r="B49" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E49" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1990</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E52" s="1">
+        <v>2011</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="33"/>
+      <c r="B53" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1990</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E53" s="1">
+        <v>2011</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="H53" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="33"/>
+      <c r="B54" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1990</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E54" s="1">
+        <v>2011</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="H54" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="33"/>
+      <c r="B55" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1990</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E55" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="33"/>
+      <c r="B56" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1990</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E56" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="H56" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="33"/>
+      <c r="B57" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C57" s="1">
+        <v>2001</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E57" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H57" s="8" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="33"/>
+      <c r="B58" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C58" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E58" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C59" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E59" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="33"/>
+      <c r="B60" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C60" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E60" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="H60" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="33"/>
+      <c r="B61" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C61" s="1">
+        <v>2001</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E61" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H61" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="33"/>
+      <c r="B62" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C62" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E62" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="H62" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="33"/>
+      <c r="B63" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C63" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E63" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="H63" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="33"/>
+      <c r="B64" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C64" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E64" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="H64" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="33"/>
+      <c r="B65" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C65" s="1">
+        <v>2018</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E65" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="H65" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="33"/>
+      <c r="B66" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C66" s="1">
+        <v>2011</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E66" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="33"/>
+      <c r="B67" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C67" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E67" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C70" s="1">
+        <v>2001</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E70" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H70" s="8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="33"/>
+      <c r="B71" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C71" s="1">
+        <v>2006</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E71" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A72" s="33"/>
+      <c r="B72" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C72" s="1">
+        <v>2006</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E72" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="H72" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="33"/>
+      <c r="B73" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C73" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E73" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="H73" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="33"/>
+      <c r="B74" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C74" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E74" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H74" s="8" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C75" s="1">
+        <v>1996</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E75" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="H75" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="33"/>
+      <c r="B76" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C76" s="1">
+        <v>2002</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E76" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="H76" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="33" t="s">
+        <v>589</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C77" s="1">
+        <v>1995</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E77" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H77" s="8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="33"/>
+      <c r="B78" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C78" s="1">
+        <v>2002</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E78" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H78" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="33"/>
+      <c r="B79" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C79" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E79" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="33"/>
+      <c r="B80" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C80" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E80" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="H80" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="33"/>
+      <c r="B81" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C81" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E81" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="H81" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C82" s="1">
+        <v>2005</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E82" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="H82" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="33"/>
+      <c r="B83" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C83" s="1">
+        <v>2005</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E83" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="H83" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A86" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C86" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E86" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H86" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="33"/>
+      <c r="B87" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C87" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E87" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H87" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A88" s="33"/>
+      <c r="B88" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C88" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E88" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H88" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="33"/>
+      <c r="B89" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C89" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E89" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H89" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="33"/>
+      <c r="B90" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C90" s="1">
+        <v>2009</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E90" s="1">
+        <v>1999</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H90" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="33"/>
+      <c r="B91" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C91" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E91" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A92" s="33"/>
+      <c r="B92" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="C92" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E92" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H92" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A93" s="33"/>
+      <c r="B93" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C93" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E93" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H93" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A94" s="33"/>
+      <c r="B94" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C94" s="1">
+        <v>2009</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E94" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H94" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A95" s="33"/>
+      <c r="B95" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C95" s="1">
+        <v>2020</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="E95" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H95" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C96" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E96" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H96" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="33"/>
+      <c r="B97" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C97" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E97" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H97" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C98" s="1">
+        <v>2003</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E98" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H98" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="33"/>
+      <c r="B99" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C99" s="1">
+        <v>2003</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E99" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H99" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" s="33"/>
+      <c r="B100" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C100" s="1">
+        <v>1996</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E100" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H100" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="33"/>
+      <c r="B101" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C101" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E101" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H101" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="33"/>
+      <c r="B102" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C102" s="1">
+        <v>2005</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E102" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H102" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="33"/>
+      <c r="B103" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C103" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E103" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H103" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="33"/>
+      <c r="B104" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C104" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E104" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H104" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" s="33"/>
+      <c r="B105" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C105" s="1">
+        <v>2004</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E105" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H105" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A106" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C106" s="1">
+        <v>2002</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E106" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H106" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="33"/>
+      <c r="B107" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C107" s="1">
+        <v>2004</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E107" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H107" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C108" s="1">
+        <v>2003</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E108" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H108" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A109" s="33"/>
+      <c r="B109" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C109" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E109" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H109" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" s="33"/>
+      <c r="B110" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C110" s="1">
+        <v>2003</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E110" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H110" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="33"/>
+      <c r="B111" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C111" s="1">
+        <v>2002</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E111" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H111" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A114" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C114" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E114" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H114" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A115" s="33"/>
+      <c r="B115" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C115" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E115" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H115" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" s="33"/>
+      <c r="B116" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C116" s="1">
+        <v>2002</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E116" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H116" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" s="33"/>
+      <c r="B117" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C117" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E117" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H117" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" s="33"/>
+      <c r="B118" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C118" s="1">
+        <v>1998</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E118" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H118" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" s="33"/>
+      <c r="B119" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C119" s="1">
+        <v>1998</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E119" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H119" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" s="33"/>
+      <c r="B120" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C120" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E120" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H120" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A121" s="33"/>
+      <c r="B121" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C121" s="1">
+        <v>2001</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E121" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H121" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" s="33"/>
+      <c r="B122" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C122" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E122" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H122" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A123" s="33"/>
+      <c r="B123" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C123" s="1">
+        <v>1995</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E123" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="H123" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="33"/>
+      <c r="B124" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C124" s="1">
+        <v>1995</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E124" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G124" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H124" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A125" s="33"/>
+      <c r="B125" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C125" s="1">
+        <v>1995</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E125" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H125" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="H126" s="1"/>
+    </row>
+    <row r="127" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A127" s="33"/>
+      <c r="B127" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C127" s="1">
+        <v>2001</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E127" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="H127" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="33"/>
+      <c r="B128" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="H128" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A129" s="33"/>
+      <c r="B129" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C129" s="1">
+        <v>2003</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E129" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H129" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="26">
+    <mergeCell ref="A98:A105"/>
+    <mergeCell ref="A106:A107"/>
+    <mergeCell ref="A108:A111"/>
+    <mergeCell ref="A113:XFD113"/>
+    <mergeCell ref="A114:A125"/>
+    <mergeCell ref="A126:A129"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="A77:A81"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="A85:XFD85"/>
+    <mergeCell ref="A86:A95"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="A35:A49"/>
+    <mergeCell ref="A51:XFD51"/>
+    <mergeCell ref="A52:A58"/>
+    <mergeCell ref="A59:A67"/>
+    <mergeCell ref="A69:XFD69"/>
+    <mergeCell ref="A70:A74"/>
+    <mergeCell ref="A4:XFD4"/>
+    <mergeCell ref="A5:A13"/>
+    <mergeCell ref="A14:A22"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="A3:XFD3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H47" r:id="rId1" xr:uid="{2424F334-F3B8-40C2-B211-E0F49AA3181B}"/>
+    <hyperlink ref="H45" r:id="rId2" xr:uid="{F6DFB795-2BE4-4938-B3C8-5213355F212F}"/>
+    <hyperlink ref="H39" r:id="rId3" xr:uid="{0F9933DD-436F-469A-9EBA-42C0B58E253D}"/>
+    <hyperlink ref="H35" r:id="rId4" xr:uid="{EC111B6A-2FC7-4CD8-B604-236E06CCA543}"/>
+    <hyperlink ref="H31" r:id="rId5" xr:uid="{A93CB1B0-90C2-467E-BEEB-59C5C0B34896}"/>
+    <hyperlink ref="H28" r:id="rId6" xr:uid="{741D5410-5E93-43E4-AD69-F5FAFFC801CE}"/>
+    <hyperlink ref="H66" r:id="rId7" xr:uid="{673A7AD1-4759-4376-AF9F-12281AB3299A}"/>
+    <hyperlink ref="H59" r:id="rId8" xr:uid="{2D3D5701-D771-47F8-A0E8-67582E0DFE2F}"/>
+    <hyperlink ref="H79" r:id="rId9" xr:uid="{E89E9370-0534-438A-815F-52D38ABEA542}"/>
+    <hyperlink ref="H71" r:id="rId10" xr:uid="{C16D8463-E246-417A-8B58-A555FCAC4FDC}"/>
+    <hyperlink ref="H128" r:id="rId11" xr:uid="{D609079C-A715-46CE-A759-E62C558C857C}"/>
+    <hyperlink ref="H124" r:id="rId12" xr:uid="{0F374A52-B81A-435C-AA43-BF913F6A0895}"/>
+    <hyperlink ref="H123" r:id="rId13" xr:uid="{89DBF275-7946-469C-ADB3-AFBDF181C169}"/>
+    <hyperlink ref="H122" r:id="rId14" xr:uid="{E44D32D0-B2E6-4578-8934-45DCD7972ABF}"/>
+    <hyperlink ref="H118" r:id="rId15" xr:uid="{1B2A9649-070B-4CCA-AC55-6B504FD9D718}"/>
+    <hyperlink ref="H114" r:id="rId16" xr:uid="{16100FF5-125C-4758-AA77-E110D497BCED}"/>
+    <hyperlink ref="H116" r:id="rId17" xr:uid="{BB53B571-0249-4406-913A-E4FB9A62AD63}"/>
+    <hyperlink ref="H115" r:id="rId18" xr:uid="{5E09660D-9E54-43BB-8EED-F421B98FC018}"/>
+    <hyperlink ref="H91" r:id="rId19" xr:uid="{24E948A5-AE4B-4237-BB6C-DAC8E654D5FD}"/>
+    <hyperlink ref="H88" r:id="rId20" xr:uid="{C0365081-E747-45B0-9868-4BAFE1217C05}"/>
+    <hyperlink ref="H5" r:id="rId21" xr:uid="{368FBA2A-ACA0-4623-AF30-EDF66A093E11}"/>
+    <hyperlink ref="H70" r:id="rId22" xr:uid="{6EFBB78E-55E4-4021-836B-3321B4F7BCF7}"/>
+    <hyperlink ref="H25" r:id="rId23" xr:uid="{B96A134D-E7D9-4340-9FB7-F3A2420C4118}"/>
+    <hyperlink ref="H49" r:id="rId24" xr:uid="{1BB90E44-9C7F-4F9A-AC89-64BE598CB294}"/>
+    <hyperlink ref="H36" r:id="rId25" xr:uid="{98A54A36-8969-4433-ADC1-A00BE53D7BE6}"/>
+    <hyperlink ref="H52" r:id="rId26" xr:uid="{F1B0217E-D120-427C-A87C-2ECC1098CBEB}"/>
+    <hyperlink ref="H127" r:id="rId27" xr:uid="{5D0D43B0-F6BF-4050-A352-0EC7BA2AD9AA}"/>
+    <hyperlink ref="H55" r:id="rId28" xr:uid="{2F0F8934-87BC-45AE-869B-F8F976DB1002}"/>
+    <hyperlink ref="H8" r:id="rId29" xr:uid="{92B87662-7013-40ED-9031-DD37A0D4C365}"/>
+    <hyperlink ref="H74" r:id="rId30" xr:uid="{DA2D3C41-6469-43E1-B79B-9CCEE049EBEF}"/>
+    <hyperlink ref="H77" r:id="rId31" xr:uid="{5E2A9DED-F51D-4B03-AAD8-745D10688DF3}"/>
+    <hyperlink ref="H96" r:id="rId32" xr:uid="{A4C18DB2-9A8E-4469-8C64-8EEA714DB554}"/>
+    <hyperlink ref="H57" r:id="rId33" xr:uid="{19A721BE-E8C3-4938-A2F4-9CE4F53A341A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId34"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C15B307-9B65-4164-8063-9F476182200F}">
+  <dimension ref="B2:O180"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="49.7109375" style="15" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="23" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" customWidth="1"/>
+    <col min="9" max="9" width="49.28515625" style="15" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="26" t="s">
+        <v>558</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="37" t="s">
+        <v>557</v>
+      </c>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="I2" s="27" t="s">
+        <v>578</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E3" s="18" t="s">
+        <v>556</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="19" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C4" s="39" t="s">
+        <v>603</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="21" t="s">
+        <v>552</v>
+      </c>
+      <c r="H4" s="12"/>
+      <c r="I4" s="16"/>
+      <c r="O4" s="14"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C5" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="I5" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="O5" s="14"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C6" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="I6" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="O6" s="14"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C7" s="17" t="s">
+        <v>570</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="O7" s="14"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C8" s="17" t="s">
+        <v>588</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="21" t="s">
+        <v>530</v>
+      </c>
+      <c r="H8" s="12"/>
+      <c r="I8" s="16"/>
+      <c r="O8" s="14"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F9" s="13"/>
+      <c r="I9" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="O9" s="14"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C10" s="24" t="s">
+        <v>554</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="20" t="s">
+        <v>553</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="I10" s="17" t="s">
+        <v>600</v>
+      </c>
+      <c r="O10" s="14"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C11" s="17" t="s">
+        <v>551</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="O11" s="14"/>
+    </row>
+    <row r="12" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="F12" s="13"/>
+      <c r="G12" s="21" t="s">
+        <v>548</v>
+      </c>
+      <c r="H12" s="12"/>
+      <c r="I12" s="16"/>
+      <c r="K12" s="3"/>
+      <c r="O12" s="14"/>
+    </row>
+    <row r="13" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="I13" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="K13" s="3"/>
+      <c r="O13" s="14"/>
+    </row>
+    <row r="14" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="46" t="s">
+        <v>590</v>
+      </c>
+      <c r="H14" s="15"/>
+      <c r="I14" s="17" t="s">
+        <v>601</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="O14" s="14"/>
+    </row>
+    <row r="15" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="13"/>
+      <c r="K15" s="45"/>
+      <c r="O15" s="14"/>
+    </row>
+    <row r="16" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="24" t="s">
+        <v>549</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="E16" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="14"/>
+      <c r="O16" s="14"/>
+    </row>
+    <row r="17" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="15" t="s">
+        <v>547</v>
+      </c>
+      <c r="F17" s="13"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="14"/>
+      <c r="O17" s="14"/>
+    </row>
+    <row r="18" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="15" t="s">
+        <v>546</v>
+      </c>
+      <c r="F18" s="13"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="15"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="14"/>
+      <c r="O18" s="14"/>
+    </row>
+    <row r="19" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="15" t="s">
+        <v>545</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>512</v>
+      </c>
+      <c r="F19" s="13"/>
+      <c r="G19" s="49" t="s">
+        <v>533</v>
+      </c>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="14"/>
+      <c r="O19" s="14"/>
+    </row>
+    <row r="20" spans="3:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="15" t="s">
+        <v>544</v>
+      </c>
+      <c r="F20" s="13"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="J20" s="53"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="14"/>
+      <c r="O20" s="14"/>
+    </row>
+    <row r="21" spans="3:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="15" t="s">
+        <v>543</v>
+      </c>
+      <c r="F21" s="13"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="15"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="14"/>
+      <c r="O21" s="14"/>
+    </row>
+    <row r="22" spans="3:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="15" t="s">
+        <v>542</v>
+      </c>
+      <c r="F22" s="13"/>
+      <c r="G22" s="49" t="s">
+        <v>523</v>
+      </c>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="14"/>
+      <c r="O22" s="14"/>
+    </row>
+    <row r="23" spans="3:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="F23" s="13"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="K23" s="45"/>
+      <c r="O23" s="14"/>
+    </row>
+    <row r="24" spans="3:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="40" t="s">
+        <v>208</v>
+      </c>
+      <c r="F24" s="13"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="17" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C25" s="15" t="s">
+        <v>541</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="52" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C26" s="44" t="s">
+        <v>593</v>
+      </c>
+      <c r="F26" s="13"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="15"/>
+    </row>
+    <row r="27" spans="3:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="F27" s="13"/>
+      <c r="G27" s="50" t="s">
+        <v>539</v>
+      </c>
+      <c r="H27" s="42"/>
+      <c r="I27" s="17"/>
+    </row>
+    <row r="28" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C28" s="25" t="s">
+        <v>571</v>
+      </c>
+      <c r="D28" s="10"/>
+      <c r="E28" s="20" t="s">
+        <v>540</v>
+      </c>
+      <c r="F28" s="13"/>
+      <c r="G28" s="51" t="s">
+        <v>515</v>
+      </c>
+      <c r="H28" s="15"/>
+      <c r="I28" s="17"/>
+    </row>
+    <row r="29" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C29" s="17" t="s">
+        <v>594</v>
+      </c>
+      <c r="F29" s="13"/>
+      <c r="G29" s="51" t="s">
+        <v>514</v>
+      </c>
+      <c r="H29" s="15"/>
+    </row>
+    <row r="30" spans="3:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="C30" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="F30" s="13"/>
+      <c r="G30" s="51" t="s">
+        <v>513</v>
+      </c>
+      <c r="H30" s="15"/>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C31" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="F31" s="13"/>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C32" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="F32" s="13"/>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C33" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="F33" s="13"/>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C34" s="17" t="s">
+        <v>595</v>
+      </c>
+      <c r="F34" s="13"/>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C35" s="17" t="s">
+        <v>596</v>
+      </c>
+      <c r="F35" s="13"/>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C36" s="17" t="s">
+        <v>383</v>
+      </c>
+      <c r="F36" s="13"/>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C37" s="17" t="s">
+        <v>384</v>
+      </c>
+      <c r="F37" s="13"/>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C38" s="17" t="s">
+        <v>562</v>
+      </c>
+      <c r="F38" s="13"/>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="13"/>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C40" s="24" t="s">
+        <v>535</v>
+      </c>
+      <c r="D40" s="10"/>
+      <c r="E40" s="20" t="s">
+        <v>534</v>
+      </c>
+      <c r="F40" s="13"/>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F41" s="13"/>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C42" s="24" t="s">
+        <v>532</v>
+      </c>
+      <c r="D42" s="10"/>
+      <c r="E42" s="20" t="s">
+        <v>531</v>
+      </c>
+      <c r="F42" s="13"/>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C43" s="15" t="s">
+        <v>529</v>
+      </c>
+      <c r="F43" s="13"/>
+    </row>
+    <row r="44" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F44" s="13"/>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C45" s="15" t="s">
+        <v>528</v>
+      </c>
+      <c r="F45" s="13"/>
+    </row>
+    <row r="46" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="15" t="s">
+        <v>527</v>
+      </c>
+      <c r="F46" s="13"/>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C47" s="17" t="s">
+        <v>526</v>
+      </c>
+      <c r="F47" s="13"/>
+    </row>
+    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C48" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="F48" s="13"/>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F49" s="13"/>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F50" s="13"/>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C51" s="24" t="s">
+        <v>602</v>
+      </c>
+      <c r="D51" s="10"/>
+      <c r="E51" s="41"/>
+      <c r="F51" s="13"/>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C52" s="15" t="s">
+        <v>490</v>
+      </c>
+      <c r="F52" s="13"/>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C53" s="15" t="s">
+        <v>537</v>
+      </c>
+      <c r="F53" s="13"/>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C54" s="15" t="s">
+        <v>536</v>
+      </c>
+      <c r="F54" s="13"/>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F55" s="13"/>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C56" s="24" t="s">
+        <v>524</v>
+      </c>
+      <c r="D56" s="10"/>
+      <c r="E56" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F56" s="13"/>
+    </row>
+    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C57" s="15" t="s">
+        <v>522</v>
+      </c>
+      <c r="F57" s="13"/>
+    </row>
+    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F58" s="13"/>
+    </row>
+    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C59" s="24" t="s">
+        <v>517</v>
+      </c>
+      <c r="D59" s="10"/>
+      <c r="E59" s="20" t="s">
+        <v>516</v>
+      </c>
+      <c r="F59" s="13"/>
+    </row>
+    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F60" s="13"/>
+    </row>
+    <row r="61" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E61" s="29" t="s">
+        <v>511</v>
+      </c>
+      <c r="F61" s="13"/>
+    </row>
+    <row r="62" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E62" s="29" t="s">
+        <v>510</v>
+      </c>
+      <c r="F62" s="13"/>
+    </row>
+    <row r="63" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E63" s="29" t="s">
+        <v>509</v>
+      </c>
+      <c r="F63" s="13"/>
+    </row>
+    <row r="64" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E64" s="29" t="s">
+        <v>508</v>
+      </c>
+      <c r="F64" s="13"/>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F65" s="13"/>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F66" s="13"/>
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F67" s="13"/>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F68" s="13"/>
+    </row>
+    <row r="69" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F69" s="13"/>
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F70" s="13"/>
+    </row>
+    <row r="71" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F71" s="13"/>
+    </row>
+    <row r="72" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F72" s="13"/>
+    </row>
+    <row r="73" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F73" s="13"/>
+    </row>
+    <row r="74" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F74" s="13"/>
+    </row>
+    <row r="75" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F75" s="13"/>
+    </row>
+    <row r="76" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F76" s="13"/>
+    </row>
+    <row r="77" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F77" s="13"/>
+    </row>
+    <row r="78" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F78" s="13"/>
+    </row>
+    <row r="79" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F79" s="13"/>
+    </row>
+    <row r="80" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F80" s="13"/>
+    </row>
+    <row r="81" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F81" s="13"/>
+    </row>
+    <row r="82" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F82" s="13"/>
+    </row>
+    <row r="83" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F83" s="13"/>
+    </row>
+    <row r="84" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F84" s="13"/>
+    </row>
+    <row r="85" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F85" s="13"/>
+    </row>
+    <row r="86" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F86" s="13"/>
+    </row>
+    <row r="87" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F87" s="13"/>
+    </row>
+    <row r="88" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F88" s="13"/>
+    </row>
+    <row r="89" spans="6:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F89" s="13"/>
+    </row>
+    <row r="90" spans="6:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F90" s="13"/>
+    </row>
+    <row r="91" spans="6:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F91" s="13"/>
+    </row>
+    <row r="92" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F92" s="13"/>
+    </row>
+    <row r="93" spans="6:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F93" s="13"/>
+    </row>
+    <row r="94" spans="6:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F94" s="13"/>
+    </row>
+    <row r="95" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F95" s="13"/>
+    </row>
+    <row r="96" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F96" s="13"/>
+    </row>
+    <row r="97" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F97" s="13"/>
+    </row>
+    <row r="98" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F98" s="13"/>
+    </row>
+    <row r="99" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F99" s="13"/>
+    </row>
+    <row r="100" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F100" s="13"/>
+    </row>
+    <row r="101" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F101" s="13"/>
+    </row>
+    <row r="102" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F102" s="13"/>
+    </row>
+    <row r="103" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F103" s="13"/>
+    </row>
+    <row r="104" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F104" s="13"/>
+    </row>
+    <row r="105" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F105" s="13"/>
+    </row>
+    <row r="106" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F106" s="13"/>
+    </row>
+    <row r="107" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F107" s="13"/>
+    </row>
+    <row r="108" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F108" s="13"/>
+    </row>
+    <row r="109" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F109" s="13"/>
+    </row>
+    <row r="110" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F110" s="13"/>
+    </row>
+    <row r="111" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F111" s="13"/>
+    </row>
+    <row r="112" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F112" s="13"/>
+    </row>
+    <row r="113" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F113" s="13"/>
+    </row>
+    <row r="114" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F114" s="13"/>
+    </row>
+    <row r="115" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F115" s="13"/>
+    </row>
+    <row r="116" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F116" s="13"/>
+    </row>
+    <row r="117" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F117" s="13"/>
+    </row>
+    <row r="118" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F118" s="13"/>
+    </row>
+    <row r="119" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F119" s="13"/>
+    </row>
+    <row r="120" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F120" s="13"/>
+    </row>
+    <row r="121" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F121" s="13"/>
+    </row>
+    <row r="122" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F122" s="13"/>
+    </row>
+    <row r="123" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F123" s="13"/>
+    </row>
+    <row r="124" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F124" s="13"/>
+    </row>
+    <row r="125" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F125" s="13"/>
+    </row>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update on all repo
</commit_message>
<xml_diff>
--- a/frontend/data/data_available.xlsx
+++ b/frontend/data/data_available.xlsx
@@ -8,20 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bianka\Documents\MSc-Internship\Observatory-of-the-Mountains\frontend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06A039C-D867-43CA-B369-EA05A02727EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{6CE4E154-741C-485D-BBC6-F74A05914EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{8809251D-B3C6-41F0-B60D-9556D90BF91D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{8809251D-B3C6-41F0-B60D-9556D90BF91D}"/>
   </bookViews>
   <sheets>
     <sheet name="per county" sheetId="1" r:id="rId1"/>
     <sheet name="per topic" sheetId="4" r:id="rId2"/>
     <sheet name="Q1_a" sheetId="5" r:id="rId3"/>
     <sheet name="Q1_b" sheetId="6" r:id="rId4"/>
+    <sheet name="Hárok1" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'per county'!$E$1:$E$195</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1638" uniqueCount="640">
   <si>
     <r>
       <t xml:space="preserve">gencat </t>
@@ -2231,12 +2233,120 @@
       <t xml:space="preserve"> Population</t>
     </r>
   </si>
+  <si>
+    <t>Domains</t>
+  </si>
+  <si>
+    <t>Idescat variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">average selling price of newly build building </t>
+  </si>
+  <si>
+    <t>average price of newly-built housing (€/m² built)</t>
+  </si>
+  <si>
+    <t>average price of second-hand housing (€/m² built)</t>
+  </si>
+  <si>
+    <t>import, filter Catalan counties, select variable average value, reshape data frame, add region column based on county, export</t>
+  </si>
+  <si>
+    <t>import, filter Catalan counties, sum Bc M PhD level of education into University education, calculate percentage of people attaining university education per county, reshape data frame, add region column based on county, export</t>
+  </si>
+  <si>
+    <t>import, filter Catalan counties, select variable GDP per capita (€), reshape data frame, add region column based on county, export</t>
+  </si>
+  <si>
+    <t>GDP per capita (€)</t>
+  </si>
+  <si>
+    <t>import, filter Catalan counties, select variable GDHI per capita (€), reshape data frame, add region column based on county, export</t>
+  </si>
+  <si>
+    <t>GDHI per capita (€)</t>
+  </si>
+  <si>
+    <t>import, filter Catalan counties, calculate per capita real investment budget in €, reshape data frame, add region column based on county, export</t>
+  </si>
+  <si>
+    <t>real investment budget per capita</t>
+  </si>
+  <si>
+    <t>percentage of population aged 15 and higher that attained university education</t>
+  </si>
+  <si>
+    <t>import, filter Catalan counties, select taxable base per contributor, reshape data frame, add region column based on county, export</t>
+  </si>
+  <si>
+    <t>income per capita (€)</t>
+  </si>
+  <si>
+    <t>urban estate tax per inhabitant  (€)</t>
+  </si>
+  <si>
+    <t>rural esta tax per capita (€)</t>
+  </si>
+  <si>
+    <t>import, filter Catalan counties, select tax base, calculate tax base per capita, reshape data frame, add region column based on county, export</t>
+  </si>
+  <si>
+    <t>import, filter Catalan counties, select total unemployed population, calculate percentage of population that is unemployed, reshape data frame, add region column based on county, export</t>
+  </si>
+  <si>
+    <t>percentage of population that in unemployed</t>
+  </si>
+  <si>
+    <t>Pre-processing steps</t>
+  </si>
+  <si>
+    <t>Final variable (per county)</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>domestic water consumption</t>
+  </si>
+  <si>
+    <t>industrial water consumption</t>
+  </si>
+  <si>
+    <t>import, filter Catalan counties, select domestic consumption, calculate amount of domestic water consumed per capita, reshape data frame, add region column based on county, export</t>
+  </si>
+  <si>
+    <t>domestic water consumption (m³)</t>
+  </si>
+  <si>
+    <t>import, filter Catalan counties, select industrial consumption, calculate amount of industrial water consumed per capita, reshape data frame, add region column based on county, export</t>
+  </si>
+  <si>
+    <t>industiral water consumption (m³)</t>
+  </si>
+  <si>
+    <t>import, filter Catalan counties, select total industrial waste, calculate the amount of industrial waste per area, reshape data frame, add region column based on county, export</t>
+  </si>
+  <si>
+    <t>industrial waste (kg)</t>
+  </si>
+  <si>
+    <t>import, filter Catalan counties, select total municipal waste, calculate the amount of municipal waste per capita, reshape data frame, add region column based on county, export</t>
+  </si>
+  <si>
+    <t>municipal waste (kg)</t>
+  </si>
+  <si>
+    <t>import, filter Catalan counties, calculate land conversion by computing the rate of change of each land cover class and summing the absolute value of the rate of change of all land cover classes per year, reshape data frame, add region column based on county, export</t>
+  </si>
+  <si>
+    <t>land conversion (%)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2284,6 +2394,46 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2395,7 +2545,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2464,6 +2614,39 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2488,40 +2671,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hypertextové prepojenie" xfId="1" builtinId="8"/>
@@ -2866,8 +3018,8 @@
   <dimension ref="A1:I195"/>
   <sheetViews>
     <sheetView zoomScale="88" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B131" sqref="A1:XFD1048576"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2885,11 +3037,11 @@
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
       <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
@@ -2915,13 +3067,13 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+    <row r="3" spans="1:9" s="48" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="48" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="30" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:9" s="47" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="47" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2971,8 +3123,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+    <row r="7" spans="1:9" s="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="47" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3013,8 +3165,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="30" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+    <row r="10" spans="1:9" s="47" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="47" t="s">
         <v>29</v>
       </c>
     </row>
@@ -3109,18 +3261,18 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+    <row r="17" spans="1:9" s="49" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="49" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30" t="s">
+    <row r="18" spans="1:9" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="47" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="50" t="s">
         <v>46</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -3146,7 +3298,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
+      <c r="A20" s="50"/>
       <c r="B20" s="2" t="s">
         <v>282</v>
       </c>
@@ -3170,7 +3322,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
+      <c r="A21" s="50"/>
       <c r="B21" s="2" t="s">
         <v>284</v>
       </c>
@@ -3194,7 +3346,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="1" t="s">
         <v>583</v>
       </c>
@@ -3215,7 +3367,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="33"/>
+      <c r="A23" s="50"/>
       <c r="B23" s="1" t="s">
         <v>287</v>
       </c>
@@ -3239,7 +3391,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="33"/>
+      <c r="A24" s="50"/>
       <c r="B24" s="1" t="s">
         <v>291</v>
       </c>
@@ -3263,7 +3415,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="33"/>
+      <c r="A25" s="50"/>
       <c r="B25" s="1" t="s">
         <v>294</v>
       </c>
@@ -3287,7 +3439,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="33"/>
+      <c r="A26" s="50"/>
       <c r="B26" s="1" t="s">
         <v>297</v>
       </c>
@@ -3311,7 +3463,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="33"/>
+      <c r="A27" s="50"/>
       <c r="B27" s="1" t="s">
         <v>300</v>
       </c>
@@ -3335,7 +3487,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="33" t="s">
+      <c r="A28" s="50" t="s">
         <v>49</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -3361,7 +3513,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="33"/>
+      <c r="A29" s="50"/>
       <c r="B29" s="1" t="s">
         <v>306</v>
       </c>
@@ -3385,7 +3537,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="33"/>
+      <c r="A30" s="50"/>
       <c r="B30" s="1" t="s">
         <v>309</v>
       </c>
@@ -3409,7 +3561,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="33"/>
+      <c r="A31" s="50"/>
       <c r="B31" s="1" t="s">
         <v>312</v>
       </c>
@@ -3433,7 +3585,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="33"/>
+      <c r="A32" s="50"/>
       <c r="B32" s="1" t="s">
         <v>314</v>
       </c>
@@ -3457,7 +3609,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="33"/>
+      <c r="A33" s="50"/>
       <c r="B33" s="1" t="s">
         <v>317</v>
       </c>
@@ -3481,7 +3633,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="33"/>
+      <c r="A34" s="50"/>
       <c r="B34" s="1" t="s">
         <v>320</v>
       </c>
@@ -3505,7 +3657,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="33"/>
+      <c r="A35" s="50"/>
       <c r="B35" s="1" t="s">
         <v>323</v>
       </c>
@@ -3529,7 +3681,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="33"/>
+      <c r="A36" s="50"/>
       <c r="B36" s="1" t="s">
         <v>327</v>
       </c>
@@ -3553,7 +3705,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="33" t="s">
+      <c r="A37" s="50" t="s">
         <v>346</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -3579,7 +3731,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="33"/>
+      <c r="A38" s="50"/>
       <c r="B38" s="1" t="s">
         <v>330</v>
       </c>
@@ -3603,7 +3755,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="33"/>
+      <c r="A39" s="50"/>
       <c r="B39" s="1" t="s">
         <v>335</v>
       </c>
@@ -3627,7 +3779,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
+      <c r="A40" s="50"/>
       <c r="B40" s="1" t="s">
         <v>338</v>
       </c>
@@ -3651,7 +3803,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="33"/>
+      <c r="A41" s="50"/>
       <c r="B41" s="1" t="s">
         <v>340</v>
       </c>
@@ -3675,7 +3827,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="33"/>
+      <c r="A42" s="50"/>
       <c r="B42" s="1" t="s">
         <v>343</v>
       </c>
@@ -3699,7 +3851,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="33" t="s">
+      <c r="A43" s="50" t="s">
         <v>48</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -3725,7 +3877,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="33"/>
+      <c r="A44" s="50"/>
       <c r="B44" s="1" t="s">
         <v>348</v>
       </c>
@@ -3749,7 +3901,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="33"/>
+      <c r="A45" s="50"/>
       <c r="B45" s="1" t="s">
         <v>349</v>
       </c>
@@ -3773,7 +3925,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="33"/>
+      <c r="A46" s="50"/>
       <c r="B46" s="1" t="s">
         <v>350</v>
       </c>
@@ -3797,7 +3949,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="33" t="s">
+      <c r="A47" s="50" t="s">
         <v>50</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -3823,7 +3975,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="33"/>
+      <c r="A48" s="50"/>
       <c r="B48" s="1" t="s">
         <v>360</v>
       </c>
@@ -3847,7 +3999,7 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="33" t="s">
+      <c r="A49" s="50" t="s">
         <v>51</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -3873,7 +4025,7 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="33"/>
+      <c r="A50" s="50"/>
       <c r="B50" s="1" t="s">
         <v>367</v>
       </c>
@@ -3897,7 +4049,7 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="33"/>
+      <c r="A51" s="50"/>
       <c r="B51" s="1" t="s">
         <v>368</v>
       </c>
@@ -3921,7 +4073,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="33"/>
+      <c r="A52" s="50"/>
       <c r="B52" s="1" t="s">
         <v>369</v>
       </c>
@@ -3945,7 +4097,7 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="33"/>
+      <c r="A53" s="50"/>
       <c r="B53" s="1" t="s">
         <v>370</v>
       </c>
@@ -3969,7 +4121,7 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="33"/>
+      <c r="A54" s="50"/>
       <c r="B54" s="1" t="s">
         <v>371</v>
       </c>
@@ -3993,7 +4145,7 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="33"/>
+      <c r="A55" s="50"/>
       <c r="B55" s="2" t="s">
         <v>383</v>
       </c>
@@ -4017,7 +4169,7 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="33"/>
+      <c r="A56" s="50"/>
       <c r="B56" s="2" t="s">
         <v>384</v>
       </c>
@@ -4041,7 +4193,7 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="33"/>
+      <c r="A57" s="50"/>
       <c r="B57" s="1" t="s">
         <v>80</v>
       </c>
@@ -4065,7 +4217,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="33"/>
+      <c r="A58" s="50"/>
       <c r="B58" s="1" t="s">
         <v>80</v>
       </c>
@@ -4089,7 +4241,7 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="33"/>
+      <c r="A59" s="50"/>
       <c r="B59" s="1" t="s">
         <v>80</v>
       </c>
@@ -4113,7 +4265,7 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="33"/>
+      <c r="A60" s="50"/>
       <c r="B60" s="1" t="s">
         <v>80</v>
       </c>
@@ -4137,7 +4289,7 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="33"/>
+      <c r="A61" s="50"/>
       <c r="B61" s="1" t="s">
         <v>396</v>
       </c>
@@ -4161,7 +4313,7 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="33"/>
+      <c r="A62" s="50"/>
       <c r="B62" s="2" t="s">
         <v>401</v>
       </c>
@@ -4185,7 +4337,7 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="33"/>
+      <c r="A63" s="50"/>
       <c r="B63" s="1" t="s">
         <v>402</v>
       </c>
@@ -4208,13 +4360,13 @@
         <v>404</v>
       </c>
     </row>
-    <row r="65" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="30" t="s">
+    <row r="65" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="47" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="33" t="s">
+      <c r="A66" s="50" t="s">
         <v>54</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -4240,7 +4392,7 @@
       </c>
     </row>
     <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="33"/>
+      <c r="A67" s="50"/>
       <c r="B67" s="1" t="s">
         <v>236</v>
       </c>
@@ -4264,7 +4416,7 @@
       </c>
     </row>
     <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="33"/>
+      <c r="A68" s="50"/>
       <c r="B68" s="1" t="s">
         <v>239</v>
       </c>
@@ -4288,7 +4440,7 @@
       </c>
     </row>
     <row r="69" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="33"/>
+      <c r="A69" s="50"/>
       <c r="B69" s="1" t="s">
         <v>507</v>
       </c>
@@ -4312,7 +4464,7 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="33"/>
+      <c r="A70" s="50"/>
       <c r="B70" s="1" t="s">
         <v>245</v>
       </c>
@@ -4336,7 +4488,7 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="33"/>
+      <c r="A71" s="50"/>
       <c r="B71" s="1" t="s">
         <v>248</v>
       </c>
@@ -4360,7 +4512,7 @@
       </c>
     </row>
     <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="33"/>
+      <c r="A72" s="50"/>
       <c r="B72" s="1" t="s">
         <v>250</v>
       </c>
@@ -4384,7 +4536,7 @@
       </c>
     </row>
     <row r="73" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="33" t="s">
+      <c r="A73" s="50" t="s">
         <v>55</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -4410,7 +4562,7 @@
       </c>
     </row>
     <row r="74" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="33"/>
+      <c r="A74" s="50"/>
       <c r="B74" s="1" t="s">
         <v>255</v>
       </c>
@@ -4434,7 +4586,7 @@
       </c>
     </row>
     <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="33"/>
+      <c r="A75" s="50"/>
       <c r="B75" s="1" t="s">
         <v>258</v>
       </c>
@@ -4458,7 +4610,7 @@
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="33"/>
+      <c r="A76" s="50"/>
       <c r="B76" s="1" t="s">
         <v>261</v>
       </c>
@@ -4482,7 +4634,7 @@
       </c>
     </row>
     <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="33"/>
+      <c r="A77" s="50"/>
       <c r="B77" s="1" t="s">
         <v>264</v>
       </c>
@@ -4506,7 +4658,7 @@
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="33"/>
+      <c r="A78" s="50"/>
       <c r="B78" s="1" t="s">
         <v>267</v>
       </c>
@@ -4530,7 +4682,7 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="33"/>
+      <c r="A79" s="50"/>
       <c r="B79" s="1" t="s">
         <v>270</v>
       </c>
@@ -4554,7 +4706,7 @@
       </c>
     </row>
     <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="33"/>
+      <c r="A80" s="50"/>
       <c r="B80" s="1" t="s">
         <v>273</v>
       </c>
@@ -4578,7 +4730,7 @@
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="33"/>
+      <c r="A81" s="50"/>
       <c r="B81" s="1" t="s">
         <v>276</v>
       </c>
@@ -4601,13 +4753,13 @@
         <v>278</v>
       </c>
     </row>
-    <row r="83" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="30" t="s">
+    <row r="83" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="47" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="33" t="s">
+      <c r="A84" s="50" t="s">
         <v>57</v>
       </c>
       <c r="B84" s="2" t="s">
@@ -4633,7 +4785,7 @@
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="33"/>
+      <c r="A85" s="50"/>
       <c r="B85" s="2" t="s">
         <v>196</v>
       </c>
@@ -4657,7 +4809,7 @@
       </c>
     </row>
     <row r="86" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A86" s="33"/>
+      <c r="A86" s="50"/>
       <c r="B86" s="2" t="s">
         <v>199</v>
       </c>
@@ -4681,7 +4833,7 @@
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="33"/>
+      <c r="A87" s="50"/>
       <c r="B87" s="2" t="s">
         <v>202</v>
       </c>
@@ -4705,7 +4857,7 @@
       </c>
     </row>
     <row r="88" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="33"/>
+      <c r="A88" s="50"/>
       <c r="B88" s="2" t="s">
         <v>205</v>
       </c>
@@ -4729,7 +4881,7 @@
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="33" t="s">
+      <c r="A89" s="50" t="s">
         <v>58</v>
       </c>
       <c r="B89" s="2" t="s">
@@ -4755,7 +4907,7 @@
       </c>
     </row>
     <row r="90" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="33"/>
+      <c r="A90" s="50"/>
       <c r="B90" s="2" t="s">
         <v>211</v>
       </c>
@@ -4779,7 +4931,7 @@
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="33" t="s">
+      <c r="A91" s="50" t="s">
         <v>59</v>
       </c>
       <c r="B91" s="2" t="s">
@@ -4802,7 +4954,7 @@
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="33"/>
+      <c r="A92" s="50"/>
       <c r="B92" s="2" t="s">
         <v>216</v>
       </c>
@@ -4826,7 +4978,7 @@
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="33"/>
+      <c r="A93" s="50"/>
       <c r="B93" s="1" t="s">
         <v>218</v>
       </c>
@@ -4850,7 +5002,7 @@
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="33"/>
+      <c r="A94" s="50"/>
       <c r="B94" s="1" t="s">
         <v>219</v>
       </c>
@@ -4874,7 +5026,7 @@
       </c>
     </row>
     <row r="95" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="33"/>
+      <c r="A95" s="50"/>
       <c r="B95" s="1" t="s">
         <v>223</v>
       </c>
@@ -4898,7 +5050,7 @@
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="33" t="s">
+      <c r="A96" s="50" t="s">
         <v>60</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -4924,7 +5076,7 @@
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="33"/>
+      <c r="A97" s="50"/>
       <c r="B97" s="1" t="s">
         <v>229</v>
       </c>
@@ -4947,13 +5099,13 @@
         <v>231</v>
       </c>
     </row>
-    <row r="99" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="30" t="s">
+    <row r="99" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="47" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A100" s="33" t="s">
+      <c r="A100" s="50" t="s">
         <v>105</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -4979,7 +5131,7 @@
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="33"/>
+      <c r="A101" s="50"/>
       <c r="B101" s="1" t="s">
         <v>72</v>
       </c>
@@ -5003,7 +5155,7 @@
       </c>
     </row>
     <row r="102" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A102" s="33"/>
+      <c r="A102" s="50"/>
       <c r="B102" s="1" t="s">
         <v>74</v>
       </c>
@@ -5027,7 +5179,7 @@
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="33"/>
+      <c r="A103" s="50"/>
       <c r="B103" s="1" t="s">
         <v>77</v>
       </c>
@@ -5051,7 +5203,7 @@
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="33"/>
+      <c r="A104" s="50"/>
       <c r="B104" s="1" t="s">
         <v>80</v>
       </c>
@@ -5075,7 +5227,7 @@
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="33"/>
+      <c r="A105" s="50"/>
       <c r="B105" s="1" t="s">
         <v>84</v>
       </c>
@@ -5099,7 +5251,7 @@
       </c>
     </row>
     <row r="106" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A106" s="33"/>
+      <c r="A106" s="50"/>
       <c r="B106" s="2" t="s">
         <v>87</v>
       </c>
@@ -5123,7 +5275,7 @@
       </c>
     </row>
     <row r="107" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A107" s="33"/>
+      <c r="A107" s="50"/>
       <c r="B107" s="1" t="s">
         <v>90</v>
       </c>
@@ -5147,7 +5299,7 @@
       </c>
     </row>
     <row r="108" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A108" s="33"/>
+      <c r="A108" s="50"/>
       <c r="B108" s="2" t="s">
         <v>93</v>
       </c>
@@ -5171,7 +5323,7 @@
       </c>
     </row>
     <row r="109" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A109" s="33"/>
+      <c r="A109" s="50"/>
       <c r="B109" s="1" t="s">
         <v>97</v>
       </c>
@@ -5195,7 +5347,7 @@
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="33" t="s">
+      <c r="A110" s="50" t="s">
         <v>106</v>
       </c>
       <c r="B110" s="1" t="s">
@@ -5221,7 +5373,7 @@
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" s="33"/>
+      <c r="A111" s="50"/>
       <c r="B111" s="1" t="s">
         <v>102</v>
       </c>
@@ -5245,7 +5397,7 @@
       </c>
     </row>
     <row r="112" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A112" s="33" t="s">
+      <c r="A112" s="50" t="s">
         <v>61</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -5271,7 +5423,7 @@
       </c>
     </row>
     <row r="113" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" s="33"/>
+      <c r="A113" s="50"/>
       <c r="B113" s="1" t="s">
         <v>110</v>
       </c>
@@ -5295,7 +5447,7 @@
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="33"/>
+      <c r="A114" s="50"/>
       <c r="B114" s="1" t="s">
         <v>112</v>
       </c>
@@ -5319,7 +5471,7 @@
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="33"/>
+      <c r="A115" s="50"/>
       <c r="B115" s="1" t="s">
         <v>115</v>
       </c>
@@ -5343,7 +5495,7 @@
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" s="33"/>
+      <c r="A116" s="50"/>
       <c r="B116" s="1" t="s">
         <v>118</v>
       </c>
@@ -5367,7 +5519,7 @@
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117" s="33"/>
+      <c r="A117" s="50"/>
       <c r="B117" s="1" t="s">
         <v>123</v>
       </c>
@@ -5391,7 +5543,7 @@
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A118" s="33"/>
+      <c r="A118" s="50"/>
       <c r="B118" s="1" t="s">
         <v>124</v>
       </c>
@@ -5415,7 +5567,7 @@
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119" s="33"/>
+      <c r="A119" s="50"/>
       <c r="B119" s="1" t="s">
         <v>127</v>
       </c>
@@ -5439,7 +5591,7 @@
       </c>
     </row>
     <row r="120" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="33" t="s">
+      <c r="A120" s="50" t="s">
         <v>62</v>
       </c>
       <c r="B120" s="1" t="s">
@@ -5465,7 +5617,7 @@
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A121" s="33"/>
+      <c r="A121" s="50"/>
       <c r="B121" s="1" t="s">
         <v>133</v>
       </c>
@@ -5489,7 +5641,7 @@
       </c>
     </row>
     <row r="122" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A122" s="33" t="s">
+      <c r="A122" s="50" t="s">
         <v>63</v>
       </c>
       <c r="B122" s="1" t="s">
@@ -5515,7 +5667,7 @@
       </c>
     </row>
     <row r="123" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A123" s="33"/>
+      <c r="A123" s="50"/>
       <c r="B123" s="1" t="s">
         <v>139</v>
       </c>
@@ -5539,7 +5691,7 @@
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" s="33"/>
+      <c r="A124" s="50"/>
       <c r="B124" s="1" t="s">
         <v>142</v>
       </c>
@@ -5563,7 +5715,7 @@
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A125" s="33"/>
+      <c r="A125" s="50"/>
       <c r="B125" s="1" t="s">
         <v>146</v>
       </c>
@@ -5586,13 +5738,13 @@
         <v>148</v>
       </c>
     </row>
-    <row r="127" spans="1:9" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="30" t="s">
+    <row r="127" spans="1:9" s="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="47" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A128" s="33" t="s">
+      <c r="A128" s="50" t="s">
         <v>65</v>
       </c>
       <c r="B128" s="1" t="s">
@@ -5618,7 +5770,7 @@
       </c>
     </row>
     <row r="129" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A129" s="33"/>
+      <c r="A129" s="50"/>
       <c r="B129" s="2" t="s">
         <v>152</v>
       </c>
@@ -5642,7 +5794,7 @@
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A130" s="33"/>
+      <c r="A130" s="50"/>
       <c r="B130" s="2" t="s">
         <v>154</v>
       </c>
@@ -5666,7 +5818,7 @@
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A131" s="33"/>
+      <c r="A131" s="50"/>
       <c r="B131" s="1" t="s">
         <v>158</v>
       </c>
@@ -5690,7 +5842,7 @@
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="33"/>
+      <c r="A132" s="50"/>
       <c r="B132" s="2" t="s">
         <v>161</v>
       </c>
@@ -5714,7 +5866,7 @@
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A133" s="33"/>
+      <c r="A133" s="50"/>
       <c r="B133" s="2" t="s">
         <v>164</v>
       </c>
@@ -5738,7 +5890,7 @@
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A134" s="33"/>
+      <c r="A134" s="50"/>
       <c r="B134" s="1" t="s">
         <v>166</v>
       </c>
@@ -5762,7 +5914,7 @@
       </c>
     </row>
     <row r="135" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A135" s="33"/>
+      <c r="A135" s="50"/>
       <c r="B135" s="2" t="s">
         <v>169</v>
       </c>
@@ -5786,7 +5938,7 @@
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A136" s="33"/>
+      <c r="A136" s="50"/>
       <c r="B136" s="1" t="s">
         <v>172</v>
       </c>
@@ -5810,7 +5962,7 @@
       </c>
     </row>
     <row r="137" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A137" s="33"/>
+      <c r="A137" s="50"/>
       <c r="B137" s="1" t="s">
         <v>175</v>
       </c>
@@ -5834,7 +5986,7 @@
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A138" s="33"/>
+      <c r="A138" s="50"/>
       <c r="B138" s="1" t="s">
         <v>178</v>
       </c>
@@ -5858,7 +6010,7 @@
       </c>
     </row>
     <row r="139" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A139" s="33"/>
+      <c r="A139" s="50"/>
       <c r="B139" s="1" t="s">
         <v>181</v>
       </c>
@@ -5882,7 +6034,7 @@
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A140" s="33" t="s">
+      <c r="A140" s="50" t="s">
         <v>66</v>
       </c>
       <c r="B140" s="1" t="s">
@@ -5894,7 +6046,7 @@
       <c r="I140" s="1"/>
     </row>
     <row r="141" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A141" s="33"/>
+      <c r="A141" s="50"/>
       <c r="B141" s="2" t="s">
         <v>185</v>
       </c>
@@ -5918,7 +6070,7 @@
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A142" s="33"/>
+      <c r="A142" s="50"/>
       <c r="B142" s="1" t="s">
         <v>188</v>
       </c>
@@ -5930,7 +6082,7 @@
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A143" s="33"/>
+      <c r="A143" s="50"/>
       <c r="B143" s="1" t="s">
         <v>190</v>
       </c>
@@ -5950,13 +6102,13 @@
         <v>192</v>
       </c>
     </row>
-    <row r="145" spans="1:9" s="35" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="35" t="s">
+    <row r="145" spans="1:9" s="52" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="52" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A146" s="33" t="s">
+      <c r="A146" s="50" t="s">
         <v>416</v>
       </c>
       <c r="B146" s="1" t="s">
@@ -5970,7 +6122,7 @@
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A147" s="33"/>
+      <c r="A147" s="50"/>
       <c r="B147" s="1" t="s">
         <v>408</v>
       </c>
@@ -5985,7 +6137,7 @@
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A148" s="33"/>
+      <c r="A148" s="50"/>
       <c r="B148" s="1" t="s">
         <v>409</v>
       </c>
@@ -5997,7 +6149,7 @@
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A149" s="33"/>
+      <c r="A149" s="50"/>
       <c r="B149" s="1" t="s">
         <v>158</v>
       </c>
@@ -6015,7 +6167,7 @@
       </c>
     </row>
     <row r="150" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="33"/>
+      <c r="A150" s="50"/>
       <c r="B150" s="1" t="s">
         <v>410</v>
       </c>
@@ -6030,7 +6182,7 @@
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A151" s="33"/>
+      <c r="A151" s="50"/>
       <c r="B151" s="1" t="s">
         <v>432</v>
       </c>
@@ -6042,7 +6194,7 @@
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A152" s="33"/>
+      <c r="A152" s="50"/>
       <c r="B152" s="1" t="s">
         <v>411</v>
       </c>
@@ -6057,7 +6209,7 @@
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A153" s="33"/>
+      <c r="A153" s="50"/>
       <c r="B153" s="1" t="s">
         <v>412</v>
       </c>
@@ -6069,7 +6221,7 @@
       </c>
     </row>
     <row r="154" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A154" s="33"/>
+      <c r="A154" s="50"/>
       <c r="B154" s="1" t="s">
         <v>413</v>
       </c>
@@ -6081,7 +6233,7 @@
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A155" s="33"/>
+      <c r="A155" s="50"/>
       <c r="B155" s="1" t="s">
         <v>414</v>
       </c>
@@ -6110,7 +6262,7 @@
       </c>
     </row>
     <row r="157" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="33" t="s">
+      <c r="A157" s="50" t="s">
         <v>420</v>
       </c>
       <c r="B157" s="1" t="s">
@@ -6127,7 +6279,7 @@
       </c>
     </row>
     <row r="158" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A158" s="33"/>
+      <c r="A158" s="50"/>
       <c r="B158" s="1" t="s">
         <v>441</v>
       </c>
@@ -6145,7 +6297,7 @@
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A159" s="33"/>
+      <c r="A159" s="50"/>
       <c r="B159" s="1" t="s">
         <v>444</v>
       </c>
@@ -6157,7 +6309,7 @@
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A160" s="33"/>
+      <c r="A160" s="50"/>
       <c r="B160" s="1" t="s">
         <v>446</v>
       </c>
@@ -6169,7 +6321,7 @@
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A161" s="33"/>
+      <c r="A161" s="50"/>
       <c r="B161" s="1" t="s">
         <v>448</v>
       </c>
@@ -6181,7 +6333,7 @@
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A162" s="33"/>
+      <c r="A162" s="50"/>
       <c r="B162" s="1" t="s">
         <v>450</v>
       </c>
@@ -6193,7 +6345,7 @@
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A163" s="33"/>
+      <c r="A163" s="50"/>
       <c r="B163" s="1" t="s">
         <v>452</v>
       </c>
@@ -6205,7 +6357,7 @@
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A164" s="33" t="s">
+      <c r="A164" s="50" t="s">
         <v>454</v>
       </c>
       <c r="B164" s="1" t="s">
@@ -6222,7 +6374,7 @@
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A165" s="33"/>
+      <c r="A165" s="50"/>
       <c r="B165" s="1" t="s">
         <v>457</v>
       </c>
@@ -6234,7 +6386,7 @@
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A166" s="33" t="s">
+      <c r="A166" s="50" t="s">
         <v>458</v>
       </c>
       <c r="B166" s="1" t="s">
@@ -6251,7 +6403,7 @@
       </c>
     </row>
     <row r="167" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A167" s="33"/>
+      <c r="A167" s="50"/>
       <c r="B167" s="1" t="s">
         <v>461</v>
       </c>
@@ -6266,7 +6418,7 @@
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A168" s="33" t="s">
+      <c r="A168" s="50" t="s">
         <v>463</v>
       </c>
       <c r="B168" s="1" t="s">
@@ -6283,7 +6435,7 @@
       </c>
     </row>
     <row r="169" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="33"/>
+      <c r="A169" s="50"/>
       <c r="B169" s="1" t="s">
         <v>465</v>
       </c>
@@ -6298,7 +6450,7 @@
       </c>
     </row>
     <row r="170" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="33" t="s">
+      <c r="A170" s="50" t="s">
         <v>467</v>
       </c>
       <c r="B170" s="1" t="s">
@@ -6319,7 +6471,7 @@
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A171" s="33"/>
+      <c r="A171" s="50"/>
       <c r="B171" s="1" t="s">
         <v>469</v>
       </c>
@@ -6332,14 +6484,14 @@
       <c r="H171" s="7"/>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A172" s="33"/>
+      <c r="A172" s="50"/>
       <c r="B172" s="1" t="s">
         <v>470</v>
       </c>
       <c r="H172" s="7"/>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A173" s="33"/>
+      <c r="A173" s="50"/>
       <c r="B173" s="1" t="s">
         <v>471</v>
       </c>
@@ -6352,14 +6504,14 @@
       <c r="H173" s="7"/>
     </row>
     <row r="174" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A174" s="33"/>
+      <c r="A174" s="50"/>
       <c r="B174" s="1" t="s">
         <v>472</v>
       </c>
       <c r="H174" s="7"/>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A175" s="33"/>
+      <c r="A175" s="50"/>
       <c r="B175" s="1" t="s">
         <v>473</v>
       </c>
@@ -6372,7 +6524,7 @@
       <c r="H175" s="7"/>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A176" s="33"/>
+      <c r="A176" s="50"/>
       <c r="B176" s="1" t="s">
         <v>474</v>
       </c>
@@ -6385,7 +6537,7 @@
       <c r="H176" s="7"/>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A177" s="33"/>
+      <c r="A177" s="50"/>
       <c r="B177" s="1" t="s">
         <v>475</v>
       </c>
@@ -6398,7 +6550,7 @@
       <c r="H177" s="7"/>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A178" s="33"/>
+      <c r="A178" s="50"/>
       <c r="B178" s="1" t="s">
         <v>476</v>
       </c>
@@ -6411,7 +6563,7 @@
       <c r="H178" s="7"/>
     </row>
     <row r="179" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="33" t="s">
+      <c r="A179" s="50" t="s">
         <v>478</v>
       </c>
       <c r="B179" s="1" t="s">
@@ -6429,7 +6581,7 @@
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A180" s="33"/>
+      <c r="A180" s="50"/>
       <c r="B180" s="1" t="s">
         <v>480</v>
       </c>
@@ -6442,7 +6594,7 @@
       <c r="H180" s="7"/>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A181" s="33"/>
+      <c r="A181" s="50"/>
       <c r="B181" s="1" t="s">
         <v>481</v>
       </c>
@@ -6455,7 +6607,7 @@
       <c r="H181" s="7"/>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A182" s="33"/>
+      <c r="A182" s="50"/>
       <c r="B182" s="1" t="s">
         <v>482</v>
       </c>
@@ -6468,7 +6620,7 @@
       <c r="H182" s="7"/>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A183" s="33"/>
+      <c r="A183" s="50"/>
       <c r="B183" s="1" t="s">
         <v>483</v>
       </c>
@@ -6481,7 +6633,7 @@
       <c r="H183" s="7"/>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A184" s="33"/>
+      <c r="A184" s="50"/>
       <c r="B184" s="1" t="s">
         <v>484</v>
       </c>
@@ -6494,7 +6646,7 @@
       <c r="H184" s="7"/>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A185" s="33"/>
+      <c r="A185" s="50"/>
       <c r="B185" s="1" t="s">
         <v>485</v>
       </c>
@@ -6507,7 +6659,7 @@
       <c r="H185" s="7"/>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A186" s="33"/>
+      <c r="A186" s="50"/>
       <c r="B186" s="1" t="s">
         <v>486</v>
       </c>
@@ -6520,7 +6672,7 @@
       <c r="H186" s="7"/>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A187" s="33"/>
+      <c r="A187" s="50"/>
       <c r="B187" s="1" t="s">
         <v>487</v>
       </c>
@@ -6533,7 +6685,7 @@
       <c r="H187" s="7"/>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A188" s="33"/>
+      <c r="A188" s="50"/>
       <c r="B188" s="1" t="s">
         <v>488</v>
       </c>
@@ -6546,7 +6698,7 @@
       <c r="H188" s="7"/>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A189" s="33"/>
+      <c r="A189" s="50"/>
       <c r="B189" s="2" t="s">
         <v>489</v>
       </c>
@@ -6559,7 +6711,7 @@
       <c r="H189" s="7"/>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A190" s="33"/>
+      <c r="A190" s="50"/>
       <c r="B190" s="1" t="s">
         <v>490</v>
       </c>
@@ -6592,7 +6744,7 @@
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A192" s="33" t="s">
+      <c r="A192" s="50" t="s">
         <v>495</v>
       </c>
       <c r="B192" s="1" t="s">
@@ -6612,7 +6764,7 @@
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A193" s="33"/>
+      <c r="A193" s="50"/>
       <c r="B193" s="1" t="s">
         <v>498</v>
       </c>
@@ -6621,7 +6773,7 @@
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A194" s="33" t="s">
+      <c r="A194" s="50" t="s">
         <v>106</v>
       </c>
       <c r="B194" s="1" t="s">
@@ -6638,7 +6790,7 @@
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A195" s="33"/>
+      <c r="A195" s="50"/>
       <c r="B195" s="1" t="s">
         <v>502</v>
       </c>
@@ -6774,17 +6926,17 @@
         <v>558</v>
       </c>
       <c r="G2" s="9"/>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="54" t="s">
         <v>557</v>
       </c>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
       <c r="M2" s="27" t="s">
         <v>578</v>
       </c>
       <c r="N2" s="1"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
@@ -8012,8 +8164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC2F606-BCE5-41DE-997B-370E48010E8A}">
   <dimension ref="A1:H129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="H123" sqref="H123"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8030,11 +8182,11 @@
       <c r="A1" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
       <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
@@ -8046,29 +8198,29 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="30" t="s">
         <v>421</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>423</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="30" t="s">
         <v>422</v>
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+    <row r="3" spans="1:8" s="49" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="49" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:8" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="47" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="50" t="s">
         <v>46</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -8094,7 +8246,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
+      <c r="A6" s="50"/>
       <c r="B6" s="2" t="s">
         <v>282</v>
       </c>
@@ -8118,7 +8270,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
+      <c r="A7" s="50"/>
       <c r="B7" s="2" t="s">
         <v>284</v>
       </c>
@@ -8142,7 +8294,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="33"/>
+      <c r="A8" s="50"/>
       <c r="B8" s="1" t="s">
         <v>592</v>
       </c>
@@ -8163,7 +8315,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
+      <c r="A9" s="50"/>
       <c r="B9" s="1" t="s">
         <v>287</v>
       </c>
@@ -8187,7 +8339,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
+      <c r="A10" s="50"/>
       <c r="B10" s="1" t="s">
         <v>291</v>
       </c>
@@ -8211,7 +8363,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
+      <c r="A11" s="50"/>
       <c r="B11" s="1" t="s">
         <v>294</v>
       </c>
@@ -8235,7 +8387,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="33"/>
+      <c r="A12" s="50"/>
       <c r="B12" s="1" t="s">
         <v>297</v>
       </c>
@@ -8259,7 +8411,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="1" t="s">
         <v>300</v>
       </c>
@@ -8283,7 +8435,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="50" t="s">
         <v>49</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -8309,7 +8461,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="33"/>
+      <c r="A15" s="50"/>
       <c r="B15" s="1" t="s">
         <v>306</v>
       </c>
@@ -8333,7 +8485,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="1" t="s">
         <v>309</v>
       </c>
@@ -8357,7 +8509,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="1" t="s">
         <v>312</v>
       </c>
@@ -8381,7 +8533,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
+      <c r="A18" s="50"/>
       <c r="B18" s="1" t="s">
         <v>314</v>
       </c>
@@ -8405,7 +8557,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
+      <c r="A19" s="50"/>
       <c r="B19" s="1" t="s">
         <v>317</v>
       </c>
@@ -8429,7 +8581,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
+      <c r="A20" s="50"/>
       <c r="B20" s="1" t="s">
         <v>320</v>
       </c>
@@ -8453,7 +8605,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
+      <c r="A21" s="50"/>
       <c r="B21" s="1" t="s">
         <v>323</v>
       </c>
@@ -8477,7 +8629,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="1" t="s">
         <v>327</v>
       </c>
@@ -8501,7 +8653,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="50" t="s">
         <v>346</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -8527,7 +8679,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="33"/>
+      <c r="A24" s="50"/>
       <c r="B24" s="1" t="s">
         <v>330</v>
       </c>
@@ -8551,8 +8703,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="33"/>
-      <c r="B25" s="43" t="s">
+      <c r="A25" s="50"/>
+      <c r="B25" s="1" t="s">
         <v>335</v>
       </c>
       <c r="C25" s="1">
@@ -8575,8 +8727,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="33"/>
-      <c r="B26" s="43" t="s">
+      <c r="A26" s="50"/>
+      <c r="B26" s="1" t="s">
         <v>338</v>
       </c>
       <c r="C26" s="1">
@@ -8599,7 +8751,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="33"/>
+      <c r="A27" s="50"/>
       <c r="B27" s="1" t="s">
         <v>340</v>
       </c>
@@ -8623,7 +8775,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="33"/>
+      <c r="A28" s="50"/>
       <c r="B28" s="2" t="s">
         <v>343</v>
       </c>
@@ -8647,7 +8799,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="33" t="s">
+      <c r="A29" s="50" t="s">
         <v>48</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -8673,7 +8825,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="33"/>
+      <c r="A30" s="50"/>
       <c r="B30" s="1" t="s">
         <v>348</v>
       </c>
@@ -8697,7 +8849,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="33"/>
+      <c r="A31" s="50"/>
       <c r="B31" s="1" t="s">
         <v>349</v>
       </c>
@@ -8721,7 +8873,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="33"/>
+      <c r="A32" s="50"/>
       <c r="B32" s="1" t="s">
         <v>350</v>
       </c>
@@ -8745,7 +8897,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="50" t="s">
         <v>50</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -8771,7 +8923,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="33"/>
+      <c r="A34" s="50"/>
       <c r="B34" s="1" t="s">
         <v>360</v>
       </c>
@@ -8795,7 +8947,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="33" t="s">
+      <c r="A35" s="50" t="s">
         <v>51</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -8821,7 +8973,7 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="33"/>
+      <c r="A36" s="50"/>
       <c r="B36" s="1" t="s">
         <v>367</v>
       </c>
@@ -8845,7 +8997,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
+      <c r="A37" s="50"/>
       <c r="B37" s="1" t="s">
         <v>368</v>
       </c>
@@ -8869,7 +9021,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="33"/>
+      <c r="A38" s="50"/>
       <c r="B38" s="1" t="s">
         <v>369</v>
       </c>
@@ -8893,7 +9045,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="33"/>
+      <c r="A39" s="50"/>
       <c r="B39" s="1" t="s">
         <v>370</v>
       </c>
@@ -8917,7 +9069,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
+      <c r="A40" s="50"/>
       <c r="B40" s="1" t="s">
         <v>371</v>
       </c>
@@ -8941,7 +9093,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="33"/>
+      <c r="A41" s="50"/>
       <c r="B41" s="2" t="s">
         <v>383</v>
       </c>
@@ -8965,7 +9117,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="33"/>
+      <c r="A42" s="50"/>
       <c r="B42" s="2" t="s">
         <v>384</v>
       </c>
@@ -8989,7 +9141,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="33"/>
+      <c r="A43" s="50"/>
       <c r="B43" s="1" t="s">
         <v>80</v>
       </c>
@@ -9005,7 +9157,7 @@
       <c r="F43" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G43" s="43" t="s">
+      <c r="G43" s="1" t="s">
         <v>388</v>
       </c>
       <c r="H43" t="s">
@@ -9013,7 +9165,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="33"/>
+      <c r="A44" s="50"/>
       <c r="B44" s="1" t="s">
         <v>80</v>
       </c>
@@ -9037,7 +9189,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="33"/>
+      <c r="A45" s="50"/>
       <c r="B45" s="1" t="s">
         <v>80</v>
       </c>
@@ -9061,7 +9213,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="33"/>
+      <c r="A46" s="50"/>
       <c r="B46" s="1" t="s">
         <v>80</v>
       </c>
@@ -9085,7 +9237,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="33"/>
+      <c r="A47" s="50"/>
       <c r="B47" s="1" t="s">
         <v>396</v>
       </c>
@@ -9109,7 +9261,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="33"/>
+      <c r="A48" s="50"/>
       <c r="B48" s="2" t="s">
         <v>401</v>
       </c>
@@ -9133,7 +9285,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="33"/>
+      <c r="A49" s="50"/>
       <c r="B49" s="1" t="s">
         <v>402</v>
       </c>
@@ -9156,13 +9308,13 @@
         <v>404</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="30" t="s">
+    <row r="51" spans="1:8" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="47" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="33" t="s">
+      <c r="A52" s="50" t="s">
         <v>54</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -9188,7 +9340,7 @@
       </c>
     </row>
     <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="33"/>
+      <c r="A53" s="50"/>
       <c r="B53" s="1" t="s">
         <v>236</v>
       </c>
@@ -9212,7 +9364,7 @@
       </c>
     </row>
     <row r="54" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="33"/>
+      <c r="A54" s="50"/>
       <c r="B54" s="1" t="s">
         <v>239</v>
       </c>
@@ -9236,7 +9388,7 @@
       </c>
     </row>
     <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A55" s="33"/>
+      <c r="A55" s="50"/>
       <c r="B55" s="1" t="s">
         <v>507</v>
       </c>
@@ -9260,7 +9412,7 @@
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="33"/>
+      <c r="A56" s="50"/>
       <c r="B56" s="1" t="s">
         <v>245</v>
       </c>
@@ -9284,7 +9436,7 @@
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="33"/>
+      <c r="A57" s="50"/>
       <c r="B57" s="2" t="s">
         <v>248</v>
       </c>
@@ -9308,7 +9460,7 @@
       </c>
     </row>
     <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="33"/>
+      <c r="A58" s="50"/>
       <c r="B58" s="2" t="s">
         <v>250</v>
       </c>
@@ -9332,7 +9484,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="33" t="s">
+      <c r="A59" s="50" t="s">
         <v>55</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -9358,7 +9510,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="33"/>
+      <c r="A60" s="50"/>
       <c r="B60" s="1" t="s">
         <v>255</v>
       </c>
@@ -9382,7 +9534,7 @@
       </c>
     </row>
     <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="33"/>
+      <c r="A61" s="50"/>
       <c r="B61" s="1" t="s">
         <v>258</v>
       </c>
@@ -9406,7 +9558,7 @@
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="33"/>
+      <c r="A62" s="50"/>
       <c r="B62" s="1" t="s">
         <v>261</v>
       </c>
@@ -9430,7 +9582,7 @@
       </c>
     </row>
     <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="33"/>
+      <c r="A63" s="50"/>
       <c r="B63" s="1" t="s">
         <v>264</v>
       </c>
@@ -9454,7 +9606,7 @@
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="33"/>
+      <c r="A64" s="50"/>
       <c r="B64" s="1" t="s">
         <v>267</v>
       </c>
@@ -9478,7 +9630,7 @@
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="33"/>
+      <c r="A65" s="50"/>
       <c r="B65" s="1" t="s">
         <v>270</v>
       </c>
@@ -9502,7 +9654,7 @@
       </c>
     </row>
     <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="33"/>
+      <c r="A66" s="50"/>
       <c r="B66" s="1" t="s">
         <v>273</v>
       </c>
@@ -9526,7 +9678,7 @@
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="33"/>
+      <c r="A67" s="50"/>
       <c r="B67" s="1" t="s">
         <v>276</v>
       </c>
@@ -9549,13 +9701,13 @@
         <v>278</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="30" t="s">
+    <row r="69" spans="1:8" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="47" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="33" t="s">
+      <c r="A70" s="50" t="s">
         <v>57</v>
       </c>
       <c r="B70" s="2" t="s">
@@ -9581,7 +9733,7 @@
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="33"/>
+      <c r="A71" s="50"/>
       <c r="B71" s="2" t="s">
         <v>196</v>
       </c>
@@ -9605,7 +9757,7 @@
       </c>
     </row>
     <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A72" s="33"/>
+      <c r="A72" s="50"/>
       <c r="B72" s="2" t="s">
         <v>199</v>
       </c>
@@ -9629,7 +9781,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="33"/>
+      <c r="A73" s="50"/>
       <c r="B73" s="2" t="s">
         <v>202</v>
       </c>
@@ -9648,12 +9800,12 @@
       <c r="G73" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="H73" t="s">
+      <c r="H73" s="8" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="33"/>
+      <c r="A74" s="50"/>
       <c r="B74" s="2" t="s">
         <v>205</v>
       </c>
@@ -9677,7 +9829,7 @@
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="33" t="s">
+      <c r="A75" s="50" t="s">
         <v>58</v>
       </c>
       <c r="B75" s="2" t="s">
@@ -9703,7 +9855,7 @@
       </c>
     </row>
     <row r="76" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="33"/>
+      <c r="A76" s="50"/>
       <c r="B76" s="2" t="s">
         <v>211</v>
       </c>
@@ -9727,7 +9879,7 @@
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="33" t="s">
+      <c r="A77" s="50" t="s">
         <v>589</v>
       </c>
       <c r="B77" s="2" t="s">
@@ -9750,7 +9902,7 @@
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="33"/>
+      <c r="A78" s="50"/>
       <c r="B78" s="2" t="s">
         <v>216</v>
       </c>
@@ -9774,7 +9926,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="33"/>
+      <c r="A79" s="50"/>
       <c r="B79" s="2" t="s">
         <v>218</v>
       </c>
@@ -9798,7 +9950,7 @@
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="33"/>
+      <c r="A80" s="50"/>
       <c r="B80" s="2" t="s">
         <v>219</v>
       </c>
@@ -9822,7 +9974,7 @@
       </c>
     </row>
     <row r="81" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="33"/>
+      <c r="A81" s="50"/>
       <c r="B81" s="2" t="s">
         <v>223</v>
       </c>
@@ -9846,7 +9998,7 @@
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="33" t="s">
+      <c r="A82" s="50" t="s">
         <v>60</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -9872,7 +10024,7 @@
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="33"/>
+      <c r="A83" s="50"/>
       <c r="B83" s="1" t="s">
         <v>229</v>
       </c>
@@ -9895,13 +10047,13 @@
         <v>231</v>
       </c>
     </row>
-    <row r="85" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="30" t="s">
+    <row r="85" spans="1:8" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="47" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A86" s="33" t="s">
+      <c r="A86" s="50" t="s">
         <v>105</v>
       </c>
       <c r="B86" s="1" t="s">
@@ -9927,7 +10079,7 @@
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="33"/>
+      <c r="A87" s="50"/>
       <c r="B87" s="1" t="s">
         <v>72</v>
       </c>
@@ -9951,7 +10103,7 @@
       </c>
     </row>
     <row r="88" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A88" s="33"/>
+      <c r="A88" s="50"/>
       <c r="B88" s="1" t="s">
         <v>74</v>
       </c>
@@ -9975,7 +10127,7 @@
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="33"/>
+      <c r="A89" s="50"/>
       <c r="B89" s="2" t="s">
         <v>77</v>
       </c>
@@ -9999,7 +10151,7 @@
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="33"/>
+      <c r="A90" s="50"/>
       <c r="B90" s="1" t="s">
         <v>80</v>
       </c>
@@ -10023,7 +10175,7 @@
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="33"/>
+      <c r="A91" s="50"/>
       <c r="B91" s="1" t="s">
         <v>84</v>
       </c>
@@ -10047,8 +10199,8 @@
       </c>
     </row>
     <row r="92" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A92" s="33"/>
-      <c r="B92" s="43" t="s">
+      <c r="A92" s="50"/>
+      <c r="B92" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C92" s="1">
@@ -10071,7 +10223,7 @@
       </c>
     </row>
     <row r="93" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A93" s="33"/>
+      <c r="A93" s="50"/>
       <c r="B93" s="1" t="s">
         <v>90</v>
       </c>
@@ -10095,7 +10247,7 @@
       </c>
     </row>
     <row r="94" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A94" s="33"/>
+      <c r="A94" s="50"/>
       <c r="B94" s="2" t="s">
         <v>93</v>
       </c>
@@ -10119,7 +10271,7 @@
       </c>
     </row>
     <row r="95" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A95" s="33"/>
+      <c r="A95" s="50"/>
       <c r="B95" s="1" t="s">
         <v>97</v>
       </c>
@@ -10143,7 +10295,7 @@
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="33" t="s">
+      <c r="A96" s="50" t="s">
         <v>106</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -10169,7 +10321,7 @@
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="33"/>
+      <c r="A97" s="50"/>
       <c r="B97" s="1" t="s">
         <v>102</v>
       </c>
@@ -10193,7 +10345,7 @@
       </c>
     </row>
     <row r="98" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="33" t="s">
+      <c r="A98" s="50" t="s">
         <v>61</v>
       </c>
       <c r="B98" s="1" t="s">
@@ -10219,7 +10371,7 @@
       </c>
     </row>
     <row r="99" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A99" s="33"/>
+      <c r="A99" s="50"/>
       <c r="B99" s="1" t="s">
         <v>110</v>
       </c>
@@ -10243,7 +10395,7 @@
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="33"/>
+      <c r="A100" s="50"/>
       <c r="B100" s="1" t="s">
         <v>112</v>
       </c>
@@ -10267,7 +10419,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="33"/>
+      <c r="A101" s="50"/>
       <c r="B101" s="1" t="s">
         <v>115</v>
       </c>
@@ -10291,7 +10443,7 @@
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="33"/>
+      <c r="A102" s="50"/>
       <c r="B102" s="1" t="s">
         <v>118</v>
       </c>
@@ -10315,7 +10467,7 @@
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="33"/>
+      <c r="A103" s="50"/>
       <c r="B103" s="1" t="s">
         <v>123</v>
       </c>
@@ -10339,7 +10491,7 @@
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="33"/>
+      <c r="A104" s="50"/>
       <c r="B104" s="1" t="s">
         <v>124</v>
       </c>
@@ -10363,7 +10515,7 @@
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="33"/>
+      <c r="A105" s="50"/>
       <c r="B105" s="1" t="s">
         <v>127</v>
       </c>
@@ -10387,7 +10539,7 @@
       </c>
     </row>
     <row r="106" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A106" s="33" t="s">
+      <c r="A106" s="50" t="s">
         <v>62</v>
       </c>
       <c r="B106" s="1" t="s">
@@ -10413,7 +10565,7 @@
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="33"/>
+      <c r="A107" s="50"/>
       <c r="B107" s="1" t="s">
         <v>133</v>
       </c>
@@ -10437,7 +10589,7 @@
       </c>
     </row>
     <row r="108" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="33" t="s">
+      <c r="A108" s="50" t="s">
         <v>63</v>
       </c>
       <c r="B108" s="1" t="s">
@@ -10463,7 +10615,7 @@
       </c>
     </row>
     <row r="109" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A109" s="33"/>
+      <c r="A109" s="50"/>
       <c r="B109" s="1" t="s">
         <v>139</v>
       </c>
@@ -10487,7 +10639,7 @@
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="33"/>
+      <c r="A110" s="50"/>
       <c r="B110" s="1" t="s">
         <v>142</v>
       </c>
@@ -10511,7 +10663,7 @@
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="33"/>
+      <c r="A111" s="50"/>
       <c r="B111" s="1" t="s">
         <v>146</v>
       </c>
@@ -10534,13 +10686,13 @@
         <v>148</v>
       </c>
     </row>
-    <row r="113" spans="1:8" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="30" t="s">
+    <row r="113" spans="1:8" s="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="47" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A114" s="33" t="s">
+      <c r="A114" s="50" t="s">
         <v>65</v>
       </c>
       <c r="B114" s="2" t="s">
@@ -10566,7 +10718,7 @@
       </c>
     </row>
     <row r="115" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A115" s="33"/>
+      <c r="A115" s="50"/>
       <c r="B115" s="2" t="s">
         <v>152</v>
       </c>
@@ -10590,7 +10742,7 @@
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A116" s="33"/>
+      <c r="A116" s="50"/>
       <c r="B116" s="2" t="s">
         <v>154</v>
       </c>
@@ -10614,7 +10766,7 @@
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A117" s="33"/>
+      <c r="A117" s="50"/>
       <c r="B117" s="2" t="s">
         <v>158</v>
       </c>
@@ -10638,7 +10790,7 @@
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A118" s="33"/>
+      <c r="A118" s="50"/>
       <c r="B118" s="2" t="s">
         <v>161</v>
       </c>
@@ -10662,7 +10814,7 @@
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A119" s="33"/>
+      <c r="A119" s="50"/>
       <c r="B119" s="2" t="s">
         <v>164</v>
       </c>
@@ -10686,7 +10838,7 @@
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" s="33"/>
+      <c r="A120" s="50"/>
       <c r="B120" s="2" t="s">
         <v>166</v>
       </c>
@@ -10710,7 +10862,7 @@
       </c>
     </row>
     <row r="121" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A121" s="33"/>
+      <c r="A121" s="50"/>
       <c r="B121" s="2" t="s">
         <v>169</v>
       </c>
@@ -10734,7 +10886,7 @@
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A122" s="33"/>
+      <c r="A122" s="50"/>
       <c r="B122" s="1" t="s">
         <v>172</v>
       </c>
@@ -10758,7 +10910,7 @@
       </c>
     </row>
     <row r="123" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A123" s="33"/>
+      <c r="A123" s="50"/>
       <c r="B123" s="2" t="s">
         <v>175</v>
       </c>
@@ -10782,7 +10934,7 @@
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A124" s="33"/>
+      <c r="A124" s="50"/>
       <c r="B124" s="1" t="s">
         <v>178</v>
       </c>
@@ -10806,7 +10958,7 @@
       </c>
     </row>
     <row r="125" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A125" s="33"/>
+      <c r="A125" s="50"/>
       <c r="B125" s="2" t="s">
         <v>181</v>
       </c>
@@ -10830,7 +10982,7 @@
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A126" s="33" t="s">
+      <c r="A126" s="50" t="s">
         <v>66</v>
       </c>
       <c r="B126" s="1" t="s">
@@ -10842,7 +10994,7 @@
       <c r="H126" s="1"/>
     </row>
     <row r="127" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A127" s="33"/>
+      <c r="A127" s="50"/>
       <c r="B127" s="2" t="s">
         <v>185</v>
       </c>
@@ -10866,7 +11018,7 @@
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A128" s="33"/>
+      <c r="A128" s="50"/>
       <c r="B128" s="1" t="s">
         <v>188</v>
       </c>
@@ -10878,7 +11030,7 @@
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A129" s="33"/>
+      <c r="A129" s="50"/>
       <c r="B129" s="1" t="s">
         <v>190</v>
       </c>
@@ -10900,11 +11052,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A98:A105"/>
-    <mergeCell ref="A106:A107"/>
-    <mergeCell ref="A108:A111"/>
-    <mergeCell ref="A113:XFD113"/>
-    <mergeCell ref="A114:A125"/>
     <mergeCell ref="A126:A129"/>
     <mergeCell ref="A75:A76"/>
     <mergeCell ref="A77:A81"/>
@@ -10912,11 +11059,13 @@
     <mergeCell ref="A85:XFD85"/>
     <mergeCell ref="A86:A95"/>
     <mergeCell ref="A96:A97"/>
-    <mergeCell ref="A35:A49"/>
-    <mergeCell ref="A51:XFD51"/>
-    <mergeCell ref="A52:A58"/>
-    <mergeCell ref="A59:A67"/>
-    <mergeCell ref="A69:XFD69"/>
+    <mergeCell ref="A98:A105"/>
+    <mergeCell ref="A106:A107"/>
+    <mergeCell ref="A108:A111"/>
+    <mergeCell ref="A113:XFD113"/>
+    <mergeCell ref="A114:A125"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="A3:XFD3"/>
     <mergeCell ref="A70:A74"/>
     <mergeCell ref="A4:XFD4"/>
     <mergeCell ref="A5:A13"/>
@@ -10924,8 +11073,11 @@
     <mergeCell ref="A23:A28"/>
     <mergeCell ref="A29:A32"/>
     <mergeCell ref="A33:A34"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="A3:XFD3"/>
+    <mergeCell ref="A35:A49"/>
+    <mergeCell ref="A51:XFD51"/>
+    <mergeCell ref="A52:A58"/>
+    <mergeCell ref="A59:A67"/>
+    <mergeCell ref="A69:XFD69"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H47" r:id="rId1" xr:uid="{2424F334-F3B8-40C2-B211-E0F49AA3181B}"/>
@@ -10961,9 +11113,10 @@
     <hyperlink ref="H77" r:id="rId31" xr:uid="{5E2A9DED-F51D-4B03-AAD8-745D10688DF3}"/>
     <hyperlink ref="H96" r:id="rId32" xr:uid="{A4C18DB2-9A8E-4469-8C64-8EEA714DB554}"/>
     <hyperlink ref="H57" r:id="rId33" xr:uid="{19A721BE-E8C3-4938-A2F4-9CE4F53A341A}"/>
+    <hyperlink ref="H73" r:id="rId34" xr:uid="{4BD04514-CA9B-4B93-8F3D-3D1959B7445F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId34"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId35"/>
 </worksheet>
 </file>
 
@@ -10971,15 +11124,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C15B307-9B65-4164-8063-9F476182200F}">
   <dimension ref="B2:O180"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" customWidth="1"/>
-    <col min="3" max="3" width="49.7109375" style="15" customWidth="1"/>
+    <col min="3" max="3" width="52.42578125" style="15" customWidth="1"/>
     <col min="4" max="4" width="4.5703125" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" style="22" customWidth="1"/>
     <col min="6" max="6" width="5.140625" customWidth="1"/>
@@ -10996,17 +11149,17 @@
         <v>558</v>
       </c>
       <c r="D2" s="9"/>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="54" t="s">
         <v>557</v>
       </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="I2" s="27" t="s">
         <v>578</v>
       </c>
       <c r="J2" s="1"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E3" s="18" t="s">
@@ -11018,7 +11171,7 @@
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="31" t="s">
         <v>603</v>
       </c>
       <c r="F4" s="13"/>
@@ -11110,9 +11263,6 @@
       <c r="O12" s="14"/>
     </row>
     <row r="13" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="15" t="s">
-        <v>123</v>
-      </c>
       <c r="F13" s="13"/>
       <c r="I13" s="17" t="s">
         <v>175</v>
@@ -11121,11 +11271,8 @@
       <c r="O13" s="14"/>
     </row>
     <row r="14" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="15" t="s">
-        <v>124</v>
-      </c>
       <c r="F14" s="13"/>
-      <c r="G14" s="46" t="s">
+      <c r="G14" s="1" t="s">
         <v>590</v>
       </c>
       <c r="H14" s="15"/>
@@ -11137,7 +11284,6 @@
     </row>
     <row r="15" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F15" s="13"/>
-      <c r="K15" s="45"/>
       <c r="O15" s="14"/>
     </row>
     <row r="16" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11149,114 +11295,97 @@
         <v>346</v>
       </c>
       <c r="F16" s="13"/>
-      <c r="G16" s="47"/>
+      <c r="G16" s="34"/>
       <c r="H16" s="15"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="45"/>
+      <c r="J16" s="38"/>
       <c r="L16" s="14"/>
       <c r="O16" s="14"/>
     </row>
     <row r="17" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="15" t="s">
-        <v>547</v>
+      <c r="C17" s="33" t="s">
+        <v>593</v>
       </c>
       <c r="F17" s="13"/>
-      <c r="G17" s="47"/>
+      <c r="G17" s="34"/>
       <c r="H17" s="15"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="45"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="38"/>
       <c r="L17" s="14"/>
       <c r="O17" s="14"/>
     </row>
     <row r="18" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="15" t="s">
-        <v>546</v>
-      </c>
       <c r="F18" s="13"/>
-      <c r="G18" s="45"/>
+      <c r="G18"/>
       <c r="H18" s="15"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="45"/>
+      <c r="J18" s="38"/>
       <c r="L18" s="14"/>
       <c r="O18" s="14"/>
     </row>
     <row r="19" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="15" t="s">
-        <v>545</v>
-      </c>
       <c r="E19" s="20" t="s">
         <v>512</v>
       </c>
       <c r="F19" s="13"/>
-      <c r="G19" s="49" t="s">
+      <c r="G19" s="36" t="s">
         <v>533</v>
       </c>
       <c r="H19" s="16"/>
       <c r="I19" s="16"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="45"/>
+      <c r="J19" s="38"/>
       <c r="L19" s="14"/>
       <c r="O19" s="14"/>
     </row>
     <row r="20" spans="3:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="15" t="s">
-        <v>544</v>
-      </c>
       <c r="F20" s="13"/>
-      <c r="G20" s="48"/>
+      <c r="G20" s="35"/>
       <c r="H20" s="15"/>
       <c r="I20" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="J20" s="53"/>
-      <c r="K20" s="45"/>
+      <c r="J20" s="38"/>
       <c r="L20" s="14"/>
       <c r="O20" s="14"/>
     </row>
     <row r="21" spans="3:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="15" t="s">
-        <v>543</v>
-      </c>
       <c r="F21" s="13"/>
-      <c r="G21" s="48"/>
+      <c r="G21" s="35"/>
       <c r="H21" s="15"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="45"/>
+      <c r="J21" s="38"/>
       <c r="L21" s="14"/>
       <c r="O21" s="14"/>
     </row>
     <row r="22" spans="3:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="15" t="s">
-        <v>542</v>
+      <c r="C22" s="25" t="s">
+        <v>571</v>
+      </c>
+      <c r="D22" s="10"/>
+      <c r="E22" s="20" t="s">
+        <v>540</v>
       </c>
       <c r="F22" s="13"/>
-      <c r="G22" s="49" t="s">
+      <c r="G22" s="36" t="s">
         <v>523</v>
       </c>
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="45"/>
+      <c r="J22" s="38"/>
       <c r="L22" s="14"/>
       <c r="O22" s="14"/>
     </row>
     <row r="23" spans="3:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="15" t="s">
-        <v>323</v>
+      <c r="C23" s="17" t="s">
+        <v>594</v>
       </c>
       <c r="F23" s="13"/>
       <c r="H23" s="15"/>
       <c r="I23" s="17" t="s">
         <v>597</v>
       </c>
-      <c r="K23" s="45"/>
       <c r="O23" s="14"/>
     </row>
     <row r="24" spans="3:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="40" t="s">
-        <v>208</v>
+      <c r="C24" s="17" t="s">
+        <v>196</v>
       </c>
       <c r="F24" s="13"/>
       <c r="H24" s="15"/>
@@ -11265,42 +11394,41 @@
       </c>
     </row>
     <row r="25" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C25" s="15" t="s">
-        <v>541</v>
+      <c r="C25" s="17" t="s">
+        <v>202</v>
       </c>
       <c r="F25" s="13"/>
-      <c r="G25" s="46"/>
+      <c r="G25" s="1"/>
       <c r="H25" s="15"/>
-      <c r="I25" s="52" t="s">
+      <c r="I25" s="17" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="26" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C26" s="44" t="s">
-        <v>593</v>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C26" s="17" t="s">
+        <v>214</v>
       </c>
       <c r="F26" s="13"/>
-      <c r="G26" s="46"/>
+      <c r="G26" s="1"/>
       <c r="H26" s="15"/>
     </row>
     <row r="27" spans="3:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="C27" s="17" t="s">
+        <v>223</v>
+      </c>
       <c r="F27" s="13"/>
-      <c r="G27" s="50" t="s">
+      <c r="G27" s="37" t="s">
         <v>539</v>
       </c>
-      <c r="H27" s="42"/>
+      <c r="H27" s="15"/>
       <c r="I27" s="17"/>
     </row>
-    <row r="28" spans="3:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="C28" s="25" t="s">
-        <v>571</v>
-      </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="20" t="s">
-        <v>540</v>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C28" s="17" t="s">
+        <v>595</v>
       </c>
       <c r="F28" s="13"/>
-      <c r="G28" s="51" t="s">
+      <c r="G28" s="37" t="s">
         <v>515</v>
       </c>
       <c r="H28" s="15"/>
@@ -11308,69 +11436,71 @@
     </row>
     <row r="29" spans="3:15" ht="30" x14ac:dyDescent="0.25">
       <c r="C29" s="17" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="F29" s="13"/>
-      <c r="G29" s="51" t="s">
+      <c r="G29" s="37" t="s">
         <v>514</v>
       </c>
       <c r="H29" s="15"/>
     </row>
     <row r="30" spans="3:15" ht="30" x14ac:dyDescent="0.25">
       <c r="C30" s="17" t="s">
-        <v>196</v>
+        <v>383</v>
       </c>
       <c r="F30" s="13"/>
-      <c r="G30" s="51" t="s">
+      <c r="G30" s="37" t="s">
         <v>513</v>
       </c>
       <c r="H30" s="15"/>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C31" s="17" t="s">
-        <v>202</v>
+        <v>384</v>
       </c>
       <c r="F31" s="13"/>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C32" s="17" t="s">
-        <v>214</v>
+        <v>562</v>
       </c>
       <c r="F32" s="13"/>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C33" s="17" t="s">
-        <v>223</v>
-      </c>
       <c r="F33" s="13"/>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" s="17" t="s">
-        <v>595</v>
+      <c r="C34" s="24" t="s">
+        <v>535</v>
+      </c>
+      <c r="D34" s="10"/>
+      <c r="E34" s="20" t="s">
+        <v>534</v>
       </c>
       <c r="F34" s="13"/>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C35" s="17" t="s">
-        <v>596</v>
-      </c>
       <c r="F35" s="13"/>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C36" s="17" t="s">
-        <v>383</v>
+      <c r="C36" s="24" t="s">
+        <v>532</v>
+      </c>
+      <c r="D36" s="10"/>
+      <c r="E36" s="20" t="s">
+        <v>531</v>
       </c>
       <c r="F36" s="13"/>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C37" s="17" t="s">
-        <v>384</v>
+        <v>84</v>
       </c>
       <c r="F37" s="13"/>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C38" s="17" t="s">
-        <v>562</v>
+        <v>526</v>
       </c>
       <c r="F38" s="13"/>
     </row>
@@ -11379,12 +11509,10 @@
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C40" s="24" t="s">
-        <v>535</v>
+        <v>602</v>
       </c>
       <c r="D40" s="10"/>
-      <c r="E40" s="20" t="s">
-        <v>534</v>
-      </c>
+      <c r="E40" s="32"/>
       <c r="F40" s="13"/>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.25">
@@ -11392,139 +11520,97 @@
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C42" s="24" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="20" t="s">
-        <v>531</v>
+        <v>51</v>
       </c>
       <c r="F42" s="13"/>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C43" s="15" t="s">
-        <v>529</v>
-      </c>
       <c r="F43" s="13"/>
     </row>
     <row r="44" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="17" t="s">
-        <v>84</v>
+      <c r="C44" s="24" t="s">
+        <v>517</v>
+      </c>
+      <c r="D44" s="10"/>
+      <c r="E44" s="20" t="s">
+        <v>516</v>
       </c>
       <c r="F44" s="13"/>
     </row>
     <row r="45" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C45" s="15" t="s">
-        <v>528</v>
-      </c>
       <c r="F45" s="13"/>
     </row>
     <row r="46" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C46" s="15" t="s">
-        <v>527</v>
+      <c r="E46" s="29" t="s">
+        <v>511</v>
       </c>
       <c r="F46" s="13"/>
     </row>
     <row r="47" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C47" s="17" t="s">
-        <v>526</v>
+      <c r="E47" s="29" t="s">
+        <v>510</v>
       </c>
       <c r="F47" s="13"/>
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C48" s="15" t="s">
-        <v>97</v>
+      <c r="E48" s="29" t="s">
+        <v>509</v>
       </c>
       <c r="F48" s="13"/>
     </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E49" s="29" t="s">
+        <v>508</v>
+      </c>
       <c r="F49" s="13"/>
     </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F50" s="13"/>
     </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C51" s="24" t="s">
-        <v>602</v>
-      </c>
-      <c r="D51" s="10"/>
-      <c r="E51" s="41"/>
+    <row r="51" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F51" s="13"/>
     </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C52" s="15" t="s">
-        <v>490</v>
-      </c>
+    <row r="52" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F52" s="13"/>
     </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C53" s="15" t="s">
-        <v>537</v>
-      </c>
+    <row r="53" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F53" s="13"/>
     </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C54" s="15" t="s">
-        <v>536</v>
-      </c>
+    <row r="54" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F54" s="13"/>
     </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F55" s="13"/>
     </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C56" s="24" t="s">
-        <v>524</v>
-      </c>
-      <c r="D56" s="10"/>
-      <c r="E56" s="20" t="s">
-        <v>51</v>
-      </c>
+    <row r="56" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F56" s="13"/>
     </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C57" s="15" t="s">
-        <v>522</v>
-      </c>
+    <row r="57" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F57" s="13"/>
     </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F58" s="13"/>
     </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C59" s="24" t="s">
-        <v>517</v>
-      </c>
-      <c r="D59" s="10"/>
-      <c r="E59" s="20" t="s">
-        <v>516</v>
-      </c>
+    <row r="59" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F59" s="13"/>
     </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F60" s="13"/>
     </row>
-    <row r="61" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="E61" s="29" t="s">
-        <v>511</v>
-      </c>
+    <row r="61" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F61" s="13"/>
     </row>
-    <row r="62" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E62" s="29" t="s">
-        <v>510</v>
-      </c>
+    <row r="62" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F62" s="13"/>
     </row>
-    <row r="63" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E63" s="29" t="s">
-        <v>509</v>
-      </c>
+    <row r="63" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F63" s="13"/>
     </row>
-    <row r="64" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E64" s="29" t="s">
-        <v>508</v>
-      </c>
+    <row r="64" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F64" s="13"/>
     </row>
     <row r="65" spans="6:6" x14ac:dyDescent="0.25">
@@ -11720,6 +11806,396 @@
     <mergeCell ref="K2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C27BB3F-052F-484F-A5E2-9F1596D6E0CC}">
+  <dimension ref="B2:G32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27:C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="40"/>
+    <col min="2" max="2" width="14.28515625" style="40" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="42" customWidth="1"/>
+    <col min="4" max="4" width="69.140625" style="40" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="40"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C2" s="40" t="s">
+        <v>604</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>605</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>625</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>626</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="55" t="s">
+        <v>556</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>553</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>606</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>609</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>607</v>
+      </c>
+      <c r="G3" s="39" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="55"/>
+      <c r="D4" s="44" t="s">
+        <v>550</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>609</v>
+      </c>
+      <c r="F4" s="40" t="s">
+        <v>608</v>
+      </c>
+      <c r="G4" s="39" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="55"/>
+      <c r="C5" s="42" t="s">
+        <v>346</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>593</v>
+      </c>
+      <c r="E5" s="40" t="s">
+        <v>610</v>
+      </c>
+      <c r="F5" s="40" t="s">
+        <v>617</v>
+      </c>
+      <c r="G5" s="40" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="55"/>
+      <c r="C6" s="42" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="55"/>
+      <c r="C7" s="42" t="s">
+        <v>540</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>594</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>611</v>
+      </c>
+      <c r="F7" s="40" t="s">
+        <v>612</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="55"/>
+      <c r="D8" s="44" t="s">
+        <v>202</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>613</v>
+      </c>
+      <c r="F8" s="40" t="s">
+        <v>614</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="55"/>
+      <c r="D9" s="44" t="s">
+        <v>214</v>
+      </c>
+      <c r="E9" s="40" t="s">
+        <v>615</v>
+      </c>
+      <c r="F9" s="40" t="s">
+        <v>616</v>
+      </c>
+      <c r="G9" s="45" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="55"/>
+      <c r="D10" s="44" t="s">
+        <v>223</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>618</v>
+      </c>
+      <c r="F10" s="40" t="s">
+        <v>619</v>
+      </c>
+      <c r="G10" s="45" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="55"/>
+      <c r="D11" s="44" t="s">
+        <v>595</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>622</v>
+      </c>
+      <c r="F11" s="40" t="s">
+        <v>621</v>
+      </c>
+      <c r="G11" s="46" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="55"/>
+      <c r="D12" s="44" t="s">
+        <v>596</v>
+      </c>
+      <c r="E12" s="40" t="s">
+        <v>622</v>
+      </c>
+      <c r="F12" s="40" t="s">
+        <v>620</v>
+      </c>
+      <c r="G12" s="39" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="55"/>
+      <c r="D13" s="44" t="s">
+        <v>562</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>623</v>
+      </c>
+      <c r="F13" s="40" t="s">
+        <v>624</v>
+      </c>
+      <c r="G13" s="45" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="55"/>
+      <c r="C14" s="43" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="55"/>
+      <c r="C15" s="43" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="55"/>
+      <c r="C16" s="43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="55"/>
+      <c r="C17" s="43" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B18" s="55"/>
+      <c r="C18" s="43" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="55"/>
+      <c r="C19" s="43" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="55"/>
+      <c r="C20" s="43" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="55"/>
+      <c r="C21" s="43" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="55"/>
+      <c r="C22" s="42" t="s">
+        <v>530</v>
+      </c>
+      <c r="D22" s="44" t="s">
+        <v>185</v>
+      </c>
+      <c r="E22" s="40" t="s">
+        <v>638</v>
+      </c>
+      <c r="F22" s="40" t="s">
+        <v>639</v>
+      </c>
+      <c r="G22" s="45" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B23" s="55"/>
+      <c r="C23" s="42" t="s">
+        <v>548</v>
+      </c>
+      <c r="D23" s="44" t="s">
+        <v>175</v>
+      </c>
+      <c r="E23" s="40" t="s">
+        <v>634</v>
+      </c>
+      <c r="F23" s="40" t="s">
+        <v>635</v>
+      </c>
+      <c r="G23" s="46" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="55"/>
+      <c r="D24" s="44" t="s">
+        <v>601</v>
+      </c>
+      <c r="E24" s="40" t="s">
+        <v>636</v>
+      </c>
+      <c r="F24" s="40" t="s">
+        <v>637</v>
+      </c>
+      <c r="G24" s="39" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B25" s="55"/>
+      <c r="C25" s="42" t="s">
+        <v>533</v>
+      </c>
+      <c r="D25" s="44" t="s">
+        <v>628</v>
+      </c>
+      <c r="E25" s="40" t="s">
+        <v>630</v>
+      </c>
+      <c r="F25" s="40" t="s">
+        <v>631</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="55"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="41" t="s">
+        <v>629</v>
+      </c>
+      <c r="E26" s="40" t="s">
+        <v>632</v>
+      </c>
+      <c r="F26" s="40" t="s">
+        <v>633</v>
+      </c>
+      <c r="G26" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B27" s="55"/>
+      <c r="C27" s="43" t="s">
+        <v>523</v>
+      </c>
+      <c r="D27" s="44"/>
+      <c r="G27" s="46"/>
+    </row>
+    <row r="28" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B28" s="55"/>
+      <c r="C28" s="43" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="55"/>
+      <c r="C29" s="43" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B30" s="55"/>
+      <c r="C30" s="43" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B31" s="55"/>
+      <c r="C31" s="43" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="43" t="s">
+        <v>552</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:B21"/>
+    <mergeCell ref="B22:B31"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G9" r:id="rId1" xr:uid="{EF3E61BA-B318-4F4C-A7AF-5BC8E9133193}"/>
+    <hyperlink ref="G11" r:id="rId2" xr:uid="{6B59BCFC-79AC-43C8-813A-06DF7F83E4F8}"/>
+    <hyperlink ref="G10" r:id="rId3" xr:uid="{8751EFB8-FBD8-4361-8550-22B77B26E17F}"/>
+    <hyperlink ref="G13" r:id="rId4" xr:uid="{9EA1EA89-F53B-4B70-9697-AB342AC89F28}"/>
+    <hyperlink ref="G22" r:id="rId5" xr:uid="{B30791C6-EA7D-48DC-A08B-FA39B41F0990}"/>
+    <hyperlink ref="G23" r:id="rId6" xr:uid="{A151BDFE-A2B1-48CC-97AA-52AE060AEFC5}"/>
+    <hyperlink ref="G25" r:id="rId7" xr:uid="{C6EBCFD0-E391-41D0-9C1E-C1B2BB1E2A69}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update on R scripts
</commit_message>
<xml_diff>
--- a/frontend/data/data_available.xlsx
+++ b/frontend/data/data_available.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bianka\Documents\MSc-Internship\Observatory-of-the-Mountains\frontend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{6CE4E154-741C-485D-BBC6-F74A05914EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02566AAA-52DA-4A8C-89E1-CD29EEFBA433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{8809251D-B3C6-41F0-B60D-9556D90BF91D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{8809251D-B3C6-41F0-B60D-9556D90BF91D}"/>
   </bookViews>
   <sheets>
     <sheet name="per county" sheetId="1" r:id="rId1"/>
     <sheet name="per topic" sheetId="4" r:id="rId2"/>
-    <sheet name="Q1_a" sheetId="5" r:id="rId3"/>
-    <sheet name="Q1_b" sheetId="6" r:id="rId4"/>
-    <sheet name="Hárok1" sheetId="7" r:id="rId5"/>
+    <sheet name="Q1" sheetId="5" r:id="rId3"/>
+    <sheet name="Q2" sheetId="6" r:id="rId4"/>
+    <sheet name="Hárok2" sheetId="9" r:id="rId5"/>
+    <sheet name="pre-processing steps" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'per county'!$E$1:$E$195</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1638" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="654">
   <si>
     <r>
       <t xml:space="preserve">gencat </t>
@@ -2341,12 +2341,54 @@
   <si>
     <t>land conversion (%)</t>
   </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t>Theil</t>
+  </si>
+  <si>
+    <t>BG</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Bgshare</t>
+  </si>
+  <si>
+    <t>Average price of newly build building (€/m²)</t>
+  </si>
+  <si>
+    <t>Real investment budget (€)</t>
+  </si>
+  <si>
+    <t>Unemployed population (%)</t>
+  </si>
+  <si>
+    <t>Social Foundation</t>
+  </si>
+  <si>
+    <t>Ecological ceiling</t>
+  </si>
+  <si>
+    <t>Land conversion (%)</t>
+  </si>
+  <si>
+    <t>Industrial waste (kg)</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Domestic water consumption (m³)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2434,6 +2476,19 @@
       <color theme="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2545,7 +2600,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2647,6 +2702,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2664,9 +2728,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3037,11 +3098,11 @@
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
       <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
@@ -3067,13 +3128,13 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" s="48" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+    <row r="3" spans="1:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="51" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="47" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+    <row r="4" spans="1:9" s="50" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="50" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3123,8 +3184,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="47" t="s">
+    <row r="7" spans="1:9" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="50" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3165,8 +3226,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="47" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+    <row r="10" spans="1:9" s="50" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="50" t="s">
         <v>29</v>
       </c>
     </row>
@@ -3261,18 +3322,18 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="49" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="49" t="s">
+    <row r="17" spans="1:9" s="52" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="52" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="47" t="s">
+    <row r="18" spans="1:9" s="50" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="50" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="53" t="s">
         <v>46</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -3298,7 +3359,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="50"/>
+      <c r="A20" s="53"/>
       <c r="B20" s="2" t="s">
         <v>282</v>
       </c>
@@ -3322,7 +3383,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
+      <c r="A21" s="53"/>
       <c r="B21" s="2" t="s">
         <v>284</v>
       </c>
@@ -3346,7 +3407,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
+      <c r="A22" s="53"/>
       <c r="B22" s="1" t="s">
         <v>583</v>
       </c>
@@ -3367,7 +3428,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="50"/>
+      <c r="A23" s="53"/>
       <c r="B23" s="1" t="s">
         <v>287</v>
       </c>
@@ -3391,7 +3452,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="50"/>
+      <c r="A24" s="53"/>
       <c r="B24" s="1" t="s">
         <v>291</v>
       </c>
@@ -3415,7 +3476,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
+      <c r="A25" s="53"/>
       <c r="B25" s="1" t="s">
         <v>294</v>
       </c>
@@ -3439,7 +3500,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="50"/>
+      <c r="A26" s="53"/>
       <c r="B26" s="1" t="s">
         <v>297</v>
       </c>
@@ -3463,7 +3524,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="50"/>
+      <c r="A27" s="53"/>
       <c r="B27" s="1" t="s">
         <v>300</v>
       </c>
@@ -3487,7 +3548,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="53" t="s">
         <v>49</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -3513,7 +3574,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="50"/>
+      <c r="A29" s="53"/>
       <c r="B29" s="1" t="s">
         <v>306</v>
       </c>
@@ -3537,7 +3598,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="50"/>
+      <c r="A30" s="53"/>
       <c r="B30" s="1" t="s">
         <v>309</v>
       </c>
@@ -3561,7 +3622,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="50"/>
+      <c r="A31" s="53"/>
       <c r="B31" s="1" t="s">
         <v>312</v>
       </c>
@@ -3585,7 +3646,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="50"/>
+      <c r="A32" s="53"/>
       <c r="B32" s="1" t="s">
         <v>314</v>
       </c>
@@ -3609,7 +3670,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="50"/>
+      <c r="A33" s="53"/>
       <c r="B33" s="1" t="s">
         <v>317</v>
       </c>
@@ -3633,7 +3694,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="50"/>
+      <c r="A34" s="53"/>
       <c r="B34" s="1" t="s">
         <v>320</v>
       </c>
@@ -3657,7 +3718,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="50"/>
+      <c r="A35" s="53"/>
       <c r="B35" s="1" t="s">
         <v>323</v>
       </c>
@@ -3681,7 +3742,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="50"/>
+      <c r="A36" s="53"/>
       <c r="B36" s="1" t="s">
         <v>327</v>
       </c>
@@ -3705,7 +3766,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="50" t="s">
+      <c r="A37" s="53" t="s">
         <v>346</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -3731,7 +3792,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="50"/>
+      <c r="A38" s="53"/>
       <c r="B38" s="1" t="s">
         <v>330</v>
       </c>
@@ -3755,7 +3816,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="50"/>
+      <c r="A39" s="53"/>
       <c r="B39" s="1" t="s">
         <v>335</v>
       </c>
@@ -3779,7 +3840,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="50"/>
+      <c r="A40" s="53"/>
       <c r="B40" s="1" t="s">
         <v>338</v>
       </c>
@@ -3803,7 +3864,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="50"/>
+      <c r="A41" s="53"/>
       <c r="B41" s="1" t="s">
         <v>340</v>
       </c>
@@ -3827,7 +3888,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="50"/>
+      <c r="A42" s="53"/>
       <c r="B42" s="1" t="s">
         <v>343</v>
       </c>
@@ -3851,7 +3912,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="50" t="s">
+      <c r="A43" s="53" t="s">
         <v>48</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -3877,7 +3938,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="50"/>
+      <c r="A44" s="53"/>
       <c r="B44" s="1" t="s">
         <v>348</v>
       </c>
@@ -3901,7 +3962,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="50"/>
+      <c r="A45" s="53"/>
       <c r="B45" s="1" t="s">
         <v>349</v>
       </c>
@@ -3925,7 +3986,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="50"/>
+      <c r="A46" s="53"/>
       <c r="B46" s="1" t="s">
         <v>350</v>
       </c>
@@ -3949,7 +4010,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="50" t="s">
+      <c r="A47" s="53" t="s">
         <v>50</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -3975,7 +4036,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="50"/>
+      <c r="A48" s="53"/>
       <c r="B48" s="1" t="s">
         <v>360</v>
       </c>
@@ -3999,7 +4060,7 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="50" t="s">
+      <c r="A49" s="53" t="s">
         <v>51</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -4025,7 +4086,7 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="50"/>
+      <c r="A50" s="53"/>
       <c r="B50" s="1" t="s">
         <v>367</v>
       </c>
@@ -4049,7 +4110,7 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="50"/>
+      <c r="A51" s="53"/>
       <c r="B51" s="1" t="s">
         <v>368</v>
       </c>
@@ -4073,7 +4134,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="50"/>
+      <c r="A52" s="53"/>
       <c r="B52" s="1" t="s">
         <v>369</v>
       </c>
@@ -4097,7 +4158,7 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="50"/>
+      <c r="A53" s="53"/>
       <c r="B53" s="1" t="s">
         <v>370</v>
       </c>
@@ -4121,7 +4182,7 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="50"/>
+      <c r="A54" s="53"/>
       <c r="B54" s="1" t="s">
         <v>371</v>
       </c>
@@ -4145,7 +4206,7 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="50"/>
+      <c r="A55" s="53"/>
       <c r="B55" s="2" t="s">
         <v>383</v>
       </c>
@@ -4169,7 +4230,7 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="50"/>
+      <c r="A56" s="53"/>
       <c r="B56" s="2" t="s">
         <v>384</v>
       </c>
@@ -4193,7 +4254,7 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="50"/>
+      <c r="A57" s="53"/>
       <c r="B57" s="1" t="s">
         <v>80</v>
       </c>
@@ -4217,7 +4278,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="50"/>
+      <c r="A58" s="53"/>
       <c r="B58" s="1" t="s">
         <v>80</v>
       </c>
@@ -4241,7 +4302,7 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="50"/>
+      <c r="A59" s="53"/>
       <c r="B59" s="1" t="s">
         <v>80</v>
       </c>
@@ -4265,7 +4326,7 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="50"/>
+      <c r="A60" s="53"/>
       <c r="B60" s="1" t="s">
         <v>80</v>
       </c>
@@ -4289,7 +4350,7 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="50"/>
+      <c r="A61" s="53"/>
       <c r="B61" s="1" t="s">
         <v>396</v>
       </c>
@@ -4313,7 +4374,7 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="50"/>
+      <c r="A62" s="53"/>
       <c r="B62" s="2" t="s">
         <v>401</v>
       </c>
@@ -4337,7 +4398,7 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="50"/>
+      <c r="A63" s="53"/>
       <c r="B63" s="1" t="s">
         <v>402</v>
       </c>
@@ -4360,13 +4421,13 @@
         <v>404</v>
       </c>
     </row>
-    <row r="65" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="47" t="s">
+    <row r="65" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="50" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="50" t="s">
+      <c r="A66" s="53" t="s">
         <v>54</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -4392,7 +4453,7 @@
       </c>
     </row>
     <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="50"/>
+      <c r="A67" s="53"/>
       <c r="B67" s="1" t="s">
         <v>236</v>
       </c>
@@ -4416,7 +4477,7 @@
       </c>
     </row>
     <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="50"/>
+      <c r="A68" s="53"/>
       <c r="B68" s="1" t="s">
         <v>239</v>
       </c>
@@ -4440,7 +4501,7 @@
       </c>
     </row>
     <row r="69" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="50"/>
+      <c r="A69" s="53"/>
       <c r="B69" s="1" t="s">
         <v>507</v>
       </c>
@@ -4464,7 +4525,7 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="50"/>
+      <c r="A70" s="53"/>
       <c r="B70" s="1" t="s">
         <v>245</v>
       </c>
@@ -4488,7 +4549,7 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="50"/>
+      <c r="A71" s="53"/>
       <c r="B71" s="1" t="s">
         <v>248</v>
       </c>
@@ -4512,7 +4573,7 @@
       </c>
     </row>
     <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="50"/>
+      <c r="A72" s="53"/>
       <c r="B72" s="1" t="s">
         <v>250</v>
       </c>
@@ -4536,7 +4597,7 @@
       </c>
     </row>
     <row r="73" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="50" t="s">
+      <c r="A73" s="53" t="s">
         <v>55</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -4562,7 +4623,7 @@
       </c>
     </row>
     <row r="74" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="50"/>
+      <c r="A74" s="53"/>
       <c r="B74" s="1" t="s">
         <v>255</v>
       </c>
@@ -4586,7 +4647,7 @@
       </c>
     </row>
     <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="50"/>
+      <c r="A75" s="53"/>
       <c r="B75" s="1" t="s">
         <v>258</v>
       </c>
@@ -4610,7 +4671,7 @@
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="50"/>
+      <c r="A76" s="53"/>
       <c r="B76" s="1" t="s">
         <v>261</v>
       </c>
@@ -4634,7 +4695,7 @@
       </c>
     </row>
     <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="50"/>
+      <c r="A77" s="53"/>
       <c r="B77" s="1" t="s">
         <v>264</v>
       </c>
@@ -4658,7 +4719,7 @@
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="50"/>
+      <c r="A78" s="53"/>
       <c r="B78" s="1" t="s">
         <v>267</v>
       </c>
@@ -4682,7 +4743,7 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="50"/>
+      <c r="A79" s="53"/>
       <c r="B79" s="1" t="s">
         <v>270</v>
       </c>
@@ -4706,7 +4767,7 @@
       </c>
     </row>
     <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="50"/>
+      <c r="A80" s="53"/>
       <c r="B80" s="1" t="s">
         <v>273</v>
       </c>
@@ -4730,7 +4791,7 @@
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="50"/>
+      <c r="A81" s="53"/>
       <c r="B81" s="1" t="s">
         <v>276</v>
       </c>
@@ -4753,13 +4814,13 @@
         <v>278</v>
       </c>
     </row>
-    <row r="83" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="47" t="s">
+    <row r="83" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="50" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="50" t="s">
+      <c r="A84" s="53" t="s">
         <v>57</v>
       </c>
       <c r="B84" s="2" t="s">
@@ -4785,7 +4846,7 @@
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="50"/>
+      <c r="A85" s="53"/>
       <c r="B85" s="2" t="s">
         <v>196</v>
       </c>
@@ -4809,7 +4870,7 @@
       </c>
     </row>
     <row r="86" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A86" s="50"/>
+      <c r="A86" s="53"/>
       <c r="B86" s="2" t="s">
         <v>199</v>
       </c>
@@ -4833,7 +4894,7 @@
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="50"/>
+      <c r="A87" s="53"/>
       <c r="B87" s="2" t="s">
         <v>202</v>
       </c>
@@ -4857,7 +4918,7 @@
       </c>
     </row>
     <row r="88" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="50"/>
+      <c r="A88" s="53"/>
       <c r="B88" s="2" t="s">
         <v>205</v>
       </c>
@@ -4881,7 +4942,7 @@
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="50" t="s">
+      <c r="A89" s="53" t="s">
         <v>58</v>
       </c>
       <c r="B89" s="2" t="s">
@@ -4907,7 +4968,7 @@
       </c>
     </row>
     <row r="90" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="50"/>
+      <c r="A90" s="53"/>
       <c r="B90" s="2" t="s">
         <v>211</v>
       </c>
@@ -4931,7 +4992,7 @@
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="50" t="s">
+      <c r="A91" s="53" t="s">
         <v>59</v>
       </c>
       <c r="B91" s="2" t="s">
@@ -4954,7 +5015,7 @@
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="50"/>
+      <c r="A92" s="53"/>
       <c r="B92" s="2" t="s">
         <v>216</v>
       </c>
@@ -4978,7 +5039,7 @@
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="50"/>
+      <c r="A93" s="53"/>
       <c r="B93" s="1" t="s">
         <v>218</v>
       </c>
@@ -5002,7 +5063,7 @@
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="50"/>
+      <c r="A94" s="53"/>
       <c r="B94" s="1" t="s">
         <v>219</v>
       </c>
@@ -5026,7 +5087,7 @@
       </c>
     </row>
     <row r="95" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="50"/>
+      <c r="A95" s="53"/>
       <c r="B95" s="1" t="s">
         <v>223</v>
       </c>
@@ -5050,7 +5111,7 @@
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="50" t="s">
+      <c r="A96" s="53" t="s">
         <v>60</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -5076,7 +5137,7 @@
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="50"/>
+      <c r="A97" s="53"/>
       <c r="B97" s="1" t="s">
         <v>229</v>
       </c>
@@ -5099,13 +5160,13 @@
         <v>231</v>
       </c>
     </row>
-    <row r="99" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="47" t="s">
+    <row r="99" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="50" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A100" s="50" t="s">
+      <c r="A100" s="53" t="s">
         <v>105</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -5131,7 +5192,7 @@
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="50"/>
+      <c r="A101" s="53"/>
       <c r="B101" s="1" t="s">
         <v>72</v>
       </c>
@@ -5155,7 +5216,7 @@
       </c>
     </row>
     <row r="102" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A102" s="50"/>
+      <c r="A102" s="53"/>
       <c r="B102" s="1" t="s">
         <v>74</v>
       </c>
@@ -5179,7 +5240,7 @@
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="50"/>
+      <c r="A103" s="53"/>
       <c r="B103" s="1" t="s">
         <v>77</v>
       </c>
@@ -5203,7 +5264,7 @@
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="50"/>
+      <c r="A104" s="53"/>
       <c r="B104" s="1" t="s">
         <v>80</v>
       </c>
@@ -5227,7 +5288,7 @@
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="50"/>
+      <c r="A105" s="53"/>
       <c r="B105" s="1" t="s">
         <v>84</v>
       </c>
@@ -5251,7 +5312,7 @@
       </c>
     </row>
     <row r="106" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A106" s="50"/>
+      <c r="A106" s="53"/>
       <c r="B106" s="2" t="s">
         <v>87</v>
       </c>
@@ -5275,7 +5336,7 @@
       </c>
     </row>
     <row r="107" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A107" s="50"/>
+      <c r="A107" s="53"/>
       <c r="B107" s="1" t="s">
         <v>90</v>
       </c>
@@ -5299,7 +5360,7 @@
       </c>
     </row>
     <row r="108" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A108" s="50"/>
+      <c r="A108" s="53"/>
       <c r="B108" s="2" t="s">
         <v>93</v>
       </c>
@@ -5323,7 +5384,7 @@
       </c>
     </row>
     <row r="109" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A109" s="50"/>
+      <c r="A109" s="53"/>
       <c r="B109" s="1" t="s">
         <v>97</v>
       </c>
@@ -5347,7 +5408,7 @@
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="50" t="s">
+      <c r="A110" s="53" t="s">
         <v>106</v>
       </c>
       <c r="B110" s="1" t="s">
@@ -5373,7 +5434,7 @@
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" s="50"/>
+      <c r="A111" s="53"/>
       <c r="B111" s="1" t="s">
         <v>102</v>
       </c>
@@ -5397,7 +5458,7 @@
       </c>
     </row>
     <row r="112" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A112" s="50" t="s">
+      <c r="A112" s="53" t="s">
         <v>61</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -5423,7 +5484,7 @@
       </c>
     </row>
     <row r="113" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" s="50"/>
+      <c r="A113" s="53"/>
       <c r="B113" s="1" t="s">
         <v>110</v>
       </c>
@@ -5447,7 +5508,7 @@
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="50"/>
+      <c r="A114" s="53"/>
       <c r="B114" s="1" t="s">
         <v>112</v>
       </c>
@@ -5471,7 +5532,7 @@
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="50"/>
+      <c r="A115" s="53"/>
       <c r="B115" s="1" t="s">
         <v>115</v>
       </c>
@@ -5495,7 +5556,7 @@
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" s="50"/>
+      <c r="A116" s="53"/>
       <c r="B116" s="1" t="s">
         <v>118</v>
       </c>
@@ -5519,7 +5580,7 @@
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117" s="50"/>
+      <c r="A117" s="53"/>
       <c r="B117" s="1" t="s">
         <v>123</v>
       </c>
@@ -5543,7 +5604,7 @@
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A118" s="50"/>
+      <c r="A118" s="53"/>
       <c r="B118" s="1" t="s">
         <v>124</v>
       </c>
@@ -5567,7 +5628,7 @@
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119" s="50"/>
+      <c r="A119" s="53"/>
       <c r="B119" s="1" t="s">
         <v>127</v>
       </c>
@@ -5591,7 +5652,7 @@
       </c>
     </row>
     <row r="120" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="50" t="s">
+      <c r="A120" s="53" t="s">
         <v>62</v>
       </c>
       <c r="B120" s="1" t="s">
@@ -5617,7 +5678,7 @@
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A121" s="50"/>
+      <c r="A121" s="53"/>
       <c r="B121" s="1" t="s">
         <v>133</v>
       </c>
@@ -5641,7 +5702,7 @@
       </c>
     </row>
     <row r="122" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A122" s="50" t="s">
+      <c r="A122" s="53" t="s">
         <v>63</v>
       </c>
       <c r="B122" s="1" t="s">
@@ -5667,7 +5728,7 @@
       </c>
     </row>
     <row r="123" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A123" s="50"/>
+      <c r="A123" s="53"/>
       <c r="B123" s="1" t="s">
         <v>139</v>
       </c>
@@ -5691,7 +5752,7 @@
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" s="50"/>
+      <c r="A124" s="53"/>
       <c r="B124" s="1" t="s">
         <v>142</v>
       </c>
@@ -5715,7 +5776,7 @@
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A125" s="50"/>
+      <c r="A125" s="53"/>
       <c r="B125" s="1" t="s">
         <v>146</v>
       </c>
@@ -5738,13 +5799,13 @@
         <v>148</v>
       </c>
     </row>
-    <row r="127" spans="1:9" s="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="47" t="s">
+    <row r="127" spans="1:9" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="50" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A128" s="50" t="s">
+      <c r="A128" s="53" t="s">
         <v>65</v>
       </c>
       <c r="B128" s="1" t="s">
@@ -5770,7 +5831,7 @@
       </c>
     </row>
     <row r="129" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A129" s="50"/>
+      <c r="A129" s="53"/>
       <c r="B129" s="2" t="s">
         <v>152</v>
       </c>
@@ -5794,7 +5855,7 @@
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A130" s="50"/>
+      <c r="A130" s="53"/>
       <c r="B130" s="2" t="s">
         <v>154</v>
       </c>
@@ -5818,7 +5879,7 @@
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A131" s="50"/>
+      <c r="A131" s="53"/>
       <c r="B131" s="1" t="s">
         <v>158</v>
       </c>
@@ -5842,7 +5903,7 @@
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="50"/>
+      <c r="A132" s="53"/>
       <c r="B132" s="2" t="s">
         <v>161</v>
       </c>
@@ -5866,7 +5927,7 @@
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A133" s="50"/>
+      <c r="A133" s="53"/>
       <c r="B133" s="2" t="s">
         <v>164</v>
       </c>
@@ -5890,7 +5951,7 @@
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A134" s="50"/>
+      <c r="A134" s="53"/>
       <c r="B134" s="1" t="s">
         <v>166</v>
       </c>
@@ -5914,7 +5975,7 @@
       </c>
     </row>
     <row r="135" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A135" s="50"/>
+      <c r="A135" s="53"/>
       <c r="B135" s="2" t="s">
         <v>169</v>
       </c>
@@ -5938,7 +5999,7 @@
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A136" s="50"/>
+      <c r="A136" s="53"/>
       <c r="B136" s="1" t="s">
         <v>172</v>
       </c>
@@ -5962,7 +6023,7 @@
       </c>
     </row>
     <row r="137" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A137" s="50"/>
+      <c r="A137" s="53"/>
       <c r="B137" s="1" t="s">
         <v>175</v>
       </c>
@@ -5986,7 +6047,7 @@
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A138" s="50"/>
+      <c r="A138" s="53"/>
       <c r="B138" s="1" t="s">
         <v>178</v>
       </c>
@@ -6010,7 +6071,7 @@
       </c>
     </row>
     <row r="139" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A139" s="50"/>
+      <c r="A139" s="53"/>
       <c r="B139" s="1" t="s">
         <v>181</v>
       </c>
@@ -6034,7 +6095,7 @@
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A140" s="50" t="s">
+      <c r="A140" s="53" t="s">
         <v>66</v>
       </c>
       <c r="B140" s="1" t="s">
@@ -6046,7 +6107,7 @@
       <c r="I140" s="1"/>
     </row>
     <row r="141" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A141" s="50"/>
+      <c r="A141" s="53"/>
       <c r="B141" s="2" t="s">
         <v>185</v>
       </c>
@@ -6070,7 +6131,7 @@
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A142" s="50"/>
+      <c r="A142" s="53"/>
       <c r="B142" s="1" t="s">
         <v>188</v>
       </c>
@@ -6082,7 +6143,7 @@
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A143" s="50"/>
+      <c r="A143" s="53"/>
       <c r="B143" s="1" t="s">
         <v>190</v>
       </c>
@@ -6102,13 +6163,13 @@
         <v>192</v>
       </c>
     </row>
-    <row r="145" spans="1:9" s="52" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="52" t="s">
+    <row r="145" spans="1:9" s="55" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="55" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A146" s="50" t="s">
+      <c r="A146" s="53" t="s">
         <v>416</v>
       </c>
       <c r="B146" s="1" t="s">
@@ -6122,7 +6183,7 @@
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A147" s="50"/>
+      <c r="A147" s="53"/>
       <c r="B147" s="1" t="s">
         <v>408</v>
       </c>
@@ -6137,7 +6198,7 @@
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A148" s="50"/>
+      <c r="A148" s="53"/>
       <c r="B148" s="1" t="s">
         <v>409</v>
       </c>
@@ -6149,7 +6210,7 @@
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A149" s="50"/>
+      <c r="A149" s="53"/>
       <c r="B149" s="1" t="s">
         <v>158</v>
       </c>
@@ -6167,7 +6228,7 @@
       </c>
     </row>
     <row r="150" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="50"/>
+      <c r="A150" s="53"/>
       <c r="B150" s="1" t="s">
         <v>410</v>
       </c>
@@ -6182,7 +6243,7 @@
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A151" s="50"/>
+      <c r="A151" s="53"/>
       <c r="B151" s="1" t="s">
         <v>432</v>
       </c>
@@ -6194,7 +6255,7 @@
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A152" s="50"/>
+      <c r="A152" s="53"/>
       <c r="B152" s="1" t="s">
         <v>411</v>
       </c>
@@ -6209,7 +6270,7 @@
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A153" s="50"/>
+      <c r="A153" s="53"/>
       <c r="B153" s="1" t="s">
         <v>412</v>
       </c>
@@ -6221,7 +6282,7 @@
       </c>
     </row>
     <row r="154" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A154" s="50"/>
+      <c r="A154" s="53"/>
       <c r="B154" s="1" t="s">
         <v>413</v>
       </c>
@@ -6233,7 +6294,7 @@
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A155" s="50"/>
+      <c r="A155" s="53"/>
       <c r="B155" s="1" t="s">
         <v>414</v>
       </c>
@@ -6262,7 +6323,7 @@
       </c>
     </row>
     <row r="157" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="50" t="s">
+      <c r="A157" s="53" t="s">
         <v>420</v>
       </c>
       <c r="B157" s="1" t="s">
@@ -6279,7 +6340,7 @@
       </c>
     </row>
     <row r="158" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A158" s="50"/>
+      <c r="A158" s="53"/>
       <c r="B158" s="1" t="s">
         <v>441</v>
       </c>
@@ -6297,7 +6358,7 @@
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A159" s="50"/>
+      <c r="A159" s="53"/>
       <c r="B159" s="1" t="s">
         <v>444</v>
       </c>
@@ -6309,7 +6370,7 @@
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A160" s="50"/>
+      <c r="A160" s="53"/>
       <c r="B160" s="1" t="s">
         <v>446</v>
       </c>
@@ -6321,7 +6382,7 @@
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A161" s="50"/>
+      <c r="A161" s="53"/>
       <c r="B161" s="1" t="s">
         <v>448</v>
       </c>
@@ -6333,7 +6394,7 @@
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A162" s="50"/>
+      <c r="A162" s="53"/>
       <c r="B162" s="1" t="s">
         <v>450</v>
       </c>
@@ -6345,7 +6406,7 @@
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A163" s="50"/>
+      <c r="A163" s="53"/>
       <c r="B163" s="1" t="s">
         <v>452</v>
       </c>
@@ -6357,7 +6418,7 @@
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A164" s="50" t="s">
+      <c r="A164" s="53" t="s">
         <v>454</v>
       </c>
       <c r="B164" s="1" t="s">
@@ -6374,7 +6435,7 @@
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A165" s="50"/>
+      <c r="A165" s="53"/>
       <c r="B165" s="1" t="s">
         <v>457</v>
       </c>
@@ -6386,7 +6447,7 @@
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A166" s="50" t="s">
+      <c r="A166" s="53" t="s">
         <v>458</v>
       </c>
       <c r="B166" s="1" t="s">
@@ -6403,7 +6464,7 @@
       </c>
     </row>
     <row r="167" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A167" s="50"/>
+      <c r="A167" s="53"/>
       <c r="B167" s="1" t="s">
         <v>461</v>
       </c>
@@ -6418,7 +6479,7 @@
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A168" s="50" t="s">
+      <c r="A168" s="53" t="s">
         <v>463</v>
       </c>
       <c r="B168" s="1" t="s">
@@ -6435,7 +6496,7 @@
       </c>
     </row>
     <row r="169" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="50"/>
+      <c r="A169" s="53"/>
       <c r="B169" s="1" t="s">
         <v>465</v>
       </c>
@@ -6450,7 +6511,7 @@
       </c>
     </row>
     <row r="170" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="50" t="s">
+      <c r="A170" s="53" t="s">
         <v>467</v>
       </c>
       <c r="B170" s="1" t="s">
@@ -6471,7 +6532,7 @@
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A171" s="50"/>
+      <c r="A171" s="53"/>
       <c r="B171" s="1" t="s">
         <v>469</v>
       </c>
@@ -6484,14 +6545,14 @@
       <c r="H171" s="7"/>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A172" s="50"/>
+      <c r="A172" s="53"/>
       <c r="B172" s="1" t="s">
         <v>470</v>
       </c>
       <c r="H172" s="7"/>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A173" s="50"/>
+      <c r="A173" s="53"/>
       <c r="B173" s="1" t="s">
         <v>471</v>
       </c>
@@ -6504,14 +6565,14 @@
       <c r="H173" s="7"/>
     </row>
     <row r="174" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A174" s="50"/>
+      <c r="A174" s="53"/>
       <c r="B174" s="1" t="s">
         <v>472</v>
       </c>
       <c r="H174" s="7"/>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A175" s="50"/>
+      <c r="A175" s="53"/>
       <c r="B175" s="1" t="s">
         <v>473</v>
       </c>
@@ -6524,7 +6585,7 @@
       <c r="H175" s="7"/>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A176" s="50"/>
+      <c r="A176" s="53"/>
       <c r="B176" s="1" t="s">
         <v>474</v>
       </c>
@@ -6537,7 +6598,7 @@
       <c r="H176" s="7"/>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A177" s="50"/>
+      <c r="A177" s="53"/>
       <c r="B177" s="1" t="s">
         <v>475</v>
       </c>
@@ -6550,7 +6611,7 @@
       <c r="H177" s="7"/>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A178" s="50"/>
+      <c r="A178" s="53"/>
       <c r="B178" s="1" t="s">
         <v>476</v>
       </c>
@@ -6563,7 +6624,7 @@
       <c r="H178" s="7"/>
     </row>
     <row r="179" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="50" t="s">
+      <c r="A179" s="53" t="s">
         <v>478</v>
       </c>
       <c r="B179" s="1" t="s">
@@ -6581,7 +6642,7 @@
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A180" s="50"/>
+      <c r="A180" s="53"/>
       <c r="B180" s="1" t="s">
         <v>480</v>
       </c>
@@ -6594,7 +6655,7 @@
       <c r="H180" s="7"/>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A181" s="50"/>
+      <c r="A181" s="53"/>
       <c r="B181" s="1" t="s">
         <v>481</v>
       </c>
@@ -6607,7 +6668,7 @@
       <c r="H181" s="7"/>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A182" s="50"/>
+      <c r="A182" s="53"/>
       <c r="B182" s="1" t="s">
         <v>482</v>
       </c>
@@ -6620,7 +6681,7 @@
       <c r="H182" s="7"/>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A183" s="50"/>
+      <c r="A183" s="53"/>
       <c r="B183" s="1" t="s">
         <v>483</v>
       </c>
@@ -6633,7 +6694,7 @@
       <c r="H183" s="7"/>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A184" s="50"/>
+      <c r="A184" s="53"/>
       <c r="B184" s="1" t="s">
         <v>484</v>
       </c>
@@ -6646,7 +6707,7 @@
       <c r="H184" s="7"/>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A185" s="50"/>
+      <c r="A185" s="53"/>
       <c r="B185" s="1" t="s">
         <v>485</v>
       </c>
@@ -6659,7 +6720,7 @@
       <c r="H185" s="7"/>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A186" s="50"/>
+      <c r="A186" s="53"/>
       <c r="B186" s="1" t="s">
         <v>486</v>
       </c>
@@ -6672,7 +6733,7 @@
       <c r="H186" s="7"/>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A187" s="50"/>
+      <c r="A187" s="53"/>
       <c r="B187" s="1" t="s">
         <v>487</v>
       </c>
@@ -6685,7 +6746,7 @@
       <c r="H187" s="7"/>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A188" s="50"/>
+      <c r="A188" s="53"/>
       <c r="B188" s="1" t="s">
         <v>488</v>
       </c>
@@ -6698,7 +6759,7 @@
       <c r="H188" s="7"/>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A189" s="50"/>
+      <c r="A189" s="53"/>
       <c r="B189" s="2" t="s">
         <v>489</v>
       </c>
@@ -6711,7 +6772,7 @@
       <c r="H189" s="7"/>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A190" s="50"/>
+      <c r="A190" s="53"/>
       <c r="B190" s="1" t="s">
         <v>490</v>
       </c>
@@ -6744,7 +6805,7 @@
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A192" s="50" t="s">
+      <c r="A192" s="53" t="s">
         <v>495</v>
       </c>
       <c r="B192" s="1" t="s">
@@ -6764,7 +6825,7 @@
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A193" s="50"/>
+      <c r="A193" s="53"/>
       <c r="B193" s="1" t="s">
         <v>498</v>
       </c>
@@ -6773,7 +6834,7 @@
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A194" s="50" t="s">
+      <c r="A194" s="53" t="s">
         <v>106</v>
       </c>
       <c r="B194" s="1" t="s">
@@ -6790,7 +6851,7 @@
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A195" s="50"/>
+      <c r="A195" s="53"/>
       <c r="B195" s="1" t="s">
         <v>502</v>
       </c>
@@ -6895,8 +6956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27833425-745A-496A-BBBC-9D84991CFB19}">
   <dimension ref="B2:S199"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="88" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView topLeftCell="A21" zoomScale="88" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39:F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6926,17 +6987,17 @@
         <v>558</v>
       </c>
       <c r="G2" s="9"/>
-      <c r="H2" s="54" t="s">
+      <c r="H2" s="56" t="s">
         <v>557</v>
       </c>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
       <c r="M2" s="27" t="s">
         <v>578</v>
       </c>
       <c r="N2" s="1"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
@@ -8164,8 +8225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC2F606-BCE5-41DE-997B-370E48010E8A}">
   <dimension ref="A1:H129"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="B121" sqref="B121"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113:XFD113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8182,11 +8243,11 @@
       <c r="A1" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
       <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
@@ -8209,18 +8270,18 @@
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" s="49" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+    <row r="3" spans="1:8" s="52" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+    <row r="4" spans="1:8" s="50" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="50" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="53" t="s">
         <v>46</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -8246,7 +8307,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="50"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="2" t="s">
         <v>282</v>
       </c>
@@ -8270,7 +8331,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="2" t="s">
         <v>284</v>
       </c>
@@ -8294,7 +8355,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="1" t="s">
         <v>592</v>
       </c>
@@ -8315,7 +8376,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="1" t="s">
         <v>287</v>
       </c>
@@ -8339,7 +8400,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
+      <c r="A10" s="53"/>
       <c r="B10" s="1" t="s">
         <v>291</v>
       </c>
@@ -8363,7 +8424,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
+      <c r="A11" s="53"/>
       <c r="B11" s="1" t="s">
         <v>294</v>
       </c>
@@ -8387,7 +8448,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
+      <c r="A12" s="53"/>
       <c r="B12" s="1" t="s">
         <v>297</v>
       </c>
@@ -8411,7 +8472,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
+      <c r="A13" s="53"/>
       <c r="B13" s="1" t="s">
         <v>300</v>
       </c>
@@ -8435,7 +8496,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="50" t="s">
+      <c r="A14" s="53" t="s">
         <v>49</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -8461,7 +8522,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="50"/>
+      <c r="A15" s="53"/>
       <c r="B15" s="1" t="s">
         <v>306</v>
       </c>
@@ -8485,7 +8546,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="50"/>
+      <c r="A16" s="53"/>
       <c r="B16" s="1" t="s">
         <v>309</v>
       </c>
@@ -8509,7 +8570,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="50"/>
+      <c r="A17" s="53"/>
       <c r="B17" s="1" t="s">
         <v>312</v>
       </c>
@@ -8533,7 +8594,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="50"/>
+      <c r="A18" s="53"/>
       <c r="B18" s="1" t="s">
         <v>314</v>
       </c>
@@ -8557,7 +8618,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="50"/>
+      <c r="A19" s="53"/>
       <c r="B19" s="1" t="s">
         <v>317</v>
       </c>
@@ -8581,7 +8642,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="50"/>
+      <c r="A20" s="53"/>
       <c r="B20" s="1" t="s">
         <v>320</v>
       </c>
@@ -8605,7 +8666,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
+      <c r="A21" s="53"/>
       <c r="B21" s="1" t="s">
         <v>323</v>
       </c>
@@ -8629,7 +8690,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
+      <c r="A22" s="53"/>
       <c r="B22" s="1" t="s">
         <v>327</v>
       </c>
@@ -8653,7 +8714,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="50" t="s">
+      <c r="A23" s="53" t="s">
         <v>346</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -8679,7 +8740,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="50"/>
+      <c r="A24" s="53"/>
       <c r="B24" s="1" t="s">
         <v>330</v>
       </c>
@@ -8703,7 +8764,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
+      <c r="A25" s="53"/>
       <c r="B25" s="1" t="s">
         <v>335</v>
       </c>
@@ -8727,7 +8788,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="50"/>
+      <c r="A26" s="53"/>
       <c r="B26" s="1" t="s">
         <v>338</v>
       </c>
@@ -8751,7 +8812,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="50"/>
+      <c r="A27" s="53"/>
       <c r="B27" s="1" t="s">
         <v>340</v>
       </c>
@@ -8775,7 +8836,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="50"/>
+      <c r="A28" s="53"/>
       <c r="B28" s="2" t="s">
         <v>343</v>
       </c>
@@ -8799,7 +8860,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="50" t="s">
+      <c r="A29" s="53" t="s">
         <v>48</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -8825,7 +8886,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="50"/>
+      <c r="A30" s="53"/>
       <c r="B30" s="1" t="s">
         <v>348</v>
       </c>
@@ -8849,7 +8910,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="50"/>
+      <c r="A31" s="53"/>
       <c r="B31" s="1" t="s">
         <v>349</v>
       </c>
@@ -8873,7 +8934,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="50"/>
+      <c r="A32" s="53"/>
       <c r="B32" s="1" t="s">
         <v>350</v>
       </c>
@@ -8897,7 +8958,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="50" t="s">
+      <c r="A33" s="53" t="s">
         <v>50</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -8923,7 +8984,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="50"/>
+      <c r="A34" s="53"/>
       <c r="B34" s="1" t="s">
         <v>360</v>
       </c>
@@ -8947,7 +9008,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="50" t="s">
+      <c r="A35" s="53" t="s">
         <v>51</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -8973,7 +9034,7 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="50"/>
+      <c r="A36" s="53"/>
       <c r="B36" s="1" t="s">
         <v>367</v>
       </c>
@@ -8997,7 +9058,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="50"/>
+      <c r="A37" s="53"/>
       <c r="B37" s="1" t="s">
         <v>368</v>
       </c>
@@ -9021,7 +9082,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="50"/>
+      <c r="A38" s="53"/>
       <c r="B38" s="1" t="s">
         <v>369</v>
       </c>
@@ -9045,7 +9106,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="50"/>
+      <c r="A39" s="53"/>
       <c r="B39" s="1" t="s">
         <v>370</v>
       </c>
@@ -9069,7 +9130,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="50"/>
+      <c r="A40" s="53"/>
       <c r="B40" s="1" t="s">
         <v>371</v>
       </c>
@@ -9093,7 +9154,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="50"/>
+      <c r="A41" s="53"/>
       <c r="B41" s="2" t="s">
         <v>383</v>
       </c>
@@ -9117,7 +9178,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="50"/>
+      <c r="A42" s="53"/>
       <c r="B42" s="2" t="s">
         <v>384</v>
       </c>
@@ -9141,7 +9202,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="50"/>
+      <c r="A43" s="53"/>
       <c r="B43" s="1" t="s">
         <v>80</v>
       </c>
@@ -9165,7 +9226,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="50"/>
+      <c r="A44" s="53"/>
       <c r="B44" s="1" t="s">
         <v>80</v>
       </c>
@@ -9189,7 +9250,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="50"/>
+      <c r="A45" s="53"/>
       <c r="B45" s="1" t="s">
         <v>80</v>
       </c>
@@ -9213,7 +9274,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="50"/>
+      <c r="A46" s="53"/>
       <c r="B46" s="1" t="s">
         <v>80</v>
       </c>
@@ -9237,7 +9298,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="50"/>
+      <c r="A47" s="53"/>
       <c r="B47" s="1" t="s">
         <v>396</v>
       </c>
@@ -9261,7 +9322,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="50"/>
+      <c r="A48" s="53"/>
       <c r="B48" s="2" t="s">
         <v>401</v>
       </c>
@@ -9285,7 +9346,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="50"/>
+      <c r="A49" s="53"/>
       <c r="B49" s="1" t="s">
         <v>402</v>
       </c>
@@ -9308,13 +9369,13 @@
         <v>404</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="47" t="s">
+    <row r="51" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="50" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="50" t="s">
+      <c r="A52" s="53" t="s">
         <v>54</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -9340,7 +9401,7 @@
       </c>
     </row>
     <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="50"/>
+      <c r="A53" s="53"/>
       <c r="B53" s="1" t="s">
         <v>236</v>
       </c>
@@ -9364,7 +9425,7 @@
       </c>
     </row>
     <row r="54" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="50"/>
+      <c r="A54" s="53"/>
       <c r="B54" s="1" t="s">
         <v>239</v>
       </c>
@@ -9388,7 +9449,7 @@
       </c>
     </row>
     <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A55" s="50"/>
+      <c r="A55" s="53"/>
       <c r="B55" s="1" t="s">
         <v>507</v>
       </c>
@@ -9412,7 +9473,7 @@
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="50"/>
+      <c r="A56" s="53"/>
       <c r="B56" s="1" t="s">
         <v>245</v>
       </c>
@@ -9436,7 +9497,7 @@
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="50"/>
+      <c r="A57" s="53"/>
       <c r="B57" s="2" t="s">
         <v>248</v>
       </c>
@@ -9460,7 +9521,7 @@
       </c>
     </row>
     <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="50"/>
+      <c r="A58" s="53"/>
       <c r="B58" s="2" t="s">
         <v>250</v>
       </c>
@@ -9484,7 +9545,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="50" t="s">
+      <c r="A59" s="53" t="s">
         <v>55</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -9510,7 +9571,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="50"/>
+      <c r="A60" s="53"/>
       <c r="B60" s="1" t="s">
         <v>255</v>
       </c>
@@ -9534,7 +9595,7 @@
       </c>
     </row>
     <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="50"/>
+      <c r="A61" s="53"/>
       <c r="B61" s="1" t="s">
         <v>258</v>
       </c>
@@ -9558,7 +9619,7 @@
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="50"/>
+      <c r="A62" s="53"/>
       <c r="B62" s="1" t="s">
         <v>261</v>
       </c>
@@ -9582,7 +9643,7 @@
       </c>
     </row>
     <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="50"/>
+      <c r="A63" s="53"/>
       <c r="B63" s="1" t="s">
         <v>264</v>
       </c>
@@ -9606,7 +9667,7 @@
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="50"/>
+      <c r="A64" s="53"/>
       <c r="B64" s="1" t="s">
         <v>267</v>
       </c>
@@ -9630,7 +9691,7 @@
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="50"/>
+      <c r="A65" s="53"/>
       <c r="B65" s="1" t="s">
         <v>270</v>
       </c>
@@ -9654,7 +9715,7 @@
       </c>
     </row>
     <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="50"/>
+      <c r="A66" s="53"/>
       <c r="B66" s="1" t="s">
         <v>273</v>
       </c>
@@ -9678,7 +9739,7 @@
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="50"/>
+      <c r="A67" s="53"/>
       <c r="B67" s="1" t="s">
         <v>276</v>
       </c>
@@ -9701,13 +9762,13 @@
         <v>278</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="47" t="s">
+    <row r="69" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="50" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="50" t="s">
+      <c r="A70" s="53" t="s">
         <v>57</v>
       </c>
       <c r="B70" s="2" t="s">
@@ -9733,7 +9794,7 @@
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="50"/>
+      <c r="A71" s="53"/>
       <c r="B71" s="2" t="s">
         <v>196</v>
       </c>
@@ -9757,7 +9818,7 @@
       </c>
     </row>
     <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A72" s="50"/>
+      <c r="A72" s="53"/>
       <c r="B72" s="2" t="s">
         <v>199</v>
       </c>
@@ -9781,7 +9842,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="50"/>
+      <c r="A73" s="53"/>
       <c r="B73" s="2" t="s">
         <v>202</v>
       </c>
@@ -9805,7 +9866,7 @@
       </c>
     </row>
     <row r="74" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="50"/>
+      <c r="A74" s="53"/>
       <c r="B74" s="2" t="s">
         <v>205</v>
       </c>
@@ -9829,7 +9890,7 @@
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="50" t="s">
+      <c r="A75" s="53" t="s">
         <v>58</v>
       </c>
       <c r="B75" s="2" t="s">
@@ -9855,7 +9916,7 @@
       </c>
     </row>
     <row r="76" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="50"/>
+      <c r="A76" s="53"/>
       <c r="B76" s="2" t="s">
         <v>211</v>
       </c>
@@ -9879,7 +9940,7 @@
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="50" t="s">
+      <c r="A77" s="53" t="s">
         <v>589</v>
       </c>
       <c r="B77" s="2" t="s">
@@ -9902,7 +9963,7 @@
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="50"/>
+      <c r="A78" s="53"/>
       <c r="B78" s="2" t="s">
         <v>216</v>
       </c>
@@ -9926,7 +9987,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="50"/>
+      <c r="A79" s="53"/>
       <c r="B79" s="2" t="s">
         <v>218</v>
       </c>
@@ -9950,7 +10011,7 @@
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="50"/>
+      <c r="A80" s="53"/>
       <c r="B80" s="2" t="s">
         <v>219</v>
       </c>
@@ -9974,7 +10035,7 @@
       </c>
     </row>
     <row r="81" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="50"/>
+      <c r="A81" s="53"/>
       <c r="B81" s="2" t="s">
         <v>223</v>
       </c>
@@ -9998,7 +10059,7 @@
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="50" t="s">
+      <c r="A82" s="53" t="s">
         <v>60</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -10024,7 +10085,7 @@
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="50"/>
+      <c r="A83" s="53"/>
       <c r="B83" s="1" t="s">
         <v>229</v>
       </c>
@@ -10047,13 +10108,13 @@
         <v>231</v>
       </c>
     </row>
-    <row r="85" spans="1:8" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="47" t="s">
+    <row r="85" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="50" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A86" s="50" t="s">
+      <c r="A86" s="53" t="s">
         <v>105</v>
       </c>
       <c r="B86" s="1" t="s">
@@ -10079,7 +10140,7 @@
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="50"/>
+      <c r="A87" s="53"/>
       <c r="B87" s="1" t="s">
         <v>72</v>
       </c>
@@ -10103,7 +10164,7 @@
       </c>
     </row>
     <row r="88" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A88" s="50"/>
+      <c r="A88" s="53"/>
       <c r="B88" s="1" t="s">
         <v>74</v>
       </c>
@@ -10127,7 +10188,7 @@
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="50"/>
+      <c r="A89" s="53"/>
       <c r="B89" s="2" t="s">
         <v>77</v>
       </c>
@@ -10151,7 +10212,7 @@
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="50"/>
+      <c r="A90" s="53"/>
       <c r="B90" s="1" t="s">
         <v>80</v>
       </c>
@@ -10175,7 +10236,7 @@
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="50"/>
+      <c r="A91" s="53"/>
       <c r="B91" s="1" t="s">
         <v>84</v>
       </c>
@@ -10199,7 +10260,7 @@
       </c>
     </row>
     <row r="92" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A92" s="50"/>
+      <c r="A92" s="53"/>
       <c r="B92" s="1" t="s">
         <v>87</v>
       </c>
@@ -10223,7 +10284,7 @@
       </c>
     </row>
     <row r="93" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A93" s="50"/>
+      <c r="A93" s="53"/>
       <c r="B93" s="1" t="s">
         <v>90</v>
       </c>
@@ -10247,7 +10308,7 @@
       </c>
     </row>
     <row r="94" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A94" s="50"/>
+      <c r="A94" s="53"/>
       <c r="B94" s="2" t="s">
         <v>93</v>
       </c>
@@ -10271,7 +10332,7 @@
       </c>
     </row>
     <row r="95" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A95" s="50"/>
+      <c r="A95" s="53"/>
       <c r="B95" s="1" t="s">
         <v>97</v>
       </c>
@@ -10295,7 +10356,7 @@
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="50" t="s">
+      <c r="A96" s="53" t="s">
         <v>106</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -10321,7 +10382,7 @@
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="50"/>
+      <c r="A97" s="53"/>
       <c r="B97" s="1" t="s">
         <v>102</v>
       </c>
@@ -10345,7 +10406,7 @@
       </c>
     </row>
     <row r="98" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="50" t="s">
+      <c r="A98" s="53" t="s">
         <v>61</v>
       </c>
       <c r="B98" s="1" t="s">
@@ -10371,7 +10432,7 @@
       </c>
     </row>
     <row r="99" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A99" s="50"/>
+      <c r="A99" s="53"/>
       <c r="B99" s="1" t="s">
         <v>110</v>
       </c>
@@ -10395,7 +10456,7 @@
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="50"/>
+      <c r="A100" s="53"/>
       <c r="B100" s="1" t="s">
         <v>112</v>
       </c>
@@ -10419,7 +10480,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="50"/>
+      <c r="A101" s="53"/>
       <c r="B101" s="1" t="s">
         <v>115</v>
       </c>
@@ -10443,7 +10504,7 @@
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="50"/>
+      <c r="A102" s="53"/>
       <c r="B102" s="1" t="s">
         <v>118</v>
       </c>
@@ -10467,7 +10528,7 @@
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="50"/>
+      <c r="A103" s="53"/>
       <c r="B103" s="1" t="s">
         <v>123</v>
       </c>
@@ -10491,7 +10552,7 @@
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="50"/>
+      <c r="A104" s="53"/>
       <c r="B104" s="1" t="s">
         <v>124</v>
       </c>
@@ -10515,7 +10576,7 @@
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="50"/>
+      <c r="A105" s="53"/>
       <c r="B105" s="1" t="s">
         <v>127</v>
       </c>
@@ -10539,7 +10600,7 @@
       </c>
     </row>
     <row r="106" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A106" s="50" t="s">
+      <c r="A106" s="53" t="s">
         <v>62</v>
       </c>
       <c r="B106" s="1" t="s">
@@ -10565,7 +10626,7 @@
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="50"/>
+      <c r="A107" s="53"/>
       <c r="B107" s="1" t="s">
         <v>133</v>
       </c>
@@ -10589,7 +10650,7 @@
       </c>
     </row>
     <row r="108" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="50" t="s">
+      <c r="A108" s="53" t="s">
         <v>63</v>
       </c>
       <c r="B108" s="1" t="s">
@@ -10615,7 +10676,7 @@
       </c>
     </row>
     <row r="109" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A109" s="50"/>
+      <c r="A109" s="53"/>
       <c r="B109" s="1" t="s">
         <v>139</v>
       </c>
@@ -10639,7 +10700,7 @@
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="50"/>
+      <c r="A110" s="53"/>
       <c r="B110" s="1" t="s">
         <v>142</v>
       </c>
@@ -10663,7 +10724,7 @@
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="50"/>
+      <c r="A111" s="53"/>
       <c r="B111" s="1" t="s">
         <v>146</v>
       </c>
@@ -10686,13 +10747,13 @@
         <v>148</v>
       </c>
     </row>
-    <row r="113" spans="1:8" s="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="47" t="s">
+    <row r="113" spans="1:8" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="50" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A114" s="50" t="s">
+      <c r="A114" s="53" t="s">
         <v>65</v>
       </c>
       <c r="B114" s="2" t="s">
@@ -10718,7 +10779,7 @@
       </c>
     </row>
     <row r="115" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A115" s="50"/>
+      <c r="A115" s="53"/>
       <c r="B115" s="2" t="s">
         <v>152</v>
       </c>
@@ -10742,7 +10803,7 @@
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A116" s="50"/>
+      <c r="A116" s="53"/>
       <c r="B116" s="2" t="s">
         <v>154</v>
       </c>
@@ -10766,7 +10827,7 @@
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A117" s="50"/>
+      <c r="A117" s="53"/>
       <c r="B117" s="2" t="s">
         <v>158</v>
       </c>
@@ -10790,7 +10851,7 @@
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A118" s="50"/>
+      <c r="A118" s="53"/>
       <c r="B118" s="2" t="s">
         <v>161</v>
       </c>
@@ -10814,7 +10875,7 @@
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A119" s="50"/>
+      <c r="A119" s="53"/>
       <c r="B119" s="2" t="s">
         <v>164</v>
       </c>
@@ -10838,7 +10899,7 @@
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" s="50"/>
+      <c r="A120" s="53"/>
       <c r="B120" s="2" t="s">
         <v>166</v>
       </c>
@@ -10862,7 +10923,7 @@
       </c>
     </row>
     <row r="121" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A121" s="50"/>
+      <c r="A121" s="53"/>
       <c r="B121" s="2" t="s">
         <v>169</v>
       </c>
@@ -10886,7 +10947,7 @@
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A122" s="50"/>
+      <c r="A122" s="53"/>
       <c r="B122" s="1" t="s">
         <v>172</v>
       </c>
@@ -10910,7 +10971,7 @@
       </c>
     </row>
     <row r="123" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A123" s="50"/>
+      <c r="A123" s="53"/>
       <c r="B123" s="2" t="s">
         <v>175</v>
       </c>
@@ -10934,7 +10995,7 @@
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A124" s="50"/>
+      <c r="A124" s="53"/>
       <c r="B124" s="1" t="s">
         <v>178</v>
       </c>
@@ -10958,7 +11019,7 @@
       </c>
     </row>
     <row r="125" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A125" s="50"/>
+      <c r="A125" s="53"/>
       <c r="B125" s="2" t="s">
         <v>181</v>
       </c>
@@ -10982,7 +11043,7 @@
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A126" s="50" t="s">
+      <c r="A126" s="53" t="s">
         <v>66</v>
       </c>
       <c r="B126" s="1" t="s">
@@ -10994,7 +11055,7 @@
       <c r="H126" s="1"/>
     </row>
     <row r="127" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A127" s="50"/>
+      <c r="A127" s="53"/>
       <c r="B127" s="2" t="s">
         <v>185</v>
       </c>
@@ -11018,7 +11079,7 @@
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A128" s="50"/>
+      <c r="A128" s="53"/>
       <c r="B128" s="1" t="s">
         <v>188</v>
       </c>
@@ -11030,7 +11091,7 @@
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A129" s="50"/>
+      <c r="A129" s="53"/>
       <c r="B129" s="1" t="s">
         <v>190</v>
       </c>
@@ -11124,8 +11185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C15B307-9B65-4164-8063-9F476182200F}">
   <dimension ref="B2:O180"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11149,17 +11210,17 @@
         <v>558</v>
       </c>
       <c r="D2" s="9"/>
-      <c r="E2" s="54" t="s">
+      <c r="E2" s="56" t="s">
         <v>557</v>
       </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
       <c r="I2" s="27" t="s">
         <v>578</v>
       </c>
       <c r="J2" s="1"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E3" s="18" t="s">
@@ -11810,11 +11871,770 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EECB9DD-973D-4158-878D-DA330B219DE9}">
+  <dimension ref="A2:S35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>652</v>
+      </c>
+      <c r="B2" t="s">
+        <v>643</v>
+      </c>
+      <c r="C2" t="s">
+        <v>640</v>
+      </c>
+      <c r="D2" t="s">
+        <v>641</v>
+      </c>
+      <c r="E2" t="s">
+        <v>642</v>
+      </c>
+      <c r="F2" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="49" t="s">
+        <v>648</v>
+      </c>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>645</v>
+      </c>
+      <c r="B4">
+        <v>2015</v>
+      </c>
+      <c r="C4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D4">
+        <v>8.7537000000000004E-2</v>
+      </c>
+      <c r="E4">
+        <v>1.6966999999999999E-2</v>
+      </c>
+      <c r="F4">
+        <v>0.193829</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>646</v>
+      </c>
+      <c r="B5">
+        <v>2017</v>
+      </c>
+      <c r="C5" s="48">
+        <v>1E-3</v>
+      </c>
+      <c r="D5" s="48">
+        <v>0.21876999999999999</v>
+      </c>
+      <c r="E5" s="48">
+        <v>7.7177999999999997E-2</v>
+      </c>
+      <c r="F5" s="48">
+        <v>0.35277900000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>646</v>
+      </c>
+      <c r="B6">
+        <v>2020</v>
+      </c>
+      <c r="C6" s="48">
+        <v>1E-3</v>
+      </c>
+      <c r="D6" s="48">
+        <v>0.31435800000000003</v>
+      </c>
+      <c r="E6" s="48">
+        <v>0.15884100000000001</v>
+      </c>
+      <c r="F6" s="48">
+        <v>0.50528799999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>646</v>
+      </c>
+      <c r="B7">
+        <v>2022</v>
+      </c>
+      <c r="C7" s="48">
+        <v>1E-3</v>
+      </c>
+      <c r="D7" s="48">
+        <v>0.32587100000000002</v>
+      </c>
+      <c r="E7" s="48">
+        <v>0.10209699999999999</v>
+      </c>
+      <c r="F7" s="48">
+        <v>0.31330400000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>646</v>
+      </c>
+      <c r="B8">
+        <v>2023</v>
+      </c>
+      <c r="C8" s="48">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D8" s="48">
+        <v>0.24501500000000001</v>
+      </c>
+      <c r="E8" s="48">
+        <v>5.1378E-2</v>
+      </c>
+      <c r="F8" s="48">
+        <v>0.20969099999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>647</v>
+      </c>
+      <c r="B9">
+        <v>2015</v>
+      </c>
+      <c r="C9" s="48">
+        <v>1E-3</v>
+      </c>
+      <c r="D9" s="48">
+        <v>2.3438000000000001E-2</v>
+      </c>
+      <c r="E9" s="48">
+        <v>7.3720000000000001E-3</v>
+      </c>
+      <c r="F9" s="48">
+        <v>0.31451600000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>647</v>
+      </c>
+      <c r="B10">
+        <v>2016</v>
+      </c>
+      <c r="C10" s="48">
+        <v>1E-3</v>
+      </c>
+      <c r="D10" s="48">
+        <v>2.5003000000000001E-2</v>
+      </c>
+      <c r="E10" s="48">
+        <v>8.2749999999999994E-3</v>
+      </c>
+      <c r="F10" s="48">
+        <v>0.33095599999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>647</v>
+      </c>
+      <c r="B11">
+        <v>2027</v>
+      </c>
+      <c r="C11" s="48">
+        <v>1E-3</v>
+      </c>
+      <c r="D11" s="48">
+        <v>2.6572999999999999E-2</v>
+      </c>
+      <c r="E11" s="48">
+        <v>8.2109999999999995E-3</v>
+      </c>
+      <c r="F11" s="48">
+        <v>0.30898999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>647</v>
+      </c>
+      <c r="B12">
+        <v>2018</v>
+      </c>
+      <c r="C12" s="48">
+        <v>1E-3</v>
+      </c>
+      <c r="D12" s="48">
+        <v>2.8007000000000001E-2</v>
+      </c>
+      <c r="E12" s="48">
+        <v>9.6419999999999995E-3</v>
+      </c>
+      <c r="F12" s="48">
+        <v>0.34428900000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>647</v>
+      </c>
+      <c r="B13">
+        <v>2019</v>
+      </c>
+      <c r="C13" s="48">
+        <v>1E-3</v>
+      </c>
+      <c r="D13" s="48">
+        <v>2.7677E-2</v>
+      </c>
+      <c r="E13" s="48">
+        <v>8.9759999999999996E-3</v>
+      </c>
+      <c r="F13" s="48">
+        <v>0.32432299999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>647</v>
+      </c>
+      <c r="B14">
+        <v>2020</v>
+      </c>
+      <c r="C14" s="48">
+        <v>2E-3</v>
+      </c>
+      <c r="D14" s="48">
+        <v>2.0927000000000001E-2</v>
+      </c>
+      <c r="E14" s="48">
+        <v>5.1599999999999997E-3</v>
+      </c>
+      <c r="F14" s="48">
+        <v>0.246561</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>647</v>
+      </c>
+      <c r="B15">
+        <v>2021</v>
+      </c>
+      <c r="C15" s="48">
+        <v>1E-3</v>
+      </c>
+      <c r="D15" s="48">
+        <v>1.9424E-2</v>
+      </c>
+      <c r="E15" s="48">
+        <v>5.0400000000000002E-3</v>
+      </c>
+      <c r="F15" s="48">
+        <v>0.25946900000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>647</v>
+      </c>
+      <c r="B16">
+        <v>2022</v>
+      </c>
+      <c r="C16" s="48">
+        <v>2E-3</v>
+      </c>
+      <c r="D16" s="48">
+        <v>2.3997999999999998E-2</v>
+      </c>
+      <c r="E16" s="48">
+        <v>8.1030000000000008E-3</v>
+      </c>
+      <c r="F16" s="48">
+        <v>0.33766699999999999</v>
+      </c>
+      <c r="M16" s="48"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>647</v>
+      </c>
+      <c r="B17">
+        <v>2023</v>
+      </c>
+      <c r="C17" s="48">
+        <v>1E-3</v>
+      </c>
+      <c r="D17" s="48">
+        <v>2.8815E-2</v>
+      </c>
+      <c r="E17" s="48">
+        <v>1.0241E-2</v>
+      </c>
+      <c r="F17" s="48">
+        <v>0.35540899999999997</v>
+      </c>
+      <c r="M17" s="48"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="49" t="s">
+        <v>649</v>
+      </c>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="M18" s="48"/>
+      <c r="S18" s="48"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>650</v>
+      </c>
+      <c r="B19">
+        <v>2017</v>
+      </c>
+      <c r="C19" s="48">
+        <v>3.9E-2</v>
+      </c>
+      <c r="D19" s="48">
+        <v>0.44165300000000002</v>
+      </c>
+      <c r="E19" s="48">
+        <v>5.8726E-2</v>
+      </c>
+      <c r="F19" s="48">
+        <v>0.132968</v>
+      </c>
+      <c r="M19" s="48"/>
+      <c r="N19" s="47"/>
+      <c r="S19" s="48"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>650</v>
+      </c>
+      <c r="B20">
+        <v>2022</v>
+      </c>
+      <c r="C20" s="48">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D20" s="48">
+        <v>0.40378199999999997</v>
+      </c>
+      <c r="E20" s="48">
+        <v>5.9514999999999998E-2</v>
+      </c>
+      <c r="F20" s="48">
+        <v>0.147393</v>
+      </c>
+      <c r="M20" s="48"/>
+      <c r="N20" s="47"/>
+      <c r="S20" s="48"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>651</v>
+      </c>
+      <c r="B21">
+        <v>2015</v>
+      </c>
+      <c r="C21" s="48">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D21" s="48">
+        <v>0.293902</v>
+      </c>
+      <c r="E21" s="48">
+        <v>5.9715999999999998E-2</v>
+      </c>
+      <c r="F21" s="48">
+        <v>0.203184</v>
+      </c>
+      <c r="G21" s="48"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="47"/>
+      <c r="S21" s="48"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>651</v>
+      </c>
+      <c r="B22">
+        <v>2016</v>
+      </c>
+      <c r="C22" s="48">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D22" s="48">
+        <v>0.31315399999999999</v>
+      </c>
+      <c r="E22" s="48">
+        <v>7.3182999999999998E-2</v>
+      </c>
+      <c r="F22" s="48">
+        <v>0.23369500000000001</v>
+      </c>
+      <c r="G22" s="48"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="48"/>
+      <c r="Q22" s="48"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>651</v>
+      </c>
+      <c r="B23">
+        <v>2017</v>
+      </c>
+      <c r="C23" s="48">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D23" s="48">
+        <v>0.29697499999999999</v>
+      </c>
+      <c r="E23" s="48">
+        <v>6.8500000000000005E-2</v>
+      </c>
+      <c r="F23" s="48">
+        <v>0.230659</v>
+      </c>
+      <c r="G23" s="48"/>
+      <c r="J23" s="47"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="48"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="48"/>
+      <c r="O23" s="48"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>651</v>
+      </c>
+      <c r="B24">
+        <v>2018</v>
+      </c>
+      <c r="C24" s="48">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D24" s="48">
+        <v>0.321718</v>
+      </c>
+      <c r="E24" s="48">
+        <v>6.3925999999999997E-2</v>
+      </c>
+      <c r="F24" s="48">
+        <v>0.19870099999999999</v>
+      </c>
+      <c r="G24" s="48"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="48"/>
+      <c r="L24" s="48"/>
+      <c r="M24" s="48"/>
+      <c r="N24" s="48"/>
+      <c r="O24" s="48"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>651</v>
+      </c>
+      <c r="B25">
+        <v>2019</v>
+      </c>
+      <c r="C25" s="48">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D25" s="48">
+        <v>0.34314099999999997</v>
+      </c>
+      <c r="E25" s="48">
+        <v>7.0125999999999994E-2</v>
+      </c>
+      <c r="F25" s="48">
+        <v>0.20436599999999999</v>
+      </c>
+      <c r="G25" s="48"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="48"/>
+      <c r="L25" s="48"/>
+      <c r="M25" s="48"/>
+      <c r="N25" s="48"/>
+      <c r="O25" s="48"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>651</v>
+      </c>
+      <c r="B26">
+        <v>2020</v>
+      </c>
+      <c r="C26" s="48">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D26" s="48">
+        <v>0.39255099999999998</v>
+      </c>
+      <c r="E26" s="48">
+        <v>8.0181000000000002E-2</v>
+      </c>
+      <c r="F26" s="48">
+        <v>0.20425499999999999</v>
+      </c>
+      <c r="G26" s="48"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="48"/>
+      <c r="L26" s="48"/>
+      <c r="M26" s="48"/>
+      <c r="N26" s="48"/>
+      <c r="O26" s="48"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>653</v>
+      </c>
+      <c r="B27">
+        <v>2015</v>
+      </c>
+      <c r="C27" s="48">
+        <v>2E-3</v>
+      </c>
+      <c r="D27" s="48">
+        <v>5.2044E-2</v>
+      </c>
+      <c r="E27" s="48">
+        <v>1.6258999999999999E-2</v>
+      </c>
+      <c r="F27" s="48">
+        <v>0.31240000000000001</v>
+      </c>
+      <c r="G27" s="48"/>
+      <c r="I27" s="47"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="48"/>
+      <c r="L27" s="48"/>
+      <c r="M27" s="48"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>653</v>
+      </c>
+      <c r="B28">
+        <v>2016</v>
+      </c>
+      <c r="C28" s="48">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D28" s="48">
+        <v>5.4601999999999998E-2</v>
+      </c>
+      <c r="E28" s="48">
+        <v>1.7017999999999998E-2</v>
+      </c>
+      <c r="F28" s="48">
+        <v>0.31167699999999998</v>
+      </c>
+      <c r="G28" s="48"/>
+      <c r="I28" s="47"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="48"/>
+      <c r="M28" s="48"/>
+      <c r="N28" s="47"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>653</v>
+      </c>
+      <c r="B29">
+        <v>2017</v>
+      </c>
+      <c r="C29" s="48">
+        <v>2E-3</v>
+      </c>
+      <c r="D29" s="48">
+        <v>5.8818000000000002E-2</v>
+      </c>
+      <c r="E29" s="48">
+        <v>1.9306E-2</v>
+      </c>
+      <c r="F29" s="48">
+        <v>0.32823400000000003</v>
+      </c>
+      <c r="G29" s="48"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="48"/>
+      <c r="K29" s="48"/>
+      <c r="L29" s="48"/>
+      <c r="M29" s="48"/>
+      <c r="N29" s="47"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>653</v>
+      </c>
+      <c r="B30">
+        <v>2018</v>
+      </c>
+      <c r="C30" s="48">
+        <v>2E-3</v>
+      </c>
+      <c r="D30" s="48">
+        <v>6.7854999999999999E-2</v>
+      </c>
+      <c r="E30" s="48">
+        <v>2.3519999999999999E-2</v>
+      </c>
+      <c r="F30" s="48">
+        <v>0.34662799999999999</v>
+      </c>
+      <c r="G30" s="48"/>
+      <c r="N30" s="47"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>653</v>
+      </c>
+      <c r="B31">
+        <v>2019</v>
+      </c>
+      <c r="C31" s="48">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D31" s="48">
+        <v>7.1820999999999996E-2</v>
+      </c>
+      <c r="E31" s="48">
+        <v>2.5166000000000001E-2</v>
+      </c>
+      <c r="F31" s="48">
+        <v>0.35039500000000001</v>
+      </c>
+      <c r="G31" s="48"/>
+      <c r="N31" s="47"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>653</v>
+      </c>
+      <c r="B32">
+        <v>2020</v>
+      </c>
+      <c r="C32" s="48">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D32" s="48">
+        <v>6.0958999999999999E-2</v>
+      </c>
+      <c r="E32" s="48">
+        <v>2.1222000000000001E-2</v>
+      </c>
+      <c r="F32" s="48">
+        <v>0.34813100000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>653</v>
+      </c>
+      <c r="B33">
+        <v>2021</v>
+      </c>
+      <c r="C33" s="48">
+        <v>1E-3</v>
+      </c>
+      <c r="D33" s="48">
+        <v>6.0049999999999999E-2</v>
+      </c>
+      <c r="E33" s="48">
+        <v>2.0402E-2</v>
+      </c>
+      <c r="F33" s="48">
+        <v>0.33975100000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>653</v>
+      </c>
+      <c r="B34">
+        <v>2022</v>
+      </c>
+      <c r="C34" s="48">
+        <v>2E-3</v>
+      </c>
+      <c r="D34" s="48">
+        <v>6.6243999999999997E-2</v>
+      </c>
+      <c r="E34" s="48">
+        <v>2.2710000000000001E-2</v>
+      </c>
+      <c r="F34" s="48">
+        <v>0.34281699999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>653</v>
+      </c>
+      <c r="B35">
+        <v>2023</v>
+      </c>
+      <c r="C35" s="48">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D35" s="48">
+        <v>6.9488999999999995E-2</v>
+      </c>
+      <c r="E35" s="48">
+        <v>2.6894000000000001E-2</v>
+      </c>
+      <c r="F35" s="48">
+        <v>0.387017</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A18:F18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C27BB3F-052F-484F-A5E2-9F1596D6E0CC}">
   <dimension ref="B2:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:C32"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -11844,7 +12664,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="57" t="s">
         <v>556</v>
       </c>
       <c r="C3" s="42" t="s">
@@ -11864,7 +12684,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="55"/>
+      <c r="B4" s="57"/>
       <c r="D4" s="44" t="s">
         <v>550</v>
       </c>
@@ -11879,7 +12699,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="55"/>
+      <c r="B5" s="57"/>
       <c r="C5" s="42" t="s">
         <v>346</v>
       </c>
@@ -11897,13 +12717,13 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="55"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="42" t="s">
         <v>512</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="55"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="42" t="s">
         <v>540</v>
       </c>
@@ -11921,7 +12741,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="55"/>
+      <c r="B8" s="57"/>
       <c r="D8" s="44" t="s">
         <v>202</v>
       </c>
@@ -11936,7 +12756,7 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="55"/>
+      <c r="B9" s="57"/>
       <c r="D9" s="44" t="s">
         <v>214</v>
       </c>
@@ -11951,7 +12771,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="55"/>
+      <c r="B10" s="57"/>
       <c r="D10" s="44" t="s">
         <v>223</v>
       </c>
@@ -11966,7 +12786,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="55"/>
+      <c r="B11" s="57"/>
       <c r="D11" s="44" t="s">
         <v>595</v>
       </c>
@@ -11981,7 +12801,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="55"/>
+      <c r="B12" s="57"/>
       <c r="D12" s="44" t="s">
         <v>596</v>
       </c>
@@ -11996,7 +12816,7 @@
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="55"/>
+      <c r="B13" s="57"/>
       <c r="D13" s="44" t="s">
         <v>562</v>
       </c>
@@ -12011,55 +12831,55 @@
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="55"/>
+      <c r="B14" s="57"/>
       <c r="C14" s="43" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="55"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="43" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="55"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="43" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="55"/>
+      <c r="B17" s="57"/>
       <c r="C17" s="43" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B18" s="55"/>
+      <c r="B18" s="57"/>
       <c r="C18" s="43" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="55"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="43" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="55"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="43" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="55"/>
+      <c r="B21" s="57"/>
       <c r="C21" s="43" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="55"/>
+      <c r="B22" s="57"/>
       <c r="C22" s="42" t="s">
         <v>530</v>
       </c>
@@ -12077,7 +12897,7 @@
       </c>
     </row>
     <row r="23" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="55"/>
+      <c r="B23" s="57"/>
       <c r="C23" s="42" t="s">
         <v>548</v>
       </c>
@@ -12095,7 +12915,7 @@
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="55"/>
+      <c r="B24" s="57"/>
       <c r="D24" s="44" t="s">
         <v>601</v>
       </c>
@@ -12110,7 +12930,7 @@
       </c>
     </row>
     <row r="25" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B25" s="55"/>
+      <c r="B25" s="57"/>
       <c r="C25" s="42" t="s">
         <v>533</v>
       </c>
@@ -12128,7 +12948,7 @@
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="55"/>
+      <c r="B26" s="57"/>
       <c r="C26" s="40"/>
       <c r="D26" s="41" t="s">
         <v>629</v>
@@ -12144,7 +12964,7 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B27" s="55"/>
+      <c r="B27" s="57"/>
       <c r="C27" s="43" t="s">
         <v>523</v>
       </c>
@@ -12152,25 +12972,25 @@
       <c r="G27" s="46"/>
     </row>
     <row r="28" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B28" s="55"/>
+      <c r="B28" s="57"/>
       <c r="C28" s="43" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="55"/>
+      <c r="B29" s="57"/>
       <c r="C29" s="43" t="s">
         <v>515</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B30" s="55"/>
+      <c r="B30" s="57"/>
       <c r="C30" s="43" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B31" s="55"/>
+      <c r="B31" s="57"/>
       <c r="C31" s="43" t="s">
         <v>513</v>
       </c>
@@ -12200,15 +13020,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_activity xmlns="9050bc6f-8f89-47a3-86fa-b072ef53d328" xsi:nil="true"/>
@@ -12216,7 +13027,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F6363AD6CE09334FA2B4FF9AA95D73C5" ma:contentTypeVersion="15" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="fea41b385c3c40a857800e800f56fbc8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9050bc6f-8f89-47a3-86fa-b072ef53d328" xmlns:ns4="bccbb3ce-f1a4-4a6f-aa39-0efc4956b4fd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="507616ff13059a37d7288ac12b1b548c" ns3:_="" ns4:_="">
     <xsd:import namespace="9050bc6f-8f89-47a3-86fa-b072ef53d328"/>
@@ -12449,15 +13260,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55792E88-4A72-42AB-9F80-0618B4EBFE2A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFC416A1-3111-4849-A533-05CA95BC2A5C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -12474,7 +13286,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13FC5822-06D7-4595-B74F-3FC67EA3A23C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12491,4 +13303,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55792E88-4A72-42AB-9F80-0618B4EBFE2A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>